<commit_message>
tune for sludge cake solids %
</commit_message>
<xml_diff>
--- a/exposan/werf/data/initial_conditions.xlsx
+++ b/exposan/werf/data/initial_conditions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joy_c\Dropbox\PhD\Research\QSD\codes_developing\EXPOsan\exposan\werf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581488A6-0405-4959-A9C2-8565AE0C3035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9BB877-B9C0-4FF5-99EA-DBE9B7D2D355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23133" yWindow="-93" windowWidth="23226" windowHeight="13866" activeTab="8" xr2:uid="{218DD762-44D5-4240-B5CB-C558EBE30BA7}"/>
+    <workbookView xWindow="-23133" yWindow="-93" windowWidth="23226" windowHeight="13866" activeTab="10" xr2:uid="{218DD762-44D5-4240-B5CB-C558EBE30BA7}"/>
   </bookViews>
   <sheets>
     <sheet name="B1" sheetId="6" r:id="rId1"/>
@@ -18,12 +18,13 @@
     <sheet name="B3" sheetId="4" r:id="rId3"/>
     <sheet name="C2" sheetId="8" r:id="rId4"/>
     <sheet name="C3" sheetId="9" r:id="rId5"/>
-    <sheet name="E2P" sheetId="11" r:id="rId6"/>
-    <sheet name="G1" sheetId="12" r:id="rId7"/>
-    <sheet name="G2" sheetId="13" r:id="rId8"/>
-    <sheet name="G3" sheetId="14" r:id="rId9"/>
-    <sheet name="AED" sheetId="10" r:id="rId10"/>
-    <sheet name="adm" sheetId="2" r:id="rId11"/>
+    <sheet name="E2" sheetId="15" r:id="rId6"/>
+    <sheet name="E2P" sheetId="11" r:id="rId7"/>
+    <sheet name="G1" sheetId="12" r:id="rId8"/>
+    <sheet name="G2" sheetId="13" r:id="rId9"/>
+    <sheet name="G3" sheetId="14" r:id="rId10"/>
+    <sheet name="AED" sheetId="10" r:id="rId11"/>
+    <sheet name="adm" sheetId="2" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="67">
   <si>
     <t>S_O2</t>
   </si>
@@ -1302,598 +1303,704 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CB7F0C9-B54B-4F93-93CE-9E10B0EA4FF3}">
-  <dimension ref="A1:AF6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1A144BC-89D4-47F0-9D49-ED1B9234D74F}">
+  <dimension ref="A1:AE7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="29" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
       </c>
       <c r="J1" t="s">
         <v>7</v>
       </c>
       <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>19</v>
       </c>
-      <c r="R1" t="s">
-        <v>14</v>
-      </c>
-      <c r="S1" t="s">
-        <v>15</v>
-      </c>
       <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V1" t="s">
+        <v>43</v>
+      </c>
+      <c r="W1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD1" t="s">
         <v>16</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AE1" t="s">
         <v>17</v>
       </c>
-      <c r="V1" t="s">
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2">
+        <v>0.03</v>
+      </c>
+      <c r="C2">
+        <v>25</v>
+      </c>
+      <c r="D2">
+        <v>0.01</v>
+      </c>
+      <c r="E2">
+        <v>1.5</v>
+      </c>
+      <c r="F2">
+        <v>0.5</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>80</v>
+      </c>
+      <c r="I2">
         <v>18</v>
       </c>
-      <c r="W1" t="s">
-        <v>47</v>
-      </c>
-      <c r="X1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>0.4</v>
-      </c>
-      <c r="D2">
-        <v>0.1</v>
-      </c>
-      <c r="E2">
-        <v>30</v>
-      </c>
-      <c r="F2">
-        <v>0.2</v>
-      </c>
-      <c r="G2">
-        <v>20</v>
-      </c>
-      <c r="H2">
-        <v>100</v>
-      </c>
-      <c r="I2">
-        <v>400</v>
-      </c>
       <c r="J2">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="K2">
-        <v>7000</v>
+        <v>28</v>
       </c>
       <c r="L2">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M2">
+        <v>3600</v>
+      </c>
+      <c r="N2">
+        <v>70</v>
+      </c>
+      <c r="O2">
+        <v>4500</v>
+      </c>
+      <c r="P2">
+        <v>60</v>
+      </c>
+      <c r="Q2">
+        <v>1.5</v>
+      </c>
+      <c r="R2">
+        <v>1.5</v>
+      </c>
+      <c r="S2">
+        <v>250</v>
+      </c>
+      <c r="T2">
+        <v>110</v>
+      </c>
+      <c r="U2">
         <v>4000</v>
-      </c>
-      <c r="N2">
-        <v>100</v>
-      </c>
-      <c r="O2">
-        <v>10</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2">
-        <v>200</v>
-      </c>
-      <c r="R2">
-        <v>28</v>
-      </c>
-      <c r="S2">
-        <v>10</v>
-      </c>
-      <c r="T2">
-        <v>86</v>
-      </c>
-      <c r="U2">
-        <v>425</v>
       </c>
       <c r="V2">
         <v>10</v>
       </c>
       <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>1000</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AD2">
+        <v>87</v>
+      </c>
+      <c r="AE2">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>25</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3">
         <v>0.01</v>
       </c>
-      <c r="X2">
-        <v>10</v>
-      </c>
-      <c r="Y2">
-        <v>250</v>
-      </c>
-      <c r="Z2">
-        <v>5000</v>
-      </c>
-      <c r="AA2">
-        <v>0.01</v>
-      </c>
-      <c r="AB2">
-        <v>0.01</v>
-      </c>
-      <c r="AC2">
-        <v>0.01</v>
-      </c>
-      <c r="AD2">
-        <v>0.01</v>
-      </c>
-      <c r="AE2">
-        <v>0.01</v>
-      </c>
-      <c r="AF2">
-        <v>997000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3">
+      <c r="F3">
+        <v>0.5</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>90</v>
+      </c>
+      <c r="I3">
+        <v>18</v>
+      </c>
+      <c r="J3">
+        <v>60</v>
+      </c>
+      <c r="K3">
+        <v>28</v>
+      </c>
+      <c r="L3">
+        <v>50</v>
+      </c>
+      <c r="M3">
+        <v>1200</v>
+      </c>
+      <c r="N3">
+        <v>60</v>
+      </c>
+      <c r="O3">
+        <v>1500</v>
+      </c>
+      <c r="P3">
+        <v>20</v>
+      </c>
+      <c r="Q3">
+        <v>0.5</v>
+      </c>
+      <c r="R3">
         <v>1</v>
       </c>
-      <c r="C3">
-        <v>0.4</v>
-      </c>
-      <c r="D3">
-        <v>0.1</v>
-      </c>
-      <c r="E3">
-        <v>30</v>
-      </c>
-      <c r="F3">
-        <v>0.2</v>
-      </c>
-      <c r="G3">
-        <v>20</v>
-      </c>
-      <c r="H3">
-        <v>1200</v>
-      </c>
-      <c r="I3">
-        <v>500</v>
-      </c>
-      <c r="J3">
-        <v>84</v>
-      </c>
-      <c r="K3">
-        <v>8000</v>
-      </c>
-      <c r="L3">
-        <v>100</v>
-      </c>
-      <c r="M3">
-        <v>4000</v>
-      </c>
-      <c r="N3">
-        <v>100</v>
-      </c>
-      <c r="O3">
-        <v>10</v>
-      </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3">
-        <v>200</v>
-      </c>
-      <c r="R3">
-        <v>28</v>
-      </c>
       <c r="S3">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="T3">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="U3">
-        <v>425</v>
+        <v>1000</v>
       </c>
       <c r="V3">
         <v>10</v>
       </c>
       <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3">
+        <v>500</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AD3">
+        <v>87</v>
+      </c>
+      <c r="AE3">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4">
         <v>0.01</v>
       </c>
-      <c r="X3">
-        <v>10</v>
-      </c>
-      <c r="Y3">
-        <v>250</v>
-      </c>
-      <c r="Z3">
-        <v>8000</v>
-      </c>
-      <c r="AA3">
-        <v>0.01</v>
-      </c>
-      <c r="AB3">
-        <v>0.01</v>
-      </c>
-      <c r="AC3">
-        <v>0.01</v>
-      </c>
-      <c r="AD3">
-        <v>0.01</v>
-      </c>
-      <c r="AE3">
-        <v>0.01</v>
-      </c>
-      <c r="AF3">
-        <v>997000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
       <c r="C4">
-        <v>0.4</v>
+        <v>25</v>
       </c>
       <c r="D4">
-        <v>0.1</v>
+        <v>5</v>
       </c>
       <c r="E4">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="F4">
         <v>0.2</v>
       </c>
       <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4">
+        <v>18</v>
+      </c>
+      <c r="J4">
+        <v>50</v>
+      </c>
+      <c r="K4">
+        <v>28</v>
+      </c>
+      <c r="L4">
+        <v>50</v>
+      </c>
+      <c r="M4">
+        <v>1000</v>
+      </c>
+      <c r="N4">
+        <v>30</v>
+      </c>
+      <c r="O4">
+        <v>1300</v>
+      </c>
+      <c r="P4">
         <v>20</v>
       </c>
-      <c r="H4">
+      <c r="Q4">
+        <v>0.5</v>
+      </c>
+      <c r="R4">
+        <v>0.5</v>
+      </c>
+      <c r="S4">
+        <v>80</v>
+      </c>
+      <c r="T4">
+        <v>110</v>
+      </c>
+      <c r="U4">
         <v>1000</v>
-      </c>
-      <c r="I4">
-        <v>500</v>
-      </c>
-      <c r="J4">
-        <v>84</v>
-      </c>
-      <c r="K4">
-        <v>8000</v>
-      </c>
-      <c r="L4">
-        <v>100</v>
-      </c>
-      <c r="M4">
-        <v>2800</v>
-      </c>
-      <c r="N4">
-        <v>100</v>
-      </c>
-      <c r="O4">
-        <v>10</v>
-      </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="Q4">
-        <v>200</v>
-      </c>
-      <c r="R4">
-        <v>28</v>
-      </c>
-      <c r="S4">
-        <v>10</v>
-      </c>
-      <c r="T4">
-        <v>86</v>
-      </c>
-      <c r="U4">
-        <v>425</v>
       </c>
       <c r="V4">
         <v>10</v>
       </c>
       <c r="W4">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="X4">
-        <v>10</v>
-      </c>
-      <c r="Y4">
-        <v>250</v>
-      </c>
-      <c r="Z4">
-        <v>8300</v>
-      </c>
-      <c r="AA4">
-        <v>0.01</v>
-      </c>
-      <c r="AB4">
-        <v>0.01</v>
-      </c>
-      <c r="AC4">
-        <v>0.01</v>
+        <v>500</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>1E-8</v>
       </c>
       <c r="AD4">
-        <v>0.01</v>
+        <v>87</v>
       </c>
       <c r="AE4">
-        <v>0.01</v>
-      </c>
-      <c r="AF4">
-        <v>997000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0.4</v>
+        <v>25</v>
       </c>
       <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
         <v>0.1</v>
-      </c>
-      <c r="E5">
-        <v>20</v>
       </c>
       <c r="F5">
         <v>0.2</v>
       </c>
       <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>18</v>
+      </c>
+      <c r="J5">
+        <v>50</v>
+      </c>
+      <c r="K5">
+        <v>28</v>
+      </c>
+      <c r="L5">
+        <v>50</v>
+      </c>
+      <c r="M5">
+        <v>1000</v>
+      </c>
+      <c r="N5">
+        <v>25</v>
+      </c>
+      <c r="O5">
+        <v>1300</v>
+      </c>
+      <c r="P5">
         <v>20</v>
       </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-      <c r="I5">
-        <v>100</v>
-      </c>
-      <c r="J5">
-        <v>84</v>
-      </c>
-      <c r="K5" s="1">
-        <v>17000</v>
-      </c>
-      <c r="L5">
-        <v>300</v>
-      </c>
-      <c r="M5" s="1">
-        <v>12000</v>
-      </c>
-      <c r="N5">
-        <v>100</v>
-      </c>
-      <c r="O5">
-        <v>10</v>
-      </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
       <c r="Q5">
-        <v>400</v>
+        <v>0.5</v>
       </c>
       <c r="R5">
-        <v>28</v>
+        <v>0.5</v>
       </c>
       <c r="S5">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="T5">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="U5">
-        <v>425</v>
+        <v>1000</v>
       </c>
       <c r="V5">
         <v>10</v>
       </c>
       <c r="W5">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="X5">
-        <v>10</v>
-      </c>
-      <c r="Y5">
-        <v>250</v>
-      </c>
-      <c r="Z5">
-        <v>6000</v>
-      </c>
-      <c r="AA5">
-        <v>0.01</v>
-      </c>
-      <c r="AB5">
-        <v>0.01</v>
-      </c>
-      <c r="AC5">
-        <v>0.01</v>
+        <v>500</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>1E-8</v>
       </c>
       <c r="AD5">
-        <v>0.01</v>
+        <v>87</v>
       </c>
       <c r="AE5">
-        <v>0.01</v>
-      </c>
-      <c r="AF5">
-        <v>997000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>0.4</v>
+        <v>25</v>
       </c>
       <c r="D6">
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="E6">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="F6">
         <v>0.2</v>
       </c>
       <c r="G6">
+        <v>0.5</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>18</v>
+      </c>
+      <c r="J6">
+        <v>50</v>
+      </c>
+      <c r="K6">
+        <v>28</v>
+      </c>
+      <c r="L6">
+        <v>50</v>
+      </c>
+      <c r="M6">
+        <v>1000</v>
+      </c>
+      <c r="N6">
+        <v>25</v>
+      </c>
+      <c r="O6">
+        <v>1300</v>
+      </c>
+      <c r="P6">
         <v>20</v>
       </c>
-      <c r="H6">
-        <v>50</v>
-      </c>
-      <c r="I6">
-        <v>200</v>
-      </c>
-      <c r="J6">
-        <v>84</v>
-      </c>
-      <c r="K6">
-        <v>7000</v>
-      </c>
-      <c r="L6">
-        <v>100</v>
-      </c>
-      <c r="M6">
-        <v>4000</v>
-      </c>
-      <c r="N6">
-        <v>100</v>
-      </c>
-      <c r="O6">
-        <v>10</v>
-      </c>
-      <c r="P6">
-        <v>1</v>
-      </c>
       <c r="Q6">
-        <v>200</v>
+        <v>0.5</v>
       </c>
       <c r="R6">
-        <v>28</v>
+        <v>0.5</v>
       </c>
       <c r="S6">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="T6">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="U6">
-        <v>425</v>
+        <v>1000</v>
       </c>
       <c r="V6">
         <v>10</v>
       </c>
       <c r="W6">
-        <v>8000</v>
+        <v>1</v>
       </c>
       <c r="X6">
+        <v>500</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AD6">
+        <v>87</v>
+      </c>
+      <c r="AE6">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>25</v>
+      </c>
+      <c r="D7">
+        <v>0.5</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>0.2</v>
+      </c>
+      <c r="G7">
+        <v>0.5</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>18</v>
+      </c>
+      <c r="J7">
+        <v>45</v>
+      </c>
+      <c r="K7">
+        <v>28</v>
+      </c>
+      <c r="L7">
+        <v>50</v>
+      </c>
+      <c r="M7">
+        <v>1000</v>
+      </c>
+      <c r="N7">
+        <v>25</v>
+      </c>
+      <c r="O7">
+        <v>1300</v>
+      </c>
+      <c r="P7">
+        <v>20</v>
+      </c>
+      <c r="Q7">
+        <v>0.5</v>
+      </c>
+      <c r="R7">
+        <v>0.5</v>
+      </c>
+      <c r="S7">
+        <v>80</v>
+      </c>
+      <c r="T7">
+        <v>110</v>
+      </c>
+      <c r="U7">
+        <v>1000</v>
+      </c>
+      <c r="V7">
         <v>10</v>
       </c>
-      <c r="Y6">
-        <v>250</v>
-      </c>
-      <c r="Z6">
-        <v>5000</v>
-      </c>
-      <c r="AA6">
-        <v>0.01</v>
-      </c>
-      <c r="AB6">
-        <v>0.01</v>
-      </c>
-      <c r="AC6">
-        <v>0.01</v>
-      </c>
-      <c r="AD6">
-        <v>0.01</v>
-      </c>
-      <c r="AE6">
-        <v>0.01</v>
-      </c>
-      <c r="AF6">
-        <v>997000</v>
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7">
+        <v>500</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AD7">
+        <v>87</v>
+      </c>
+      <c r="AE7">
+        <v>425</v>
       </c>
     </row>
   </sheetData>
@@ -1902,6 +2009,609 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CB7F0C9-B54B-4F93-93CE-9E10B0EA4FF3}">
+  <dimension ref="A1:AF6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>30</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="G2" s="2">
+        <v>20</v>
+      </c>
+      <c r="H2" s="2">
+        <v>100</v>
+      </c>
+      <c r="I2" s="2">
+        <v>400</v>
+      </c>
+      <c r="J2" s="2">
+        <v>84</v>
+      </c>
+      <c r="K2" s="2">
+        <v>7000</v>
+      </c>
+      <c r="L2" s="2">
+        <v>100</v>
+      </c>
+      <c r="M2" s="2">
+        <v>4000</v>
+      </c>
+      <c r="N2" s="2">
+        <v>100</v>
+      </c>
+      <c r="O2" s="2">
+        <v>10</v>
+      </c>
+      <c r="P2" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>200</v>
+      </c>
+      <c r="R2" s="2">
+        <v>28</v>
+      </c>
+      <c r="S2" s="2">
+        <v>10</v>
+      </c>
+      <c r="T2" s="2">
+        <v>86</v>
+      </c>
+      <c r="U2" s="2">
+        <v>425</v>
+      </c>
+      <c r="V2" s="2">
+        <v>10</v>
+      </c>
+      <c r="W2" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="X2" s="2">
+        <v>10</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>250</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>5000</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="AE2" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="AF2" s="2">
+        <v>997000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>30</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="G3" s="2">
+        <v>20</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1200</v>
+      </c>
+      <c r="I3" s="2">
+        <v>500</v>
+      </c>
+      <c r="J3" s="2">
+        <v>84</v>
+      </c>
+      <c r="K3" s="2">
+        <v>8000</v>
+      </c>
+      <c r="L3" s="2">
+        <v>100</v>
+      </c>
+      <c r="M3" s="2">
+        <v>4000</v>
+      </c>
+      <c r="N3" s="2">
+        <v>100</v>
+      </c>
+      <c r="O3" s="2">
+        <v>10</v>
+      </c>
+      <c r="P3" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>200</v>
+      </c>
+      <c r="R3" s="2">
+        <v>28</v>
+      </c>
+      <c r="S3" s="2">
+        <v>10</v>
+      </c>
+      <c r="T3" s="2">
+        <v>86</v>
+      </c>
+      <c r="U3" s="2">
+        <v>425</v>
+      </c>
+      <c r="V3" s="2">
+        <v>10</v>
+      </c>
+      <c r="W3" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="X3" s="2">
+        <v>10</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>250</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>8000</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="AB3" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="AC3" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="AD3" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="AE3" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="AF3" s="2">
+        <v>997000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>30</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="G4" s="2">
+        <v>20</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1000</v>
+      </c>
+      <c r="I4" s="2">
+        <v>500</v>
+      </c>
+      <c r="J4" s="2">
+        <v>84</v>
+      </c>
+      <c r="K4" s="2">
+        <v>8000</v>
+      </c>
+      <c r="L4" s="2">
+        <v>100</v>
+      </c>
+      <c r="M4" s="2">
+        <v>2800</v>
+      </c>
+      <c r="N4" s="2">
+        <v>100</v>
+      </c>
+      <c r="O4" s="2">
+        <v>10</v>
+      </c>
+      <c r="P4" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>200</v>
+      </c>
+      <c r="R4" s="2">
+        <v>28</v>
+      </c>
+      <c r="S4" s="2">
+        <v>10</v>
+      </c>
+      <c r="T4" s="2">
+        <v>86</v>
+      </c>
+      <c r="U4" s="2">
+        <v>425</v>
+      </c>
+      <c r="V4" s="2">
+        <v>10</v>
+      </c>
+      <c r="W4" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="X4" s="2">
+        <v>10</v>
+      </c>
+      <c r="Y4" s="2">
+        <v>250</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>8300</v>
+      </c>
+      <c r="AA4" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="AB4" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="AC4" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="AD4" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="AE4" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="AF4" s="2">
+        <v>997000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>20</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="G5" s="2">
+        <v>20</v>
+      </c>
+      <c r="H5" s="2">
+        <v>20</v>
+      </c>
+      <c r="I5" s="2">
+        <v>100</v>
+      </c>
+      <c r="J5" s="2">
+        <v>84</v>
+      </c>
+      <c r="K5" s="2">
+        <v>15000</v>
+      </c>
+      <c r="L5" s="2">
+        <v>300</v>
+      </c>
+      <c r="M5" s="2">
+        <v>10000</v>
+      </c>
+      <c r="N5" s="2">
+        <v>100</v>
+      </c>
+      <c r="O5" s="2">
+        <v>10</v>
+      </c>
+      <c r="P5" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>400</v>
+      </c>
+      <c r="R5" s="2">
+        <v>28</v>
+      </c>
+      <c r="S5" s="2">
+        <v>40</v>
+      </c>
+      <c r="T5" s="2">
+        <v>86</v>
+      </c>
+      <c r="U5" s="2">
+        <v>425</v>
+      </c>
+      <c r="V5" s="2">
+        <v>10</v>
+      </c>
+      <c r="W5" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="X5" s="2">
+        <v>10</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>250</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>5000</v>
+      </c>
+      <c r="AA5" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="AB5" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="AC5" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="AD5" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="AE5" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="AF5" s="2">
+        <v>997000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>20</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="G6" s="2">
+        <v>20</v>
+      </c>
+      <c r="H6" s="2">
+        <v>50</v>
+      </c>
+      <c r="I6" s="2">
+        <v>200</v>
+      </c>
+      <c r="J6" s="2">
+        <v>84</v>
+      </c>
+      <c r="K6" s="2">
+        <v>7000</v>
+      </c>
+      <c r="L6" s="2">
+        <v>100</v>
+      </c>
+      <c r="M6" s="2">
+        <v>4000</v>
+      </c>
+      <c r="N6" s="2">
+        <v>100</v>
+      </c>
+      <c r="O6" s="2">
+        <v>10</v>
+      </c>
+      <c r="P6" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>200</v>
+      </c>
+      <c r="R6" s="2">
+        <v>28</v>
+      </c>
+      <c r="S6" s="2">
+        <v>10</v>
+      </c>
+      <c r="T6" s="2">
+        <v>86</v>
+      </c>
+      <c r="U6" s="2">
+        <v>425</v>
+      </c>
+      <c r="V6" s="2">
+        <v>10</v>
+      </c>
+      <c r="W6" s="2">
+        <v>8000</v>
+      </c>
+      <c r="X6" s="2">
+        <v>10</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>250</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>5000</v>
+      </c>
+      <c r="AA6" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="AB6" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="AC6" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="AD6" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="AE6" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="AF6" s="2">
+        <v>997000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{472A4E84-05F6-482F-94AF-2C8CE149BF8E}">
   <dimension ref="A1:AP57"/>
   <sheetViews>
@@ -5621,11 +6331,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5589379-171B-4A97-AC18-14A5DD584161}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E307A296-2558-4740-844A-6971D987A213}">
   <dimension ref="A1:AE7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5730,91 +6440,91 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>15.598949295750201</v>
+        <v>15</v>
       </c>
       <c r="D2">
-        <v>8.6204579891603608</v>
+        <v>10</v>
       </c>
       <c r="E2">
-        <v>14.5046160761559</v>
+        <v>20</v>
       </c>
       <c r="F2">
-        <v>0.33616849768273399</v>
+        <v>0.5</v>
       </c>
       <c r="G2">
-        <v>1.63274914714391</v>
+        <v>2</v>
       </c>
       <c r="H2">
-        <v>0.41361452807892901</v>
+        <v>0.5</v>
       </c>
       <c r="I2">
-        <v>17.9000017485738</v>
+        <v>18</v>
       </c>
       <c r="J2">
-        <v>26.8107831665654</v>
+        <v>30</v>
       </c>
       <c r="K2">
-        <v>28.000003808201399</v>
+        <v>28</v>
       </c>
       <c r="L2">
-        <v>49.999724147812103</v>
+        <v>50</v>
       </c>
       <c r="M2">
-        <v>1015.03372708692</v>
+        <v>1200</v>
       </c>
       <c r="N2">
-        <v>55.0422620178351</v>
+        <v>100</v>
       </c>
       <c r="O2">
-        <v>1164.4940121392201</v>
+        <v>1100</v>
       </c>
       <c r="P2" s="1">
-        <v>2.1859735620121E-10</v>
+        <v>1E-8</v>
       </c>
       <c r="Q2" s="1">
-        <v>5.8898187677390694E-11</v>
+        <v>1E-8</v>
       </c>
       <c r="R2" s="1">
-        <v>3.2989269261525801E-13</v>
+        <v>1E-8</v>
       </c>
       <c r="S2">
-        <v>83.161561984309103</v>
+        <v>50</v>
       </c>
       <c r="T2">
-        <v>130.81507073853999</v>
+        <v>130</v>
       </c>
       <c r="U2" s="1">
-        <v>3.1331586475129499E-8</v>
-      </c>
-      <c r="V2" s="1">
-        <v>3.18489546411206E-5</v>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="V2">
+        <v>0.01</v>
       </c>
       <c r="W2">
-        <v>3.9356200874160804E-3</v>
+        <v>2</v>
       </c>
       <c r="X2">
-        <v>576.69896357149003</v>
+        <v>350</v>
       </c>
       <c r="Y2" s="1">
-        <v>3.1330718046475798E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="Z2" s="1">
-        <v>3.1330716862048399E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="AA2" s="1">
-        <v>3.13307198982397E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="AB2" s="1">
-        <v>3.13307167343325E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="AC2" s="1">
-        <v>3.13307198982397E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="AD2">
-        <v>86.999999167358396</v>
+        <v>87</v>
       </c>
       <c r="AE2">
-        <v>425.00000000003598</v>
+        <v>425</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
@@ -5825,91 +6535,91 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>14.964112358119699</v>
+        <v>15</v>
       </c>
       <c r="D3">
-        <v>3.5682524968894298</v>
+        <v>4</v>
       </c>
       <c r="E3">
-        <v>19.2923960227773</v>
+        <v>20</v>
       </c>
       <c r="F3">
-        <v>0.26499060956376302</v>
+        <v>0.5</v>
       </c>
       <c r="G3">
-        <v>0.45993815050630998</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>5.6431848977041503E-2</v>
+        <v>0.1</v>
       </c>
       <c r="I3">
-        <v>17.9000017520539</v>
+        <v>18</v>
       </c>
       <c r="J3">
-        <v>13.643586052327899</v>
+        <v>8</v>
       </c>
       <c r="K3">
-        <v>28.000003815780602</v>
+        <v>28</v>
       </c>
       <c r="L3">
-        <v>49.999723820472397</v>
+        <v>50</v>
       </c>
       <c r="M3">
-        <v>1016.11699896993</v>
+        <v>1200</v>
       </c>
       <c r="N3">
-        <v>43.1743681524717</v>
+        <v>60</v>
       </c>
       <c r="O3">
-        <v>1168.3871256212001</v>
+        <v>1100</v>
       </c>
       <c r="P3" s="1">
-        <v>2.18981438448107E-10</v>
+        <v>1E-8</v>
       </c>
       <c r="Q3" s="1">
-        <v>5.9022484932081505E-11</v>
+        <v>1E-8</v>
       </c>
       <c r="R3" s="1">
-        <v>1.1760898211310701E-13</v>
+        <v>1E-8</v>
       </c>
       <c r="S3">
-        <v>84.104633103904703</v>
+        <v>50</v>
       </c>
       <c r="T3">
-        <v>130.75126724610001</v>
+        <v>130</v>
       </c>
       <c r="U3" s="1">
-        <v>3.1387544966605997E-8</v>
-      </c>
-      <c r="V3" s="1">
-        <v>3.19058377884337E-5</v>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="V3">
+        <v>0.01</v>
       </c>
       <c r="W3">
-        <v>3.9405575382428096E-3</v>
+        <v>2</v>
       </c>
       <c r="X3">
-        <v>576.86350385646801</v>
+        <v>350</v>
       </c>
       <c r="Y3" s="1">
-        <v>3.1386674985870803E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="Z3" s="1">
-        <v>3.1386673799340797E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="AA3" s="1">
-        <v>3.1386676840921801E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="AB3" s="1">
-        <v>3.1386673671398197E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="AC3" s="1">
-        <v>3.1386676840921801E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="AD3">
-        <v>86.999999165701198</v>
+        <v>87</v>
       </c>
       <c r="AE3">
-        <v>425.00000000003899</v>
+        <v>425</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
@@ -5920,91 +6630,91 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>14.6442966277118</v>
+        <v>15</v>
       </c>
       <c r="D4">
-        <v>0.80390861676764103</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>21.987083651526302</v>
+        <v>20</v>
       </c>
       <c r="F4">
-        <v>0.26222282910640399</v>
+        <v>0.5</v>
       </c>
       <c r="G4">
-        <v>0.35587464308705202</v>
+        <v>0.5</v>
       </c>
       <c r="H4">
-        <v>1.8168951933000801E-2</v>
+        <v>0.1</v>
       </c>
       <c r="I4">
-        <v>17.900001755540799</v>
+        <v>18</v>
       </c>
       <c r="J4">
-        <v>7.3579196525691</v>
+        <v>5</v>
       </c>
       <c r="K4">
-        <v>28.000003823374801</v>
+        <v>28</v>
       </c>
       <c r="L4">
-        <v>49.999723492754498</v>
+        <v>50</v>
       </c>
       <c r="M4">
-        <v>1017.20142376323</v>
+        <v>1200</v>
       </c>
       <c r="N4">
-        <v>34.617532477773999</v>
+        <v>40</v>
       </c>
       <c r="O4">
-        <v>1169.3398710757001</v>
+        <v>1100</v>
       </c>
       <c r="P4" s="1">
-        <v>2.1920632479658099E-10</v>
+        <v>1E-8</v>
       </c>
       <c r="Q4" s="1">
-        <v>5.9094159622198901E-11</v>
+        <v>1E-8</v>
       </c>
       <c r="R4" s="1">
-        <v>4.08029203179745E-14</v>
+        <v>1E-8</v>
       </c>
       <c r="S4">
-        <v>84.533415281793197</v>
+        <v>50</v>
       </c>
       <c r="T4">
-        <v>130.72334595062901</v>
+        <v>130</v>
       </c>
       <c r="U4" s="1">
-        <v>3.1443603391254401E-8</v>
-      </c>
-      <c r="V4" s="1">
-        <v>3.1962822522962802E-5</v>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="V4">
+        <v>0.01</v>
       </c>
       <c r="W4">
-        <v>3.9455012522009204E-3</v>
+        <v>2</v>
       </c>
       <c r="X4">
-        <v>576.93547607702101</v>
+        <v>350</v>
       </c>
       <c r="Y4" s="1">
-        <v>3.1442731855661099E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="Z4" s="1">
-        <v>3.14427306670248E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="AA4" s="1">
-        <v>3.1442733714005103E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="AB4" s="1">
-        <v>3.1442730538855103E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="AC4" s="1">
-        <v>3.1442733714005103E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="AD4">
-        <v>86.999999164040801</v>
+        <v>87</v>
       </c>
       <c r="AE4">
-        <v>425.00000000004297</v>
+        <v>425</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
@@ -6015,91 +6725,91 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>14.481506405706</v>
+        <v>15</v>
       </c>
       <c r="D5">
-        <v>0.15300418092906701</v>
+        <v>0.5</v>
       </c>
       <c r="E5">
-        <v>22.6916329781867</v>
+        <v>20</v>
       </c>
       <c r="F5">
-        <v>0.26612874665899</v>
+        <v>0.5</v>
       </c>
       <c r="G5">
-        <v>0.37523477692567803</v>
+        <v>0.5</v>
       </c>
       <c r="H5">
-        <v>1.26533178214389E-2</v>
+        <v>0.1</v>
       </c>
       <c r="I5">
-        <v>17.900001759034701</v>
+        <v>18</v>
       </c>
       <c r="J5">
-        <v>4.3813630782996</v>
+        <v>5</v>
       </c>
       <c r="K5">
-        <v>28.000003830984099</v>
+        <v>28</v>
       </c>
       <c r="L5">
-        <v>49.999723164656601</v>
+        <v>50</v>
       </c>
       <c r="M5">
-        <v>1018.28520115629</v>
+        <v>1200</v>
       </c>
       <c r="N5">
-        <v>28.610318541424899</v>
+        <v>30</v>
       </c>
       <c r="O5">
-        <v>1168.60417302562</v>
+        <v>1100</v>
       </c>
       <c r="P5" s="1">
-        <v>2.1938524825922701E-10</v>
+        <v>1E-8</v>
       </c>
       <c r="Q5" s="1">
-        <v>5.9147338702993104E-11</v>
+        <v>1E-8</v>
       </c>
       <c r="R5" s="1">
-        <v>2.24744064996045E-14</v>
+        <v>1E-8</v>
       </c>
       <c r="S5">
-        <v>84.478542963583806</v>
+        <v>50</v>
       </c>
       <c r="T5">
-        <v>130.646562144711</v>
+        <v>130</v>
       </c>
       <c r="U5" s="1">
-        <v>3.14997619325491E-8</v>
-      </c>
-      <c r="V5" s="1">
-        <v>3.2019909031230802E-5</v>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="V5">
+        <v>0.01</v>
       </c>
       <c r="W5">
-        <v>3.9504512379276496E-3</v>
+        <v>2</v>
       </c>
       <c r="X5">
-        <v>577.13350254920397</v>
+        <v>350</v>
       </c>
       <c r="Y5" s="1">
-        <v>3.14988888393161E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="Z5" s="1">
-        <v>3.1498887648570001E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="AA5" s="1">
-        <v>3.1498890700959E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="AB5" s="1">
-        <v>3.1498887520172697E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="AC5" s="1">
-        <v>3.1498890700959E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="AD5">
-        <v>86.999999162376994</v>
+        <v>87</v>
       </c>
       <c r="AE5">
-        <v>425.00000000004701</v>
+        <v>425</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
@@ -6110,91 +6820,91 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>14.395965302157</v>
+        <v>15</v>
       </c>
       <c r="D6">
-        <v>5.7439358089912899E-2</v>
+        <v>0.5</v>
       </c>
       <c r="E6">
-        <v>22.9095362176583</v>
+        <v>20</v>
       </c>
       <c r="F6">
-        <v>0.26853658419603399</v>
+        <v>0.5</v>
       </c>
       <c r="G6">
-        <v>0.47255846135428597</v>
+        <v>0.5</v>
       </c>
       <c r="H6">
-        <v>1.4753203031975E-2</v>
+        <v>0.1</v>
       </c>
       <c r="I6">
-        <v>17.900001762535599</v>
+        <v>18</v>
       </c>
       <c r="J6">
-        <v>2.9243047280127898</v>
+        <v>5</v>
       </c>
       <c r="K6">
-        <v>28.000003838608599</v>
+        <v>28</v>
       </c>
       <c r="L6">
-        <v>49.9997228361784</v>
+        <v>50</v>
       </c>
       <c r="M6">
-        <v>1019.36716857009</v>
+        <v>1200</v>
       </c>
       <c r="N6">
-        <v>24.47459210233</v>
+        <v>20</v>
       </c>
       <c r="O6">
-        <v>1166.6526904365501</v>
+        <v>1100</v>
       </c>
       <c r="P6" s="1">
-        <v>2.1955601072794799E-10</v>
+        <v>1E-8</v>
       </c>
       <c r="Q6" s="1">
-        <v>5.9200708010223198E-11</v>
+        <v>1E-8</v>
       </c>
       <c r="R6" s="1">
-        <v>2.4604133854558401E-14</v>
+        <v>1E-8</v>
       </c>
       <c r="S6">
-        <v>84.302903391423996</v>
+        <v>50</v>
       </c>
       <c r="T6">
-        <v>130.53212152221801</v>
+        <v>130</v>
       </c>
       <c r="U6" s="1">
-        <v>3.1556020769271201E-8</v>
-      </c>
-      <c r="V6" s="1">
-        <v>3.20770974949901E-5</v>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="V6">
+        <v>0.01</v>
       </c>
       <c r="W6">
-        <v>3.9554075035385999E-3</v>
+        <v>2</v>
       </c>
       <c r="X6">
-        <v>577.42867509898599</v>
+        <v>350</v>
       </c>
       <c r="Y6" s="1">
-        <v>3.1555146115612202E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="Z6" s="1">
-        <v>3.1555144922752299E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="AA6" s="1">
-        <v>3.1555147980559602E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="AB6" s="1">
-        <v>3.1555144794127203E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="AC6" s="1">
-        <v>3.1555147980559602E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="AD6">
-        <v>86.999999160709905</v>
+        <v>87</v>
       </c>
       <c r="AE6">
-        <v>425.00000000005099</v>
+        <v>425</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
@@ -6205,91 +6915,91 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>14.3500493797647</v>
+        <v>15</v>
       </c>
       <c r="D7">
-        <v>4.7219465114919701E-2</v>
+        <v>0.5</v>
       </c>
       <c r="E7">
-        <v>23.079430934547901</v>
+        <v>20</v>
       </c>
       <c r="F7">
-        <v>0.269951648479759</v>
+        <v>0.5</v>
       </c>
       <c r="G7">
-        <v>0.47515958099733302</v>
+        <v>0.5</v>
       </c>
       <c r="H7">
-        <v>1.5970634327309802E-2</v>
+        <v>0.1</v>
       </c>
       <c r="I7">
-        <v>17.900001766043399</v>
+        <v>18</v>
       </c>
       <c r="J7">
-        <v>2.1911105202131198</v>
+        <v>5</v>
       </c>
       <c r="K7">
-        <v>28.000003846248301</v>
+        <v>28</v>
       </c>
       <c r="L7">
-        <v>49.999722507319497</v>
+        <v>50</v>
       </c>
       <c r="M7">
-        <v>1020.4466328645</v>
+        <v>1200</v>
       </c>
       <c r="N7">
-        <v>21.664366649243799</v>
+        <v>20</v>
       </c>
       <c r="O7">
-        <v>1163.94289399628</v>
+        <v>1100</v>
       </c>
       <c r="P7" s="1">
-        <v>2.1972809718705899E-10</v>
+        <v>1E-8</v>
       </c>
       <c r="Q7" s="1">
-        <v>5.9257841918964701E-11</v>
+        <v>1E-8</v>
       </c>
       <c r="R7" s="1">
-        <v>2.82742072015921E-14</v>
+        <v>1E-8</v>
       </c>
       <c r="S7">
-        <v>84.1134600374223</v>
+        <v>50</v>
       </c>
       <c r="T7">
-        <v>130.396796067769</v>
+        <v>130</v>
       </c>
       <c r="U7" s="1">
-        <v>3.1612380080523598E-8</v>
-      </c>
-      <c r="V7" s="1">
-        <v>3.2134388096320103E-5</v>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="V7">
+        <v>0.01</v>
       </c>
       <c r="W7">
-        <v>3.9603700571605397E-3</v>
+        <v>2</v>
       </c>
       <c r="X7">
-        <v>577.77772577208998</v>
+        <v>350</v>
       </c>
       <c r="Y7" s="1">
-        <v>3.1611503863647097E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="Z7" s="1">
-        <v>3.1611502668669797E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="AA7" s="1">
-        <v>3.1611505731905E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="AB7" s="1">
-        <v>3.16115025398163E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="AC7" s="1">
-        <v>3.1611505731905E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="AD7">
-        <v>86.999999159039504</v>
+        <v>87</v>
       </c>
       <c r="AE7">
-        <v>425.00000000005502</v>
+        <v>425</v>
       </c>
     </row>
   </sheetData>
@@ -6298,6 +7008,683 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5589379-171B-4A97-AC18-14A5DD584161}">
+  <dimension ref="A1:AE7"/>
+  <sheetViews>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="AA3" sqref="AA3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V1" t="s">
+        <v>43</v>
+      </c>
+      <c r="W1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>16</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>0.5</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>18</v>
+      </c>
+      <c r="J2">
+        <v>30</v>
+      </c>
+      <c r="K2">
+        <v>28.000003808201399</v>
+      </c>
+      <c r="L2">
+        <v>50</v>
+      </c>
+      <c r="M2">
+        <v>1100</v>
+      </c>
+      <c r="N2">
+        <v>60</v>
+      </c>
+      <c r="O2">
+        <v>1200</v>
+      </c>
+      <c r="P2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="R2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="S2">
+        <v>90</v>
+      </c>
+      <c r="T2">
+        <v>130</v>
+      </c>
+      <c r="U2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="V2" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="W2">
+        <v>0.1</v>
+      </c>
+      <c r="X2">
+        <v>500</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AD2">
+        <v>86.999999167358396</v>
+      </c>
+      <c r="AE2">
+        <v>425.00000000003598</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>0.5</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0.5</v>
+      </c>
+      <c r="I3">
+        <v>18</v>
+      </c>
+      <c r="J3">
+        <v>20</v>
+      </c>
+      <c r="K3">
+        <v>28.000003815780602</v>
+      </c>
+      <c r="L3">
+        <v>50</v>
+      </c>
+      <c r="M3">
+        <v>1100</v>
+      </c>
+      <c r="N3">
+        <v>50</v>
+      </c>
+      <c r="O3">
+        <v>1200</v>
+      </c>
+      <c r="P3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="R3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="S3">
+        <v>90</v>
+      </c>
+      <c r="T3">
+        <v>130</v>
+      </c>
+      <c r="U3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="V3" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="W3">
+        <v>0.1</v>
+      </c>
+      <c r="X3">
+        <v>500</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AD3">
+        <v>86.999999165701198</v>
+      </c>
+      <c r="AE3">
+        <v>425.00000000003899</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>0.5</v>
+      </c>
+      <c r="G4">
+        <v>0.5</v>
+      </c>
+      <c r="H4">
+        <v>0.1</v>
+      </c>
+      <c r="I4">
+        <v>18</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="K4">
+        <v>28.000003823374801</v>
+      </c>
+      <c r="L4">
+        <v>50</v>
+      </c>
+      <c r="M4">
+        <v>1100</v>
+      </c>
+      <c r="N4">
+        <v>40</v>
+      </c>
+      <c r="O4">
+        <v>1200</v>
+      </c>
+      <c r="P4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="R4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="S4">
+        <v>90</v>
+      </c>
+      <c r="T4">
+        <v>130</v>
+      </c>
+      <c r="U4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="V4" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="W4">
+        <v>0.1</v>
+      </c>
+      <c r="X4">
+        <v>500</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AD4">
+        <v>86.999999164040801</v>
+      </c>
+      <c r="AE4">
+        <v>425.00000000004297</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>16</v>
+      </c>
+      <c r="D5">
+        <v>0.5</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>0.5</v>
+      </c>
+      <c r="G5">
+        <v>0.5</v>
+      </c>
+      <c r="H5">
+        <v>0.1</v>
+      </c>
+      <c r="I5">
+        <v>18</v>
+      </c>
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>28.000003830984099</v>
+      </c>
+      <c r="L5">
+        <v>50</v>
+      </c>
+      <c r="M5">
+        <v>1100</v>
+      </c>
+      <c r="N5">
+        <v>30</v>
+      </c>
+      <c r="O5">
+        <v>1200</v>
+      </c>
+      <c r="P5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="R5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="S5">
+        <v>90</v>
+      </c>
+      <c r="T5">
+        <v>130</v>
+      </c>
+      <c r="U5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="V5" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="W5">
+        <v>0.1</v>
+      </c>
+      <c r="X5">
+        <v>500</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AD5">
+        <v>86.999999162376994</v>
+      </c>
+      <c r="AE5">
+        <v>425.00000000004701</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>0.5</v>
+      </c>
+      <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <v>0.5</v>
+      </c>
+      <c r="G6">
+        <v>0.5</v>
+      </c>
+      <c r="H6">
+        <v>0.1</v>
+      </c>
+      <c r="I6">
+        <v>18</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>28.000003838608599</v>
+      </c>
+      <c r="L6">
+        <v>50</v>
+      </c>
+      <c r="M6">
+        <v>1100</v>
+      </c>
+      <c r="N6">
+        <v>25</v>
+      </c>
+      <c r="O6">
+        <v>1200</v>
+      </c>
+      <c r="P6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="R6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="S6">
+        <v>90</v>
+      </c>
+      <c r="T6">
+        <v>130</v>
+      </c>
+      <c r="U6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="V6" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="W6">
+        <v>0.1</v>
+      </c>
+      <c r="X6">
+        <v>500</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AD6">
+        <v>86.999999160709905</v>
+      </c>
+      <c r="AE6">
+        <v>425.00000000005099</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <v>0.5</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>0.5</v>
+      </c>
+      <c r="G7">
+        <v>0.5</v>
+      </c>
+      <c r="H7">
+        <v>0.1</v>
+      </c>
+      <c r="I7">
+        <v>18</v>
+      </c>
+      <c r="J7">
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <v>28.000003846248301</v>
+      </c>
+      <c r="L7">
+        <v>50</v>
+      </c>
+      <c r="M7">
+        <v>1100</v>
+      </c>
+      <c r="N7">
+        <v>25</v>
+      </c>
+      <c r="O7">
+        <v>1200</v>
+      </c>
+      <c r="P7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="R7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="S7">
+        <v>90</v>
+      </c>
+      <c r="T7">
+        <v>130</v>
+      </c>
+      <c r="U7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="V7" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="W7">
+        <v>0.1</v>
+      </c>
+      <c r="X7">
+        <v>500</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AD7">
+        <v>86.999999159039504</v>
+      </c>
+      <c r="AE7">
+        <v>425.00000000005502</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC5318B9-9FE8-4735-97AC-C84ECA362166}">
   <dimension ref="A1:AE7"/>
   <sheetViews>
@@ -6975,7 +8362,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56C0A5FC-7678-45CB-A7B0-500412E1C0CC}">
   <dimension ref="A1:AE7"/>
   <sheetViews>
@@ -7650,704 +9037,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1A144BC-89D4-47F0-9D49-ED1B9234D74F}">
-  <dimension ref="A1:AE7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="3" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="29" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="34" max="16384" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="C2" s="2">
-        <v>25</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="E2" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="G2" s="2">
-        <v>2</v>
-      </c>
-      <c r="H2" s="2">
-        <v>80</v>
-      </c>
-      <c r="I2" s="2">
-        <v>18</v>
-      </c>
-      <c r="J2" s="2">
-        <v>50</v>
-      </c>
-      <c r="K2" s="2">
-        <v>28</v>
-      </c>
-      <c r="L2" s="2">
-        <v>50</v>
-      </c>
-      <c r="M2" s="2">
-        <v>3600</v>
-      </c>
-      <c r="N2" s="2">
-        <v>70</v>
-      </c>
-      <c r="O2" s="2">
-        <v>4500</v>
-      </c>
-      <c r="P2" s="2">
-        <v>60</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="R2" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="S2" s="2">
-        <v>250</v>
-      </c>
-      <c r="T2" s="2">
-        <v>110</v>
-      </c>
-      <c r="U2" s="2">
-        <v>4000</v>
-      </c>
-      <c r="V2" s="2">
-        <v>10</v>
-      </c>
-      <c r="W2" s="2">
-        <v>1</v>
-      </c>
-      <c r="X2" s="2">
-        <v>1000</v>
-      </c>
-      <c r="Y2" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="Z2" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AA2" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AB2" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AC2" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AD2" s="2">
-        <v>87</v>
-      </c>
-      <c r="AE2" s="2">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>25</v>
-      </c>
-      <c r="D3" s="2">
-        <v>20</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="G3" s="2">
-        <v>2</v>
-      </c>
-      <c r="H3" s="2">
-        <v>90</v>
-      </c>
-      <c r="I3" s="2">
-        <v>18</v>
-      </c>
-      <c r="J3" s="2">
-        <v>60</v>
-      </c>
-      <c r="K3" s="2">
-        <v>28</v>
-      </c>
-      <c r="L3" s="2">
-        <v>50</v>
-      </c>
-      <c r="M3" s="2">
-        <v>1200</v>
-      </c>
-      <c r="N3" s="2">
-        <v>60</v>
-      </c>
-      <c r="O3" s="2">
-        <v>1500</v>
-      </c>
-      <c r="P3" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="R3" s="2">
-        <v>1</v>
-      </c>
-      <c r="S3" s="2">
-        <v>90</v>
-      </c>
-      <c r="T3" s="2">
-        <v>110</v>
-      </c>
-      <c r="U3" s="2">
-        <v>1000</v>
-      </c>
-      <c r="V3" s="2">
-        <v>10</v>
-      </c>
-      <c r="W3" s="2">
-        <v>1</v>
-      </c>
-      <c r="X3" s="2">
-        <v>500</v>
-      </c>
-      <c r="Y3" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="Z3" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AA3" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AB3" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AC3" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AD3" s="2">
-        <v>87</v>
-      </c>
-      <c r="AE3" s="2">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="C4" s="2">
-        <v>25</v>
-      </c>
-      <c r="D4" s="2">
-        <v>5</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1</v>
-      </c>
-      <c r="H4" s="2">
-        <v>10</v>
-      </c>
-      <c r="I4" s="2">
-        <v>18</v>
-      </c>
-      <c r="J4" s="2">
-        <v>50</v>
-      </c>
-      <c r="K4" s="2">
-        <v>28</v>
-      </c>
-      <c r="L4" s="2">
-        <v>50</v>
-      </c>
-      <c r="M4" s="2">
-        <v>1000</v>
-      </c>
-      <c r="N4" s="2">
-        <v>30</v>
-      </c>
-      <c r="O4" s="2">
-        <v>1300</v>
-      </c>
-      <c r="P4" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="R4" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="S4" s="2">
-        <v>80</v>
-      </c>
-      <c r="T4" s="2">
-        <v>110</v>
-      </c>
-      <c r="U4" s="2">
-        <v>1000</v>
-      </c>
-      <c r="V4" s="2">
-        <v>10</v>
-      </c>
-      <c r="W4" s="2">
-        <v>1</v>
-      </c>
-      <c r="X4" s="2">
-        <v>500</v>
-      </c>
-      <c r="Y4" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="Z4" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AA4" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AB4" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AC4" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AD4" s="2">
-        <v>87</v>
-      </c>
-      <c r="AE4" s="2">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2">
-        <v>25</v>
-      </c>
-      <c r="D5" s="2">
-        <v>5</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="G5" s="2">
-        <v>1</v>
-      </c>
-      <c r="H5" s="2">
-        <v>5</v>
-      </c>
-      <c r="I5" s="2">
-        <v>18</v>
-      </c>
-      <c r="J5" s="2">
-        <v>50</v>
-      </c>
-      <c r="K5" s="2">
-        <v>28</v>
-      </c>
-      <c r="L5" s="2">
-        <v>50</v>
-      </c>
-      <c r="M5" s="2">
-        <v>1000</v>
-      </c>
-      <c r="N5" s="2">
-        <v>25</v>
-      </c>
-      <c r="O5" s="2">
-        <v>1300</v>
-      </c>
-      <c r="P5" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="R5" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="S5" s="2">
-        <v>80</v>
-      </c>
-      <c r="T5" s="2">
-        <v>110</v>
-      </c>
-      <c r="U5" s="2">
-        <v>1000</v>
-      </c>
-      <c r="V5" s="2">
-        <v>10</v>
-      </c>
-      <c r="W5" s="2">
-        <v>1</v>
-      </c>
-      <c r="X5" s="2">
-        <v>500</v>
-      </c>
-      <c r="Y5" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="Z5" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AA5" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AB5" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AC5" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AD5" s="2">
-        <v>87</v>
-      </c>
-      <c r="AE5" s="2">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" s="2">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2">
-        <v>25</v>
-      </c>
-      <c r="D6" s="2">
-        <v>2</v>
-      </c>
-      <c r="E6" s="2">
-        <v>3</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="H6" s="2">
-        <v>1</v>
-      </c>
-      <c r="I6" s="2">
-        <v>18</v>
-      </c>
-      <c r="J6" s="2">
-        <v>50</v>
-      </c>
-      <c r="K6" s="2">
-        <v>28</v>
-      </c>
-      <c r="L6" s="2">
-        <v>50</v>
-      </c>
-      <c r="M6" s="2">
-        <v>1000</v>
-      </c>
-      <c r="N6" s="2">
-        <v>25</v>
-      </c>
-      <c r="O6" s="2">
-        <v>1300</v>
-      </c>
-      <c r="P6" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="R6" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="S6" s="2">
-        <v>80</v>
-      </c>
-      <c r="T6" s="2">
-        <v>110</v>
-      </c>
-      <c r="U6" s="2">
-        <v>1000</v>
-      </c>
-      <c r="V6" s="2">
-        <v>10</v>
-      </c>
-      <c r="W6" s="2">
-        <v>1</v>
-      </c>
-      <c r="X6" s="2">
-        <v>500</v>
-      </c>
-      <c r="Y6" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="Z6" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AA6" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AB6" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AC6" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AD6" s="2">
-        <v>87</v>
-      </c>
-      <c r="AE6" s="2">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" s="2">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2">
-        <v>25</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E7" s="2">
-        <v>5</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="H7" s="2">
-        <v>1</v>
-      </c>
-      <c r="I7" s="2">
-        <v>18</v>
-      </c>
-      <c r="J7" s="2">
-        <v>45</v>
-      </c>
-      <c r="K7" s="2">
-        <v>28</v>
-      </c>
-      <c r="L7" s="2">
-        <v>50</v>
-      </c>
-      <c r="M7" s="2">
-        <v>1000</v>
-      </c>
-      <c r="N7" s="2">
-        <v>25</v>
-      </c>
-      <c r="O7" s="2">
-        <v>1300</v>
-      </c>
-      <c r="P7" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q7" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="R7" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="S7" s="2">
-        <v>80</v>
-      </c>
-      <c r="T7" s="2">
-        <v>110</v>
-      </c>
-      <c r="U7" s="2">
-        <v>1000</v>
-      </c>
-      <c r="V7" s="2">
-        <v>10</v>
-      </c>
-      <c r="W7" s="2">
-        <v>1</v>
-      </c>
-      <c r="X7" s="2">
-        <v>500</v>
-      </c>
-      <c r="Y7" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="Z7" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AA7" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AB7" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AC7" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AD7" s="2">
-        <v>87</v>
-      </c>
-      <c r="AE7" s="2">
-        <v>425</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
checkpoint converged to ss
</commit_message>
<xml_diff>
--- a/exposan/werf/data/initial_conditions.xlsx
+++ b/exposan/werf/data/initial_conditions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joy_c\Dropbox\PhD\Research\QSD\codes_developing\EXPOsan\exposan\werf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87A50F0-63ED-45AA-8571-ABBA89F72873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E2D26A-51C4-40BF-822E-AE1021111414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23133" yWindow="-93" windowWidth="23226" windowHeight="13866" activeTab="10" xr2:uid="{218DD762-44D5-4240-B5CB-C558EBE30BA7}"/>
+    <workbookView xWindow="1290" yWindow="3135" windowWidth="22440" windowHeight="13680" firstSheet="2" activeTab="11" xr2:uid="{218DD762-44D5-4240-B5CB-C558EBE30BA7}"/>
   </bookViews>
   <sheets>
     <sheet name="B1" sheetId="6" r:id="rId1"/>
@@ -24,12 +24,13 @@
     <sheet name="G2" sheetId="13" r:id="rId9"/>
     <sheet name="G3" sheetId="14" r:id="rId10"/>
     <sheet name="H1" sheetId="20" r:id="rId11"/>
-    <sheet name="I1" sheetId="17" r:id="rId12"/>
-    <sheet name="I2" sheetId="16" r:id="rId13"/>
-    <sheet name="I3" sheetId="18" r:id="rId14"/>
-    <sheet name="N1" sheetId="19" r:id="rId15"/>
-    <sheet name="AED" sheetId="10" r:id="rId16"/>
-    <sheet name="adm" sheetId="2" r:id="rId17"/>
+    <sheet name="H" sheetId="21" r:id="rId12"/>
+    <sheet name="I1" sheetId="17" r:id="rId13"/>
+    <sheet name="I2" sheetId="16" r:id="rId14"/>
+    <sheet name="I3" sheetId="18" r:id="rId15"/>
+    <sheet name="N1" sheetId="19" r:id="rId16"/>
+    <sheet name="AED" sheetId="10" r:id="rId17"/>
+    <sheet name="adm" sheetId="2" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="75">
   <si>
     <t>S_O2</t>
   </si>
@@ -271,6 +272,12 @@
   </si>
   <si>
     <t>N1</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>H1</t>
   </si>
 </sst>
 </file>
@@ -2032,10 +2039,1431 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E599D95C-4D24-432D-9B3F-CE35D4365C13}">
+  <dimension ref="A1:AG21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="16" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V1" t="s">
+        <v>43</v>
+      </c>
+      <c r="W1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2">
+        <v>0.02</v>
+      </c>
+      <c r="C2">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <v>0.3</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>16</v>
+      </c>
+      <c r="J2">
+        <v>30</v>
+      </c>
+      <c r="K2">
+        <v>28</v>
+      </c>
+      <c r="L2">
+        <v>50</v>
+      </c>
+      <c r="M2">
+        <v>1300</v>
+      </c>
+      <c r="N2">
+        <v>50</v>
+      </c>
+      <c r="O2">
+        <v>1200</v>
+      </c>
+      <c r="P2">
+        <v>10</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>100</v>
+      </c>
+      <c r="T2">
+        <v>140</v>
+      </c>
+      <c r="U2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="V2">
+        <v>2</v>
+      </c>
+      <c r="W2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X2">
+        <v>150</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA2">
+        <v>150</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AD2">
+        <v>87</v>
+      </c>
+      <c r="AE2">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3">
+        <v>1E-3</v>
+      </c>
+      <c r="C3">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>0.3</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0.5</v>
+      </c>
+      <c r="I3">
+        <v>16</v>
+      </c>
+      <c r="J3">
+        <v>30</v>
+      </c>
+      <c r="K3">
+        <v>28</v>
+      </c>
+      <c r="L3">
+        <v>50</v>
+      </c>
+      <c r="M3">
+        <v>1300</v>
+      </c>
+      <c r="N3">
+        <v>40</v>
+      </c>
+      <c r="O3">
+        <v>1200</v>
+      </c>
+      <c r="P3">
+        <v>10</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>100</v>
+      </c>
+      <c r="T3">
+        <v>140</v>
+      </c>
+      <c r="U3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="V3">
+        <v>2</v>
+      </c>
+      <c r="W3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X3">
+        <v>150</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA3">
+        <v>150</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AD3">
+        <v>87</v>
+      </c>
+      <c r="AE3">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>0.3</v>
+      </c>
+      <c r="G4">
+        <v>0.5</v>
+      </c>
+      <c r="H4">
+        <v>0.1</v>
+      </c>
+      <c r="I4">
+        <v>16</v>
+      </c>
+      <c r="J4">
+        <v>15</v>
+      </c>
+      <c r="K4">
+        <v>28</v>
+      </c>
+      <c r="L4">
+        <v>50</v>
+      </c>
+      <c r="M4">
+        <v>1300</v>
+      </c>
+      <c r="N4">
+        <v>30</v>
+      </c>
+      <c r="O4">
+        <v>1200</v>
+      </c>
+      <c r="P4">
+        <v>10</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>100</v>
+      </c>
+      <c r="T4">
+        <v>140</v>
+      </c>
+      <c r="U4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="V4">
+        <v>2</v>
+      </c>
+      <c r="W4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X4">
+        <v>150</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA4">
+        <v>150</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AD4">
+        <v>87</v>
+      </c>
+      <c r="AE4">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>0.3</v>
+      </c>
+      <c r="G5">
+        <v>0.5</v>
+      </c>
+      <c r="H5">
+        <v>0.1</v>
+      </c>
+      <c r="I5">
+        <v>16</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <v>28</v>
+      </c>
+      <c r="L5">
+        <v>50</v>
+      </c>
+      <c r="M5">
+        <v>1300</v>
+      </c>
+      <c r="N5">
+        <v>25</v>
+      </c>
+      <c r="O5">
+        <v>1200</v>
+      </c>
+      <c r="P5">
+        <v>10</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>100</v>
+      </c>
+      <c r="T5">
+        <v>140</v>
+      </c>
+      <c r="U5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="V5">
+        <v>2</v>
+      </c>
+      <c r="W5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X5">
+        <v>150</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA5">
+        <v>150</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AD5">
+        <v>87</v>
+      </c>
+      <c r="AE5">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6">
+        <v>0.05</v>
+      </c>
+      <c r="C6">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>0.5</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>0.3</v>
+      </c>
+      <c r="G6">
+        <v>0.5</v>
+      </c>
+      <c r="H6">
+        <v>0.1</v>
+      </c>
+      <c r="I6">
+        <v>16</v>
+      </c>
+      <c r="J6">
+        <v>10</v>
+      </c>
+      <c r="K6">
+        <v>28</v>
+      </c>
+      <c r="L6">
+        <v>50</v>
+      </c>
+      <c r="M6">
+        <v>1300</v>
+      </c>
+      <c r="N6">
+        <v>25</v>
+      </c>
+      <c r="O6">
+        <v>1200</v>
+      </c>
+      <c r="P6">
+        <v>10</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>100</v>
+      </c>
+      <c r="T6">
+        <v>140</v>
+      </c>
+      <c r="U6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="V6">
+        <v>2</v>
+      </c>
+      <c r="W6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X6">
+        <v>150</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA6">
+        <v>150</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AD6">
+        <v>87</v>
+      </c>
+      <c r="AE6">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>0.5</v>
+      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <v>0.3</v>
+      </c>
+      <c r="G7">
+        <v>0.5</v>
+      </c>
+      <c r="H7">
+        <v>0.1</v>
+      </c>
+      <c r="I7">
+        <v>16</v>
+      </c>
+      <c r="J7">
+        <v>10</v>
+      </c>
+      <c r="K7">
+        <v>28</v>
+      </c>
+      <c r="L7">
+        <v>50</v>
+      </c>
+      <c r="M7">
+        <v>1300</v>
+      </c>
+      <c r="N7">
+        <v>25</v>
+      </c>
+      <c r="O7">
+        <v>1200</v>
+      </c>
+      <c r="P7">
+        <v>10</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>100</v>
+      </c>
+      <c r="T7">
+        <v>140</v>
+      </c>
+      <c r="U7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="V7">
+        <v>2</v>
+      </c>
+      <c r="W7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X7">
+        <v>150</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA7">
+        <v>150</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AD7">
+        <v>87</v>
+      </c>
+      <c r="AE7">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" t="s">
+        <v>15</v>
+      </c>
+      <c r="M10" t="s">
+        <v>8</v>
+      </c>
+      <c r="N10" t="s">
+        <v>9</v>
+      </c>
+      <c r="O10" t="s">
+        <v>10</v>
+      </c>
+      <c r="P10" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>12</v>
+      </c>
+      <c r="R10" t="s">
+        <v>13</v>
+      </c>
+      <c r="S10" t="s">
+        <v>19</v>
+      </c>
+      <c r="T10" t="s">
+        <v>18</v>
+      </c>
+      <c r="U10" t="s">
+        <v>47</v>
+      </c>
+      <c r="V10" t="s">
+        <v>43</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X10" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>1.86178545508357E-2</v>
+      </c>
+      <c r="C11">
+        <v>18.705401257864001</v>
+      </c>
+      <c r="D11">
+        <v>6.4100403605532401</v>
+      </c>
+      <c r="E11">
+        <v>5.5201802808141904</v>
+      </c>
+      <c r="F11">
+        <v>0.28508549233059799</v>
+      </c>
+      <c r="G11">
+        <v>1.8387596731704601</v>
+      </c>
+      <c r="H11">
+        <v>1.3210092375717699</v>
+      </c>
+      <c r="I11">
+        <v>15.3642918877258</v>
+      </c>
+      <c r="J11">
+        <v>26.892706135865499</v>
+      </c>
+      <c r="K11">
+        <v>28.001366868521899</v>
+      </c>
+      <c r="L11">
+        <v>49.808199525011602</v>
+      </c>
+      <c r="M11">
+        <v>1325.8059861367699</v>
+      </c>
+      <c r="N11">
+        <v>40.818816012537802</v>
+      </c>
+      <c r="O11">
+        <v>1277.2256189694001</v>
+      </c>
+      <c r="P11">
+        <v>3.4499346929127701</v>
+      </c>
+      <c r="Q11">
+        <v>0.44864213707331502</v>
+      </c>
+      <c r="R11">
+        <v>1.40605155135318E-2</v>
+      </c>
+      <c r="S11">
+        <v>96.4307757584168</v>
+      </c>
+      <c r="T11">
+        <v>137.67574126186301</v>
+      </c>
+      <c r="U11" s="1">
+        <v>2.2248168068096101E-8</v>
+      </c>
+      <c r="V11">
+        <v>2.0416782790847599</v>
+      </c>
+      <c r="W11" s="1">
+        <v>5.0533577099473898E-6</v>
+      </c>
+      <c r="X11">
+        <v>161.829156416785</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>2.2248168068096101E-8</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>163.35430194664099</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>2.2248167909736601E-8</v>
+      </c>
+      <c r="AC11" s="1">
+        <v>2.2248168291581201E-8</v>
+      </c>
+      <c r="AD11">
+        <v>86.977349047237198</v>
+      </c>
+      <c r="AE11">
+        <v>424.889348793973</v>
+      </c>
+      <c r="AF11">
+        <v>993797.90530903195</v>
+      </c>
+      <c r="AG11">
+        <v>166924.10420038801</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>3.917783854509E-4</v>
+      </c>
+      <c r="C12">
+        <v>19.511693431743701</v>
+      </c>
+      <c r="D12">
+        <v>6.3346852693685296</v>
+      </c>
+      <c r="E12">
+        <v>4.5640029514580203</v>
+      </c>
+      <c r="F12">
+        <v>0.24854552934655799</v>
+      </c>
+      <c r="G12">
+        <v>0.48258291340550702</v>
+      </c>
+      <c r="H12">
+        <v>0.23529728817302301</v>
+      </c>
+      <c r="I12">
+        <v>15.364294688276299</v>
+      </c>
+      <c r="J12">
+        <v>26.940749777123401</v>
+      </c>
+      <c r="K12">
+        <v>28.000912185763099</v>
+      </c>
+      <c r="L12">
+        <v>49.807917750332201</v>
+      </c>
+      <c r="M12">
+        <v>1325.9954092538601</v>
+      </c>
+      <c r="N12">
+        <v>37.970927551296398</v>
+      </c>
+      <c r="O12">
+        <v>1279.5352004224501</v>
+      </c>
+      <c r="P12">
+        <v>3.4584448394092302</v>
+      </c>
+      <c r="Q12">
+        <v>0.45056601885326403</v>
+      </c>
+      <c r="R12">
+        <v>1.16336815749128E-2</v>
+      </c>
+      <c r="S12">
+        <v>96.391588263550702</v>
+      </c>
+      <c r="T12">
+        <v>137.66137634529699</v>
+      </c>
+      <c r="U12" s="1">
+        <v>2.22375551607491E-8</v>
+      </c>
+      <c r="V12">
+        <v>2.0416111013437299</v>
+      </c>
+      <c r="W12" s="1">
+        <v>5.0486119033987796E-6</v>
+      </c>
+      <c r="X12">
+        <v>161.85132834599401</v>
+      </c>
+      <c r="Y12" s="1">
+        <v>2.22375551607491E-8</v>
+      </c>
+      <c r="Z12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="1">
+        <v>163.33775120241199</v>
+      </c>
+      <c r="AB12" s="1">
+        <v>2.2237555002780701E-8</v>
+      </c>
+      <c r="AC12" s="1">
+        <v>2.2237555383682199E-8</v>
+      </c>
+      <c r="AD12">
+        <v>86.977349070396002</v>
+      </c>
+      <c r="AE12">
+        <v>424.88934890710499</v>
+      </c>
+      <c r="AF12">
+        <v>993796.79694345302</v>
+      </c>
+      <c r="AG12">
+        <v>166924.10420038801</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>16.659737728264101</v>
+      </c>
+      <c r="D13">
+        <v>1.5499877134971201</v>
+      </c>
+      <c r="E13">
+        <v>9.3235963622053593</v>
+      </c>
+      <c r="F13">
+        <v>0.250126259884491</v>
+      </c>
+      <c r="G13">
+        <v>0.309381582499973</v>
+      </c>
+      <c r="H13">
+        <v>3.32509198906355E-2</v>
+      </c>
+      <c r="I13">
+        <v>15.3643023431069</v>
+      </c>
+      <c r="J13">
+        <v>12.9142053977706</v>
+      </c>
+      <c r="K13">
+        <v>28.0001118153276</v>
+      </c>
+      <c r="L13">
+        <v>49.807422615024201</v>
+      </c>
+      <c r="M13">
+        <v>1327.20186761888</v>
+      </c>
+      <c r="N13">
+        <v>30.948153276351601</v>
+      </c>
+      <c r="O13">
+        <v>1278.6559102414999</v>
+      </c>
+      <c r="P13">
+        <v>3.4646008355448799</v>
+      </c>
+      <c r="Q13">
+        <v>0.45477118105630698</v>
+      </c>
+      <c r="R13">
+        <v>2.8561477245780801E-3</v>
+      </c>
+      <c r="S13">
+        <v>97.252401089977397</v>
+      </c>
+      <c r="T13">
+        <v>137.611339663634</v>
+      </c>
+      <c r="U13" s="1">
+        <v>2.22084186154779E-8</v>
+      </c>
+      <c r="V13">
+        <v>2.0414277941143002</v>
+      </c>
+      <c r="W13" s="1">
+        <v>5.0355945925928803E-6</v>
+      </c>
+      <c r="X13">
+        <v>161.93964040080101</v>
+      </c>
+      <c r="Y13" s="1">
+        <v>2.22084186154779E-8</v>
+      </c>
+      <c r="Z13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="1">
+        <v>163.29248598137801</v>
+      </c>
+      <c r="AB13" s="1">
+        <v>2.22084184585762E-8</v>
+      </c>
+      <c r="AC13" s="1">
+        <v>2.2208418836905798E-8</v>
+      </c>
+      <c r="AD13">
+        <v>86.977349133706198</v>
+      </c>
+      <c r="AE13">
+        <v>424.88934921637701</v>
+      </c>
+      <c r="AF13">
+        <v>993793.76701472502</v>
+      </c>
+      <c r="AG13">
+        <v>166924.10420038801</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>15.371720123446799</v>
+      </c>
+      <c r="D14">
+        <v>0.24287174228213801</v>
+      </c>
+      <c r="E14">
+        <v>10.7592912110018</v>
+      </c>
+      <c r="F14">
+        <v>0.25750845123173399</v>
+      </c>
+      <c r="G14">
+        <v>0.29651792933701199</v>
+      </c>
+      <c r="H14">
+        <v>1.5035782145430601E-2</v>
+      </c>
+      <c r="I14">
+        <v>15.364310006080901</v>
+      </c>
+      <c r="J14">
+        <v>6.6868931689078499</v>
+      </c>
+      <c r="K14">
+        <v>28.000558641534099</v>
+      </c>
+      <c r="L14">
+        <v>49.807702805488297</v>
+      </c>
+      <c r="M14">
+        <v>1328.4059859598101</v>
+      </c>
+      <c r="N14">
+        <v>26.264650341820101</v>
+      </c>
+      <c r="O14">
+        <v>1276.10950525163</v>
+      </c>
+      <c r="P14">
+        <v>3.4662463154845402</v>
+      </c>
+      <c r="Q14">
+        <v>0.45599342533538101</v>
+      </c>
+      <c r="R14">
+        <v>8.4427872201377002E-4</v>
+      </c>
+      <c r="S14">
+        <v>97.309372273837397</v>
+      </c>
+      <c r="T14">
+        <v>137.49038444402501</v>
+      </c>
+      <c r="U14" s="1">
+        <v>2.2179122873573E-8</v>
+      </c>
+      <c r="V14">
+        <v>2.0412446060132301</v>
+      </c>
+      <c r="W14" s="1">
+        <v>5.0225179028182301E-6</v>
+      </c>
+      <c r="X14">
+        <v>162.21078104231299</v>
+      </c>
+      <c r="Y14" s="1">
+        <v>2.2179122873573E-8</v>
+      </c>
+      <c r="Z14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="1">
+        <v>163.24714614497799</v>
+      </c>
+      <c r="AB14" s="1">
+        <v>2.2179122717736401E-8</v>
+      </c>
+      <c r="AC14" s="1">
+        <v>2.21791230934976E-8</v>
+      </c>
+      <c r="AD14">
+        <v>86.977349197093105</v>
+      </c>
+      <c r="AE14">
+        <v>424.88934952602699</v>
+      </c>
+      <c r="AF14">
+        <v>993790.73343402694</v>
+      </c>
+      <c r="AG14">
+        <v>166924.10420038801</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>4.8970053077685802E-2</v>
+      </c>
+      <c r="C15">
+        <v>16.337555792362</v>
+      </c>
+      <c r="D15">
+        <v>0.24628231259267699</v>
+      </c>
+      <c r="E15">
+        <v>9.8059017442293506</v>
+      </c>
+      <c r="F15">
+        <v>0.25504663122592403</v>
+      </c>
+      <c r="G15">
+        <v>0.232752266988353</v>
+      </c>
+      <c r="H15">
+        <v>3.1920880116811802E-2</v>
+      </c>
+      <c r="I15">
+        <v>15.3643187960158</v>
+      </c>
+      <c r="J15">
+        <v>7.4484457753193096</v>
+      </c>
+      <c r="K15">
+        <v>28.000968468599201</v>
+      </c>
+      <c r="L15">
+        <v>49.807960376487301</v>
+      </c>
+      <c r="M15">
+        <v>1329.1923002467299</v>
+      </c>
+      <c r="N15">
+        <v>22.748087270468101</v>
+      </c>
+      <c r="O15">
+        <v>1274.41335895932</v>
+      </c>
+      <c r="P15">
+        <v>3.4776774938526902</v>
+      </c>
+      <c r="Q15">
+        <v>0.45765344752481901</v>
+      </c>
+      <c r="R15">
+        <v>8.3972219943019403E-4</v>
+      </c>
+      <c r="S15">
+        <v>97.199513573712593</v>
+      </c>
+      <c r="T15">
+        <v>137.38732749399901</v>
+      </c>
+      <c r="U15" s="1">
+        <v>2.2145350088190599E-8</v>
+      </c>
+      <c r="V15">
+        <v>2.04103489328357</v>
+      </c>
+      <c r="W15" s="1">
+        <v>5.0074581969888596E-6</v>
+      </c>
+      <c r="X15">
+        <v>162.429626335439</v>
+      </c>
+      <c r="Y15" s="1">
+        <v>2.2145350088190599E-8</v>
+      </c>
+      <c r="Z15" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="1">
+        <v>163.19510381032799</v>
+      </c>
+      <c r="AB15" s="1">
+        <v>2.21453499335725E-8</v>
+      </c>
+      <c r="AC15" s="1">
+        <v>2.21453503063956E-8</v>
+      </c>
+      <c r="AD15">
+        <v>86.9773492698166</v>
+      </c>
+      <c r="AE15">
+        <v>424.88934988128602</v>
+      </c>
+      <c r="AF15">
+        <v>993787.25310666102</v>
+      </c>
+      <c r="AG15">
+        <v>53361.744200388501</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>15.8320538313329</v>
+      </c>
+      <c r="D16">
+        <v>0.114690743338486</v>
+      </c>
+      <c r="E16">
+        <v>9.99568555172708</v>
+      </c>
+      <c r="F16">
+        <v>0.25986349649142299</v>
+      </c>
+      <c r="G16">
+        <v>0.305209512656758</v>
+      </c>
+      <c r="H16">
+        <v>2.0959158978757501E-2</v>
+      </c>
+      <c r="I16">
+        <v>15.3643208603325</v>
+      </c>
+      <c r="J16">
+        <v>5.97104230608167</v>
+      </c>
+      <c r="K16">
+        <v>28.001144991950799</v>
+      </c>
+      <c r="L16">
+        <v>49.808070770651803</v>
+      </c>
+      <c r="M16">
+        <v>1329.5153019500899</v>
+      </c>
+      <c r="N16">
+        <v>22.0813295571362</v>
+      </c>
+      <c r="O16">
+        <v>1273.3172946030199</v>
+      </c>
+      <c r="P16">
+        <v>3.4779692663620301</v>
+      </c>
+      <c r="Q16">
+        <v>0.45785122510170601</v>
+      </c>
+      <c r="R16">
+        <v>6.5911387337076104E-4</v>
+      </c>
+      <c r="S16">
+        <v>97.166338394184805</v>
+      </c>
+      <c r="T16">
+        <v>137.348062993914</v>
+      </c>
+      <c r="U16" s="1">
+        <v>2.2137409255818799E-8</v>
+      </c>
+      <c r="V16">
+        <v>2.04098566519863</v>
+      </c>
+      <c r="W16" s="1">
+        <v>5.0039181249820599E-6</v>
+      </c>
+      <c r="X16">
+        <v>162.51987172454699</v>
+      </c>
+      <c r="Y16" s="1">
+        <v>2.2137409255818799E-8</v>
+      </c>
+      <c r="Z16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="1">
+        <v>163.18287976415101</v>
+      </c>
+      <c r="AB16" s="1">
+        <v>2.21374091014867E-8</v>
+      </c>
+      <c r="AC16" s="1">
+        <v>2.2137409473620299E-8</v>
+      </c>
+      <c r="AD16">
+        <v>86.977349286896597</v>
+      </c>
+      <c r="AE16">
+        <v>424.88934996472301</v>
+      </c>
+      <c r="AF16">
+        <v>993786.43571731099</v>
+      </c>
+      <c r="AG16">
+        <v>53361.744200388501</v>
+      </c>
+    </row>
+    <row r="17" spans="18:29" x14ac:dyDescent="0.25">
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="1"/>
+    </row>
+    <row r="18" spans="18:29" x14ac:dyDescent="0.25">
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="1"/>
+    </row>
+    <row r="19" spans="18:29" x14ac:dyDescent="0.25">
+      <c r="R19" s="1"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1"/>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="1"/>
+      <c r="AC19" s="1"/>
+    </row>
+    <row r="20" spans="18:29" x14ac:dyDescent="0.25">
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="1"/>
+    </row>
+    <row r="21" spans="18:29" x14ac:dyDescent="0.25">
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="1"/>
+      <c r="AC21" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FA85F62-9524-4DFD-AED1-1DC5BC35C55C}">
   <dimension ref="A1:AE21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2180,7 +3608,7 @@
         <v>50</v>
       </c>
       <c r="O2">
-        <v>1200</v>
+        <v>2000</v>
       </c>
       <c r="P2">
         <v>10</v>
@@ -2275,7 +3703,7 @@
         <v>40</v>
       </c>
       <c r="O3">
-        <v>1200</v>
+        <v>2000</v>
       </c>
       <c r="P3">
         <v>10</v>
@@ -2370,7 +3798,7 @@
         <v>30</v>
       </c>
       <c r="O4">
-        <v>1200</v>
+        <v>2000</v>
       </c>
       <c r="P4">
         <v>10</v>
@@ -2465,7 +3893,7 @@
         <v>25</v>
       </c>
       <c r="O5">
-        <v>1200</v>
+        <v>2000</v>
       </c>
       <c r="P5">
         <v>10</v>
@@ -2560,7 +3988,7 @@
         <v>25</v>
       </c>
       <c r="O6">
-        <v>1200</v>
+        <v>2000</v>
       </c>
       <c r="P6">
         <v>10</v>
@@ -2655,7 +4083,7 @@
         <v>25</v>
       </c>
       <c r="O7">
-        <v>1200</v>
+        <v>2000</v>
       </c>
       <c r="P7">
         <v>10</v>
@@ -2809,7 +4237,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D7FEF2-86A6-4650-A253-23D719FC805E}">
   <dimension ref="A1:AE21"/>
   <sheetViews>
@@ -3581,7 +5009,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E4487D-883D-4E85-B2E5-7356A39B3F61}">
   <dimension ref="A1:AE21"/>
   <sheetViews>
@@ -4305,7 +5733,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42016BA4-57DB-462D-9767-837B2F986A82}">
   <dimension ref="A1:AE7"/>
   <sheetViews>
@@ -4982,7 +6410,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12367F69-A662-4BD3-AE36-01641D10E752}">
   <dimension ref="A1:AE16"/>
   <sheetViews>
@@ -5720,7 +7148,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CB7F0C9-B54B-4F93-93CE-9E10B0EA4FF3}">
   <dimension ref="A1:AF7"/>
   <sheetViews>
@@ -6418,12 +7846,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{472A4E84-05F6-482F-94AF-2C8CE149BF8E}">
   <dimension ref="A1:AP57"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="AJ18" sqref="AJ18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7331,6 +8759,134 @@
         <v>87</v>
       </c>
       <c r="AP7">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>75</v>
+      </c>
+      <c r="E8">
+        <v>9</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>12</v>
+      </c>
+      <c r="H8">
+        <v>45</v>
+      </c>
+      <c r="I8">
+        <v>1E-4</v>
+      </c>
+      <c r="J8">
+        <v>100</v>
+      </c>
+      <c r="K8">
+        <v>900</v>
+      </c>
+      <c r="L8">
+        <v>1200</v>
+      </c>
+      <c r="M8">
+        <v>200</v>
+      </c>
+      <c r="N8">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="O8">
+        <v>20</v>
+      </c>
+      <c r="P8">
+        <v>20</v>
+      </c>
+      <c r="Q8">
+        <v>25</v>
+      </c>
+      <c r="R8">
+        <v>350</v>
+      </c>
+      <c r="S8">
+        <v>270</v>
+      </c>
+      <c r="T8">
+        <v>250</v>
+      </c>
+      <c r="U8">
+        <v>120</v>
+      </c>
+      <c r="V8">
+        <v>60</v>
+      </c>
+      <c r="W8">
+        <v>400</v>
+      </c>
+      <c r="X8">
+        <v>200</v>
+      </c>
+      <c r="Y8">
+        <v>13000</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA8" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC8">
+        <v>28</v>
+      </c>
+      <c r="AD8">
+        <v>0.3</v>
+      </c>
+      <c r="AE8">
+        <v>2</v>
+      </c>
+      <c r="AF8" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AG8">
+        <v>500</v>
+      </c>
+      <c r="AH8">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AI8">
+        <v>3000</v>
+      </c>
+      <c r="AJ8" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AK8" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AL8" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AM8" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AN8" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AO8">
+        <v>87</v>
+      </c>
+      <c r="AP8">
         <v>425</v>
       </c>
     </row>

</xml_diff>

<commit_message>
clean up H1 code
</commit_message>
<xml_diff>
--- a/exposan/werf/data/initial_conditions.xlsx
+++ b/exposan/werf/data/initial_conditions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joy_c\Dropbox\PhD\Research\QSD\codes_developing\EXPOsan\exposan\werf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BE8037-0118-4DE1-A01A-FA78D90372DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8DD14A-F1DA-4E71-A3EB-F4A3164FF222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1635" yWindow="3480" windowWidth="22440" windowHeight="13680" firstSheet="3" activeTab="18" xr2:uid="{218DD762-44D5-4240-B5CB-C558EBE30BA7}"/>
+    <workbookView xWindow="1635" yWindow="3480" windowWidth="22440" windowHeight="13680" firstSheet="3" activeTab="10" xr2:uid="{218DD762-44D5-4240-B5CB-C558EBE30BA7}"/>
   </bookViews>
   <sheets>
     <sheet name="B1" sheetId="6" r:id="rId1"/>
@@ -23,15 +23,13 @@
     <sheet name="G1" sheetId="12" r:id="rId8"/>
     <sheet name="G2" sheetId="13" r:id="rId9"/>
     <sheet name="G3" sheetId="14" r:id="rId10"/>
-    <sheet name="H1" sheetId="20" r:id="rId11"/>
-    <sheet name="H" sheetId="21" r:id="rId12"/>
-    <sheet name="H2" sheetId="22" r:id="rId13"/>
-    <sheet name="I1" sheetId="17" r:id="rId14"/>
-    <sheet name="I2" sheetId="16" r:id="rId15"/>
-    <sheet name="I3" sheetId="18" r:id="rId16"/>
-    <sheet name="N1" sheetId="19" r:id="rId17"/>
-    <sheet name="AED" sheetId="10" r:id="rId18"/>
-    <sheet name="adm" sheetId="2" r:id="rId19"/>
+    <sheet name="H1" sheetId="22" r:id="rId11"/>
+    <sheet name="I1" sheetId="17" r:id="rId12"/>
+    <sheet name="I2" sheetId="16" r:id="rId13"/>
+    <sheet name="I3" sheetId="18" r:id="rId14"/>
+    <sheet name="N1" sheetId="19" r:id="rId15"/>
+    <sheet name="AED" sheetId="10" r:id="rId16"/>
+    <sheet name="adm" sheetId="2" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="74">
   <si>
     <t>S_O2</t>
   </si>
@@ -276,12 +274,6 @@
   </si>
   <si>
     <t>H1</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>H2</t>
   </si>
 </sst>
 </file>
@@ -2043,1570 +2035,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E599D95C-4D24-432D-9B3F-CE35D4365C13}">
-  <dimension ref="A1:AE21"/>
-  <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="K1" sqref="A1:XFD7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="16" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" t="s">
-        <v>47</v>
-      </c>
-      <c r="V1" t="s">
-        <v>43</v>
-      </c>
-      <c r="W1" t="s">
-        <v>49</v>
-      </c>
-      <c r="X1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1.8439431519742401E-2</v>
-      </c>
-      <c r="C2">
-        <v>18.723737506934601</v>
-      </c>
-      <c r="D2">
-        <v>6.6756371259607201</v>
-      </c>
-      <c r="E2">
-        <v>6.4380458213734002</v>
-      </c>
-      <c r="F2">
-        <v>0.28600131743294999</v>
-      </c>
-      <c r="G2">
-        <v>1.7783089233109699</v>
-      </c>
-      <c r="H2">
-        <v>1.2634816253559</v>
-      </c>
-      <c r="I2">
-        <v>15.356765551024401</v>
-      </c>
-      <c r="J2">
-        <v>26.9908036812134</v>
-      </c>
-      <c r="K2">
-        <v>27.9926900722288</v>
-      </c>
-      <c r="L2">
-        <v>49.803936705613999</v>
-      </c>
-      <c r="M2">
-        <v>1354.1994346044</v>
-      </c>
-      <c r="N2">
-        <v>41.166547815641898</v>
-      </c>
-      <c r="O2">
-        <v>1300.6773842489499</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>100.19948525221599</v>
-      </c>
-      <c r="T2">
-        <v>137.61031943003499</v>
-      </c>
-      <c r="U2" s="1">
-        <v>1.77702558281408E-12</v>
-      </c>
-      <c r="V2">
-        <v>2.2679649572920302</v>
-      </c>
-      <c r="W2" s="1">
-        <v>5.3056682920207098E-10</v>
-      </c>
-      <c r="X2">
-        <v>160.005460866151</v>
-      </c>
-      <c r="Y2" s="1">
-        <v>1.7770244159545001E-12</v>
-      </c>
-      <c r="Z2" s="1">
-        <v>7.7095717931670901E-2</v>
-      </c>
-      <c r="AA2" s="1">
-        <v>194.98520885981699</v>
-      </c>
-      <c r="AB2" s="1">
-        <v>1.7771438058213599E-12</v>
-      </c>
-      <c r="AC2" s="1">
-        <v>1.7771442736184499E-12</v>
-      </c>
-      <c r="AD2">
-        <v>86.977286911151594</v>
-      </c>
-      <c r="AE2">
-        <v>424.88904525562202</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>3.8075616397918602E-4</v>
-      </c>
-      <c r="C3">
-        <v>19.528754560547899</v>
-      </c>
-      <c r="D3">
-        <v>6.6057586085602997</v>
-      </c>
-      <c r="E3">
-        <v>5.48305221219095</v>
-      </c>
-      <c r="F3">
-        <v>0.25016739170056101</v>
-      </c>
-      <c r="G3">
-        <v>0.46543293922505302</v>
-      </c>
-      <c r="H3">
-        <v>0.21726993546047799</v>
-      </c>
-      <c r="I3">
-        <v>15.3567655510509</v>
-      </c>
-      <c r="J3">
-        <v>27.0366890170768</v>
-      </c>
-      <c r="K3">
-        <v>27.992690072241</v>
-      </c>
-      <c r="L3">
-        <v>49.803936705615499</v>
-      </c>
-      <c r="M3">
-        <v>1354.4322388962401</v>
-      </c>
-      <c r="N3">
-        <v>38.310269176141503</v>
-      </c>
-      <c r="O3">
-        <v>1302.96191620382</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>100.156649897107</v>
-      </c>
-      <c r="T3">
-        <v>137.59218659244499</v>
-      </c>
-      <c r="U3" s="1">
-        <v>1.7776210743856199E-12</v>
-      </c>
-      <c r="V3">
-        <v>2.2679649568061802</v>
-      </c>
-      <c r="W3" s="1">
-        <v>5.3074456239632705E-10</v>
-      </c>
-      <c r="X3">
-        <v>160.05223978227701</v>
-      </c>
-      <c r="Y3" s="1">
-        <v>1.7776199064619701E-12</v>
-      </c>
-      <c r="Z3" s="1">
-        <v>7.7095724447903496E-2</v>
-      </c>
-      <c r="AA3" s="1">
-        <v>194.985208770323</v>
-      </c>
-      <c r="AB3" s="1">
-        <v>1.77773941315704E-12</v>
-      </c>
-      <c r="AC3" s="1">
-        <v>1.77773988124445E-12</v>
-      </c>
-      <c r="AD3">
-        <v>86.977286911151793</v>
-      </c>
-      <c r="AE3">
-        <v>424.88904525562299</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>16.668600222313501</v>
-      </c>
-      <c r="D4">
-        <v>1.5854130487354701</v>
-      </c>
-      <c r="E4">
-        <v>10.480474459936501</v>
-      </c>
-      <c r="F4">
-        <v>0.251251737675245</v>
-      </c>
-      <c r="G4">
-        <v>0.305324809125325</v>
-      </c>
-      <c r="H4">
-        <v>3.13923590586399E-2</v>
-      </c>
-      <c r="I4">
-        <v>15.356765551123299</v>
-      </c>
-      <c r="J4">
-        <v>12.9591883688393</v>
-      </c>
-      <c r="K4">
-        <v>27.992690072274399</v>
-      </c>
-      <c r="L4">
-        <v>49.803936705619797</v>
-      </c>
-      <c r="M4">
-        <v>1355.7592414092801</v>
-      </c>
-      <c r="N4">
-        <v>31.271493825556199</v>
-      </c>
-      <c r="O4">
-        <v>1302.11270448805</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>101.058305327372</v>
-      </c>
-      <c r="T4">
-        <v>137.535093818327</v>
-      </c>
-      <c r="U4" s="1">
-        <v>1.7792485091517999E-12</v>
-      </c>
-      <c r="V4">
-        <v>2.2679649553606298</v>
-      </c>
-      <c r="W4" s="1">
-        <v>5.3123029373300198E-10</v>
-      </c>
-      <c r="X4">
-        <v>160.199527039846</v>
-      </c>
-      <c r="Y4" s="1">
-        <v>1.77924733830179E-12</v>
-      </c>
-      <c r="Z4" s="1">
-        <v>7.7095742374841597E-2</v>
-      </c>
-      <c r="AA4" s="1">
-        <v>194.98520851546101</v>
-      </c>
-      <c r="AB4" s="1">
-        <v>1.7793671648680601E-12</v>
-      </c>
-      <c r="AC4" s="1">
-        <v>1.77936763376402E-12</v>
-      </c>
-      <c r="AD4">
-        <v>86.977286911152305</v>
-      </c>
-      <c r="AE4">
-        <v>424.889045255626</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>15.376869212144401</v>
-      </c>
-      <c r="D5">
-        <v>0.239744676148724</v>
-      </c>
-      <c r="E5">
-        <v>11.9598703415672</v>
-      </c>
-      <c r="F5">
-        <v>0.25805414171103203</v>
-      </c>
-      <c r="G5">
-        <v>0.29492429537944798</v>
-      </c>
-      <c r="H5">
-        <v>1.44159795532794E-2</v>
-      </c>
-      <c r="I5">
-        <v>15.356765551195799</v>
-      </c>
-      <c r="J5">
-        <v>6.7180709098917397</v>
-      </c>
-      <c r="K5">
-        <v>27.992690072307902</v>
-      </c>
-      <c r="L5">
-        <v>49.803936705623997</v>
-      </c>
-      <c r="M5">
-        <v>1357.08411916769</v>
-      </c>
-      <c r="N5">
-        <v>26.581517709341</v>
-      </c>
-      <c r="O5">
-        <v>1299.6059719480099</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>101.109509880801</v>
-      </c>
-      <c r="T5">
-        <v>137.411329572189</v>
-      </c>
-      <c r="U5" s="1">
-        <v>1.78087742911636E-12</v>
-      </c>
-      <c r="V5">
-        <v>2.2679649537979798</v>
-      </c>
-      <c r="W5" s="1">
-        <v>5.3171646791373995E-10</v>
-      </c>
-      <c r="X5">
-        <v>160.51881171589201</v>
-      </c>
-      <c r="Y5" s="1">
-        <v>1.7808762553586299E-12</v>
-      </c>
-      <c r="Z5" s="1">
-        <v>7.7095760434526706E-2</v>
-      </c>
-      <c r="AA5" s="1">
-        <v>194.98520825023101</v>
-      </c>
-      <c r="AB5" s="1">
-        <v>1.7809964026404701E-12</v>
-      </c>
-      <c r="AC5" s="1">
-        <v>1.7809968723181401E-12</v>
-      </c>
-      <c r="AD5">
-        <v>86.977286911152802</v>
-      </c>
-      <c r="AE5">
-        <v>424.88904525562901</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>4.7774057427950101E-2</v>
-      </c>
-      <c r="C6">
-        <v>16.3643357693864</v>
-      </c>
-      <c r="D6">
-        <v>0.24533883432495199</v>
-      </c>
-      <c r="E6">
-        <v>10.986524976619499</v>
-      </c>
-      <c r="F6">
-        <v>0.25544255504503399</v>
-      </c>
-      <c r="G6">
-        <v>0.229984174421</v>
-      </c>
-      <c r="H6">
-        <v>2.9961930874037299E-2</v>
-      </c>
-      <c r="I6">
-        <v>15.3567655512778</v>
-      </c>
-      <c r="J6">
-        <v>7.4962315048390398</v>
-      </c>
-      <c r="K6">
-        <v>27.992690072344001</v>
-      </c>
-      <c r="L6">
-        <v>49.8039367056289</v>
-      </c>
-      <c r="M6">
-        <v>1357.9984367331299</v>
-      </c>
-      <c r="N6">
-        <v>23.0579037266955</v>
-      </c>
-      <c r="O6">
-        <v>1298.0087326181099</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>100.989608083706</v>
-      </c>
-      <c r="T6">
-        <v>137.30705470602899</v>
-      </c>
-      <c r="U6" s="1">
-        <v>1.7827455752838901E-12</v>
-      </c>
-      <c r="V6">
-        <v>2.2679649518580201</v>
-      </c>
-      <c r="W6" s="1">
-        <v>5.3227404200787999E-10</v>
-      </c>
-      <c r="X6">
-        <v>160.78781826055899</v>
-      </c>
-      <c r="Y6" s="1">
-        <v>1.78274439824846E-12</v>
-      </c>
-      <c r="Z6" s="1">
-        <v>7.7095781296055196E-2</v>
-      </c>
-      <c r="AA6" s="1">
-        <v>194.985207933092</v>
-      </c>
-      <c r="AB6" s="1">
-        <v>1.78286491406444E-12</v>
-      </c>
-      <c r="AC6" s="1">
-        <v>1.7828653847340399E-12</v>
-      </c>
-      <c r="AD6">
-        <v>86.977286911153399</v>
-      </c>
-      <c r="AE6">
-        <v>424.88904525563203</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>15.8526742597712</v>
-      </c>
-      <c r="D7">
-        <v>0.11197738443265499</v>
-      </c>
-      <c r="E7">
-        <v>11.179783182443</v>
-      </c>
-      <c r="F7">
-        <v>0.26028081354823901</v>
-      </c>
-      <c r="G7">
-        <v>0.30525671056466902</v>
-      </c>
-      <c r="H7">
-        <v>2.0033928702624101E-2</v>
-      </c>
-      <c r="I7">
-        <v>15.3567655512985</v>
-      </c>
-      <c r="J7">
-        <v>6.0121197585416901</v>
-      </c>
-      <c r="K7">
-        <v>27.992690072353401</v>
-      </c>
-      <c r="L7">
-        <v>49.8039367056301</v>
-      </c>
-      <c r="M7">
-        <v>1358.3540270318599</v>
-      </c>
-      <c r="N7">
-        <v>22.391625250582901</v>
-      </c>
-      <c r="O7">
-        <v>1296.9202411124099</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>100.952881596895</v>
-      </c>
-      <c r="T7">
-        <v>137.267470224617</v>
-      </c>
-      <c r="U7" s="1">
-        <v>1.78318429111043E-12</v>
-      </c>
-      <c r="V7">
-        <v>2.2679649513942901</v>
-      </c>
-      <c r="W7" s="1">
-        <v>5.3240498278290203E-10</v>
-      </c>
-      <c r="X7">
-        <v>160.88993752245901</v>
-      </c>
-      <c r="Y7" s="1">
-        <v>1.7831831133063901E-12</v>
-      </c>
-      <c r="Z7" s="1">
-        <v>7.7095786203338804E-2</v>
-      </c>
-      <c r="AA7" s="1">
-        <v>194.98520785785601</v>
-      </c>
-      <c r="AB7" s="1">
-        <v>1.7833037157083101E-12</v>
-      </c>
-      <c r="AC7" s="1">
-        <v>1.78330418660685E-12</v>
-      </c>
-      <c r="AD7">
-        <v>86.977286911153598</v>
-      </c>
-      <c r="AE7">
-        <v>424.88904525563203</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="U10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
-      <c r="AC10" s="1"/>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="U11" s="1"/>
-      <c r="W11" s="1"/>
-      <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
-      <c r="AA11" s="1"/>
-      <c r="AB11" s="1"/>
-      <c r="AC11" s="1"/>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="U12" s="1"/>
-      <c r="W12" s="1"/>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
-      <c r="AA12" s="1"/>
-      <c r="AB12" s="1"/>
-      <c r="AC12" s="1"/>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="U13" s="1"/>
-      <c r="W13" s="1"/>
-      <c r="Y13" s="1"/>
-      <c r="Z13" s="1"/>
-      <c r="AA13" s="1"/>
-      <c r="AB13" s="1"/>
-      <c r="AC13" s="1"/>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="U14" s="1"/>
-      <c r="W14" s="1"/>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
-      <c r="AA14" s="1"/>
-      <c r="AB14" s="1"/>
-      <c r="AC14" s="1"/>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="U15" s="1"/>
-      <c r="W15" s="1"/>
-      <c r="Y15" s="1"/>
-      <c r="Z15" s="1"/>
-      <c r="AA15" s="1"/>
-      <c r="AB15" s="1"/>
-      <c r="AC15" s="1"/>
-    </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="U16" s="1"/>
-      <c r="W16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
-      <c r="AA16" s="1"/>
-      <c r="AB16" s="1"/>
-      <c r="AC16" s="1"/>
-    </row>
-    <row r="17" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="1"/>
-      <c r="AA17" s="1"/>
-      <c r="AB17" s="1"/>
-      <c r="AC17" s="1"/>
-    </row>
-    <row r="18" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="Y18" s="1"/>
-      <c r="Z18" s="1"/>
-      <c r="AA18" s="1"/>
-      <c r="AB18" s="1"/>
-      <c r="AC18" s="1"/>
-    </row>
-    <row r="19" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R19" s="1"/>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="1"/>
-      <c r="AA19" s="1"/>
-      <c r="AB19" s="1"/>
-      <c r="AC19" s="1"/>
-    </row>
-    <row r="20" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="Y20" s="1"/>
-      <c r="Z20" s="1"/>
-      <c r="AA20" s="1"/>
-      <c r="AB20" s="1"/>
-      <c r="AC20" s="1"/>
-    </row>
-    <row r="21" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="Y21" s="1"/>
-      <c r="Z21" s="1"/>
-      <c r="AA21" s="1"/>
-      <c r="AB21" s="1"/>
-      <c r="AC21" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FA85F62-9524-4DFD-AED1-1DC5BC35C55C}">
-  <dimension ref="A1:AE21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AF1" sqref="AF1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="16" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" t="s">
-        <v>47</v>
-      </c>
-      <c r="V1" t="s">
-        <v>43</v>
-      </c>
-      <c r="W1" t="s">
-        <v>49</v>
-      </c>
-      <c r="X1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2">
-        <v>0.02</v>
-      </c>
-      <c r="C2">
-        <v>18</v>
-      </c>
-      <c r="D2">
-        <v>7</v>
-      </c>
-      <c r="E2">
-        <v>6</v>
-      </c>
-      <c r="F2">
-        <v>0.3</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>16</v>
-      </c>
-      <c r="J2">
-        <v>30</v>
-      </c>
-      <c r="K2">
-        <v>28</v>
-      </c>
-      <c r="L2">
-        <v>50</v>
-      </c>
-      <c r="M2">
-        <v>1300</v>
-      </c>
-      <c r="N2">
-        <v>50</v>
-      </c>
-      <c r="O2">
-        <v>2000</v>
-      </c>
-      <c r="P2">
-        <v>10</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="R2">
-        <v>1</v>
-      </c>
-      <c r="S2">
-        <v>100</v>
-      </c>
-      <c r="T2">
-        <v>140</v>
-      </c>
-      <c r="U2" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="V2">
-        <v>2</v>
-      </c>
-      <c r="W2" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="X2">
-        <v>150</v>
-      </c>
-      <c r="Y2" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="Z2" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AA2">
-        <v>150</v>
-      </c>
-      <c r="AB2" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AC2" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AD2">
-        <v>87</v>
-      </c>
-      <c r="AE2">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3">
-        <v>1E-3</v>
-      </c>
-      <c r="C3">
-        <v>18</v>
-      </c>
-      <c r="D3">
-        <v>7</v>
-      </c>
-      <c r="E3">
-        <v>6</v>
-      </c>
-      <c r="F3">
-        <v>0.3</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>0.5</v>
-      </c>
-      <c r="I3">
-        <v>16</v>
-      </c>
-      <c r="J3">
-        <v>30</v>
-      </c>
-      <c r="K3">
-        <v>28</v>
-      </c>
-      <c r="L3">
-        <v>50</v>
-      </c>
-      <c r="M3">
-        <v>1300</v>
-      </c>
-      <c r="N3">
-        <v>40</v>
-      </c>
-      <c r="O3">
-        <v>2000</v>
-      </c>
-      <c r="P3">
-        <v>10</v>
-      </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
-      <c r="R3">
-        <v>1</v>
-      </c>
-      <c r="S3">
-        <v>100</v>
-      </c>
-      <c r="T3">
-        <v>140</v>
-      </c>
-      <c r="U3" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="V3">
-        <v>2</v>
-      </c>
-      <c r="W3" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="X3">
-        <v>150</v>
-      </c>
-      <c r="Y3" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="Z3" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AA3">
-        <v>150</v>
-      </c>
-      <c r="AB3" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AC3" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AD3">
-        <v>87</v>
-      </c>
-      <c r="AE3">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>18</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>7</v>
-      </c>
-      <c r="F4">
-        <v>0.3</v>
-      </c>
-      <c r="G4">
-        <v>0.5</v>
-      </c>
-      <c r="H4">
-        <v>0.1</v>
-      </c>
-      <c r="I4">
-        <v>16</v>
-      </c>
-      <c r="J4">
-        <v>15</v>
-      </c>
-      <c r="K4">
-        <v>28</v>
-      </c>
-      <c r="L4">
-        <v>50</v>
-      </c>
-      <c r="M4">
-        <v>1300</v>
-      </c>
-      <c r="N4">
-        <v>30</v>
-      </c>
-      <c r="O4">
-        <v>2000</v>
-      </c>
-      <c r="P4">
-        <v>10</v>
-      </c>
-      <c r="Q4">
-        <v>1</v>
-      </c>
-      <c r="R4">
-        <v>1</v>
-      </c>
-      <c r="S4">
-        <v>100</v>
-      </c>
-      <c r="T4">
-        <v>140</v>
-      </c>
-      <c r="U4" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="V4">
-        <v>2</v>
-      </c>
-      <c r="W4" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="X4">
-        <v>150</v>
-      </c>
-      <c r="Y4" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="Z4" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AA4">
-        <v>150</v>
-      </c>
-      <c r="AB4" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AC4" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AD4">
-        <v>87</v>
-      </c>
-      <c r="AE4">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>18</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>7</v>
-      </c>
-      <c r="F5">
-        <v>0.3</v>
-      </c>
-      <c r="G5">
-        <v>0.5</v>
-      </c>
-      <c r="H5">
-        <v>0.1</v>
-      </c>
-      <c r="I5">
-        <v>16</v>
-      </c>
-      <c r="J5">
-        <v>10</v>
-      </c>
-      <c r="K5">
-        <v>28</v>
-      </c>
-      <c r="L5">
-        <v>50</v>
-      </c>
-      <c r="M5">
-        <v>1300</v>
-      </c>
-      <c r="N5">
-        <v>25</v>
-      </c>
-      <c r="O5">
-        <v>2000</v>
-      </c>
-      <c r="P5">
-        <v>10</v>
-      </c>
-      <c r="Q5">
-        <v>1</v>
-      </c>
-      <c r="R5">
-        <v>1</v>
-      </c>
-      <c r="S5">
-        <v>100</v>
-      </c>
-      <c r="T5">
-        <v>140</v>
-      </c>
-      <c r="U5" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="V5">
-        <v>2</v>
-      </c>
-      <c r="W5" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="X5">
-        <v>150</v>
-      </c>
-      <c r="Y5" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="Z5" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AA5">
-        <v>150</v>
-      </c>
-      <c r="AB5" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AC5" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AD5">
-        <v>87</v>
-      </c>
-      <c r="AE5">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6">
-        <v>0.05</v>
-      </c>
-      <c r="C6">
-        <v>18</v>
-      </c>
-      <c r="D6">
-        <v>0.5</v>
-      </c>
-      <c r="E6">
-        <v>8</v>
-      </c>
-      <c r="F6">
-        <v>0.3</v>
-      </c>
-      <c r="G6">
-        <v>0.5</v>
-      </c>
-      <c r="H6">
-        <v>0.1</v>
-      </c>
-      <c r="I6">
-        <v>16</v>
-      </c>
-      <c r="J6">
-        <v>10</v>
-      </c>
-      <c r="K6">
-        <v>28</v>
-      </c>
-      <c r="L6">
-        <v>50</v>
-      </c>
-      <c r="M6">
-        <v>1300</v>
-      </c>
-      <c r="N6">
-        <v>25</v>
-      </c>
-      <c r="O6">
-        <v>2000</v>
-      </c>
-      <c r="P6">
-        <v>10</v>
-      </c>
-      <c r="Q6">
-        <v>1</v>
-      </c>
-      <c r="R6">
-        <v>1</v>
-      </c>
-      <c r="S6">
-        <v>100</v>
-      </c>
-      <c r="T6">
-        <v>140</v>
-      </c>
-      <c r="U6" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="V6">
-        <v>2</v>
-      </c>
-      <c r="W6" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="X6">
-        <v>150</v>
-      </c>
-      <c r="Y6" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="Z6" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AA6">
-        <v>150</v>
-      </c>
-      <c r="AB6" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AC6" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AD6">
-        <v>87</v>
-      </c>
-      <c r="AE6">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>18</v>
-      </c>
-      <c r="D7">
-        <v>0.5</v>
-      </c>
-      <c r="E7">
-        <v>8</v>
-      </c>
-      <c r="F7">
-        <v>0.3</v>
-      </c>
-      <c r="G7">
-        <v>0.5</v>
-      </c>
-      <c r="H7">
-        <v>0.1</v>
-      </c>
-      <c r="I7">
-        <v>16</v>
-      </c>
-      <c r="J7">
-        <v>10</v>
-      </c>
-      <c r="K7">
-        <v>28</v>
-      </c>
-      <c r="L7">
-        <v>50</v>
-      </c>
-      <c r="M7">
-        <v>1300</v>
-      </c>
-      <c r="N7">
-        <v>25</v>
-      </c>
-      <c r="O7">
-        <v>2000</v>
-      </c>
-      <c r="P7">
-        <v>10</v>
-      </c>
-      <c r="Q7">
-        <v>1</v>
-      </c>
-      <c r="R7">
-        <v>1</v>
-      </c>
-      <c r="S7">
-        <v>100</v>
-      </c>
-      <c r="T7">
-        <v>140</v>
-      </c>
-      <c r="U7" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="V7">
-        <v>2</v>
-      </c>
-      <c r="W7" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="X7">
-        <v>150</v>
-      </c>
-      <c r="Y7" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="Z7" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AA7">
-        <v>150</v>
-      </c>
-      <c r="AB7" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AC7" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AD7">
-        <v>87</v>
-      </c>
-      <c r="AE7">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="W10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
-      <c r="AC10" s="1"/>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="U11" s="1"/>
-      <c r="W11" s="1"/>
-      <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
-      <c r="AA11" s="1"/>
-      <c r="AB11" s="1"/>
-      <c r="AC11" s="1"/>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="U12" s="1"/>
-      <c r="W12" s="1"/>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
-      <c r="AA12" s="1"/>
-      <c r="AB12" s="1"/>
-      <c r="AC12" s="1"/>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="U13" s="1"/>
-      <c r="W13" s="1"/>
-      <c r="Y13" s="1"/>
-      <c r="Z13" s="1"/>
-      <c r="AA13" s="1"/>
-      <c r="AB13" s="1"/>
-      <c r="AC13" s="1"/>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="U14" s="1"/>
-      <c r="W14" s="1"/>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
-      <c r="AA14" s="1"/>
-      <c r="AB14" s="1"/>
-      <c r="AC14" s="1"/>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="U15" s="1"/>
-      <c r="W15" s="1"/>
-      <c r="Y15" s="1"/>
-      <c r="Z15" s="1"/>
-      <c r="AA15" s="1"/>
-      <c r="AB15" s="1"/>
-      <c r="AC15" s="1"/>
-    </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="U16" s="1"/>
-      <c r="W16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
-      <c r="AA16" s="1"/>
-      <c r="AB16" s="1"/>
-      <c r="AC16" s="1"/>
-    </row>
-    <row r="17" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="1"/>
-      <c r="AA17" s="1"/>
-      <c r="AB17" s="1"/>
-      <c r="AC17" s="1"/>
-    </row>
-    <row r="18" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="Y18" s="1"/>
-      <c r="Z18" s="1"/>
-      <c r="AA18" s="1"/>
-      <c r="AB18" s="1"/>
-      <c r="AC18" s="1"/>
-    </row>
-    <row r="19" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R19" s="1"/>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="1"/>
-      <c r="AA19" s="1"/>
-      <c r="AB19" s="1"/>
-      <c r="AC19" s="1"/>
-    </row>
-    <row r="20" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="Y20" s="1"/>
-      <c r="Z20" s="1"/>
-      <c r="AA20" s="1"/>
-      <c r="AB20" s="1"/>
-      <c r="AC20" s="1"/>
-    </row>
-    <row r="21" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="Y21" s="1"/>
-      <c r="Z21" s="1"/>
-      <c r="AA21" s="1"/>
-      <c r="AB21" s="1"/>
-      <c r="AC21" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED027A3C-A3AE-4576-A4DA-71233CC9AAA8}">
   <dimension ref="A1:AF21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4402,7 +2835,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D7FEF2-86A6-4650-A253-23D719FC805E}">
   <dimension ref="A1:AE21"/>
   <sheetViews>
@@ -5174,7 +3607,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E4487D-883D-4E85-B2E5-7356A39B3F61}">
   <dimension ref="A1:AE21"/>
   <sheetViews>
@@ -5898,7 +4331,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42016BA4-57DB-462D-9767-837B2F986A82}">
   <dimension ref="A1:AE7"/>
   <sheetViews>
@@ -6575,7 +5008,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12367F69-A662-4BD3-AE36-01641D10E752}">
   <dimension ref="A1:AE16"/>
   <sheetViews>
@@ -7313,7 +5746,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CB7F0C9-B54B-4F93-93CE-9E10B0EA4FF3}">
   <dimension ref="A1:AF7"/>
   <sheetViews>
@@ -8011,12 +6444,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{472A4E84-05F6-482F-94AF-2C8CE149BF8E}">
-  <dimension ref="A1:AU57"/>
+  <dimension ref="A1:AU55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AQ10" sqref="AQ10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8673,156 +7106,161 @@
     </row>
     <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B6">
+        <v>73</v>
+      </c>
+      <c r="B6" s="2">
         <v>10</v>
       </c>
       <c r="C6" s="2">
-        <v>4</v>
-      </c>
-      <c r="D6">
-        <v>75</v>
-      </c>
-      <c r="E6">
+        <v>4.5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>83</v>
+      </c>
+      <c r="E6" s="2">
         <v>9</v>
       </c>
-      <c r="F6">
-        <v>10</v>
-      </c>
-      <c r="G6">
+      <c r="F6" s="2">
         <v>12</v>
       </c>
-      <c r="H6">
-        <v>45</v>
-      </c>
-      <c r="I6">
-        <v>1E-4</v>
-      </c>
-      <c r="J6">
-        <v>100</v>
-      </c>
-      <c r="K6">
-        <v>900</v>
-      </c>
-      <c r="L6">
-        <v>1200</v>
-      </c>
-      <c r="M6">
+      <c r="G6" s="2">
+        <v>14</v>
+      </c>
+      <c r="H6" s="2">
+        <v>52</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <v>180</v>
+      </c>
+      <c r="K6" s="2">
+        <v>915</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1560</v>
+      </c>
+      <c r="M6" s="2">
         <v>200</v>
       </c>
-      <c r="N6">
-        <v>17.899999999999999</v>
-      </c>
-      <c r="O6">
-        <v>20</v>
-      </c>
-      <c r="P6">
-        <v>20</v>
-      </c>
-      <c r="Q6">
-        <v>25</v>
-      </c>
-      <c r="R6">
-        <v>350</v>
-      </c>
-      <c r="S6">
-        <v>270</v>
-      </c>
-      <c r="T6">
-        <v>250</v>
-      </c>
-      <c r="U6">
-        <v>120</v>
-      </c>
-      <c r="V6">
-        <v>60</v>
-      </c>
-      <c r="W6">
-        <v>400</v>
-      </c>
-      <c r="X6">
-        <v>200</v>
-      </c>
-      <c r="Y6">
-        <v>32000</v>
-      </c>
-      <c r="Z6" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AA6" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AB6" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AC6">
+      <c r="N6" s="2">
+        <v>16</v>
+      </c>
+      <c r="O6" s="2">
+        <v>46</v>
+      </c>
+      <c r="P6" s="2">
+        <v>49</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>65</v>
+      </c>
+      <c r="R6" s="2">
+        <v>830</v>
+      </c>
+      <c r="S6" s="2">
+        <v>660</v>
+      </c>
+      <c r="T6" s="2">
+        <v>630</v>
+      </c>
+      <c r="U6" s="2">
+        <v>280</v>
+      </c>
+      <c r="V6" s="2">
+        <v>130</v>
+      </c>
+      <c r="W6" s="2">
+        <v>870</v>
+      </c>
+      <c r="X6" s="2">
+        <v>420</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>23760</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="2">
         <v>28</v>
       </c>
-      <c r="AD6">
-        <v>0.3</v>
-      </c>
-      <c r="AE6">
+      <c r="AD6" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="AE6" s="2">
         <v>2</v>
       </c>
-      <c r="AF6" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AG6">
-        <v>500</v>
-      </c>
-      <c r="AH6">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="AI6">
-        <v>9000</v>
-      </c>
-      <c r="AJ6" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AK6" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AL6" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AM6" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AN6" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AO6">
+      <c r="AF6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="2">
+        <v>540</v>
+      </c>
+      <c r="AH6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="2">
+        <v>1700</v>
+      </c>
+      <c r="AJ6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="2">
+        <v>23</v>
+      </c>
+      <c r="AL6" s="2">
+        <v>3900</v>
+      </c>
+      <c r="AM6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AN6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AO6" s="2">
         <v>87</v>
       </c>
-      <c r="AP6">
+      <c r="AP6" s="2">
         <v>425</v>
       </c>
+      <c r="AQ6" s="2"/>
+      <c r="AR6" s="2"/>
+      <c r="AS6" s="2"/>
+      <c r="AT6" s="2"/>
+      <c r="AU6" s="2"/>
     </row>
     <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2">
-        <v>0.5</v>
+        <v>4</v>
       </c>
       <c r="D7">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H7">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="I7">
         <v>1E-4</v>
@@ -8831,82 +7269,82 @@
         <v>100</v>
       </c>
       <c r="K7">
-        <v>750</v>
+        <v>900</v>
       </c>
       <c r="L7">
-        <v>1500</v>
+        <v>1200</v>
       </c>
       <c r="M7">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="N7">
         <v>17.899999999999999</v>
       </c>
       <c r="O7">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="P7">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="Q7">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="R7">
-        <v>1000</v>
+        <v>350</v>
       </c>
       <c r="S7">
-        <v>1000</v>
+        <v>270</v>
       </c>
       <c r="T7">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="U7">
-        <v>650</v>
+        <v>120</v>
       </c>
       <c r="V7">
-        <v>350</v>
+        <v>60</v>
       </c>
       <c r="W7">
-        <v>850</v>
+        <v>400</v>
       </c>
       <c r="X7">
-        <v>600</v>
+        <v>200</v>
       </c>
       <c r="Y7">
         <v>32000</v>
       </c>
-      <c r="Z7">
-        <v>65</v>
-      </c>
-      <c r="AA7">
-        <v>0.01</v>
-      </c>
-      <c r="AB7">
-        <v>80</v>
+      <c r="Z7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>1E-8</v>
       </c>
       <c r="AC7">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="AD7">
         <v>0.3</v>
       </c>
       <c r="AE7">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="AF7" s="1">
-        <v>0.1</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="AG7">
-        <v>950</v>
+        <v>500</v>
       </c>
       <c r="AH7">
-        <v>0.02</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="AI7">
-        <v>200</v>
+        <v>9000</v>
       </c>
       <c r="AJ7" s="1">
-        <v>0.01</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="AK7" s="1">
         <v>1.0000000000000001E-5</v>
@@ -8929,28 +7367,28 @@
     </row>
     <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C8" s="2">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="D8">
-        <v>75</v>
+        <v>7</v>
       </c>
       <c r="E8">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H8">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="I8">
         <v>1E-4</v>
@@ -8959,82 +7397,82 @@
         <v>100</v>
       </c>
       <c r="K8">
-        <v>900</v>
+        <v>750</v>
       </c>
       <c r="L8">
-        <v>1200</v>
+        <v>1500</v>
       </c>
       <c r="M8">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="N8">
         <v>17.899999999999999</v>
       </c>
       <c r="O8">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="P8">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="Q8">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="R8">
+        <v>1000</v>
+      </c>
+      <c r="S8">
+        <v>1000</v>
+      </c>
+      <c r="T8">
+        <v>1000</v>
+      </c>
+      <c r="U8">
+        <v>650</v>
+      </c>
+      <c r="V8">
         <v>350</v>
       </c>
-      <c r="S8">
-        <v>270</v>
-      </c>
-      <c r="T8">
-        <v>250</v>
-      </c>
-      <c r="U8">
-        <v>120</v>
-      </c>
-      <c r="V8">
+      <c r="W8">
+        <v>850</v>
+      </c>
+      <c r="X8">
+        <v>600</v>
+      </c>
+      <c r="Y8">
+        <v>32000</v>
+      </c>
+      <c r="Z8">
+        <v>65</v>
+      </c>
+      <c r="AA8">
+        <v>0.01</v>
+      </c>
+      <c r="AB8">
+        <v>80</v>
+      </c>
+      <c r="AC8">
         <v>60</v>
-      </c>
-      <c r="W8">
-        <v>400</v>
-      </c>
-      <c r="X8">
-        <v>200</v>
-      </c>
-      <c r="Y8">
-        <v>13000</v>
-      </c>
-      <c r="Z8" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AA8" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AB8" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AC8">
-        <v>28</v>
       </c>
       <c r="AD8">
         <v>0.3</v>
       </c>
       <c r="AE8">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="AF8" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>0.1</v>
       </c>
       <c r="AG8">
-        <v>500</v>
+        <v>950</v>
       </c>
       <c r="AH8">
-        <v>3.0000000000000001E-3</v>
+        <v>0.02</v>
       </c>
       <c r="AI8">
-        <v>3000</v>
+        <v>200</v>
       </c>
       <c r="AJ8" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>0.01</v>
       </c>
       <c r="AK8" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9055,278 +7493,23 @@
         <v>425</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9">
-        <v>10.093</v>
-      </c>
-      <c r="C9" s="2">
-        <v>4.5190000000000001</v>
-      </c>
-      <c r="D9">
-        <v>82.86</v>
-      </c>
-      <c r="E9">
-        <v>9.0549999999999997</v>
-      </c>
-      <c r="F9">
-        <v>11.852</v>
-      </c>
-      <c r="G9">
-        <v>13.739000000000001</v>
-      </c>
-      <c r="H9">
-        <v>50.536000000000001</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>179.49299999999999</v>
-      </c>
-      <c r="K9">
-        <v>905.221</v>
-      </c>
-      <c r="L9">
-        <v>1483.5730000000001</v>
-      </c>
-      <c r="M9">
-        <v>173.75299999999999</v>
-      </c>
-      <c r="N9">
-        <v>15.356999999999999</v>
-      </c>
-      <c r="O9">
-        <v>44.575000000000003</v>
-      </c>
-      <c r="P9">
-        <v>47.235999999999997</v>
-      </c>
-      <c r="Q9">
-        <v>63.726999999999997</v>
-      </c>
-      <c r="R9">
-        <v>807.69799999999998</v>
-      </c>
-      <c r="S9">
-        <v>639.30499999999995</v>
-      </c>
-      <c r="T9">
-        <v>611.42899999999997</v>
-      </c>
-      <c r="U9">
-        <v>272.01900000000001</v>
-      </c>
-      <c r="V9">
-        <v>127.06</v>
-      </c>
-      <c r="W9">
-        <v>848.22500000000002</v>
-      </c>
-      <c r="X9" s="1">
-        <v>406.822</v>
-      </c>
-      <c r="Y9">
-        <v>23251.673999999999</v>
-      </c>
-      <c r="Z9">
-        <v>0</v>
-      </c>
-      <c r="AA9">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC9">
-        <v>27.992999999999999</v>
-      </c>
-      <c r="AD9">
-        <v>0.42299999999999999</v>
-      </c>
-      <c r="AE9">
-        <v>2.1869999999999998</v>
-      </c>
-      <c r="AF9">
-        <v>0</v>
-      </c>
-      <c r="AG9">
-        <v>543.9</v>
-      </c>
-      <c r="AH9" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI9">
-        <v>1699.57</v>
-      </c>
-      <c r="AJ9">
-        <v>0</v>
-      </c>
-      <c r="AK9">
-        <v>1.542</v>
-      </c>
-      <c r="AL9" s="1">
-        <v>3894.2739999999999</v>
-      </c>
-      <c r="AM9">
-        <v>0</v>
-      </c>
-      <c r="AN9">
-        <v>0</v>
-      </c>
-      <c r="AO9">
-        <v>86.978999999999999</v>
-      </c>
-      <c r="AP9">
-        <v>424.89800000000002</v>
-      </c>
-    </row>
     <row r="10" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>75</v>
-      </c>
-      <c r="B10" s="2">
-        <v>10</v>
-      </c>
-      <c r="C10" s="2">
-        <v>4.5</v>
-      </c>
-      <c r="D10" s="2">
-        <v>83</v>
-      </c>
-      <c r="E10" s="2">
-        <v>9</v>
-      </c>
-      <c r="F10" s="2">
-        <v>12</v>
-      </c>
-      <c r="G10" s="2">
-        <v>14</v>
-      </c>
-      <c r="H10" s="2">
-        <v>52</v>
-      </c>
-      <c r="I10" s="2">
-        <v>0</v>
-      </c>
-      <c r="J10" s="2">
-        <v>180</v>
-      </c>
-      <c r="K10" s="2">
-        <v>915</v>
-      </c>
-      <c r="L10" s="2">
-        <v>1560</v>
-      </c>
-      <c r="M10" s="2">
-        <v>200</v>
-      </c>
-      <c r="N10" s="2">
-        <v>16</v>
-      </c>
-      <c r="O10" s="2">
-        <v>46</v>
-      </c>
-      <c r="P10" s="2">
-        <v>49</v>
-      </c>
-      <c r="Q10" s="2">
-        <v>65</v>
-      </c>
-      <c r="R10" s="2">
-        <v>830</v>
-      </c>
-      <c r="S10" s="2">
-        <v>660</v>
-      </c>
-      <c r="T10" s="2">
-        <v>630</v>
-      </c>
-      <c r="U10" s="2">
-        <v>280</v>
-      </c>
-      <c r="V10" s="2">
-        <v>130</v>
-      </c>
-      <c r="W10" s="2">
-        <v>870</v>
-      </c>
-      <c r="X10" s="2">
-        <v>420</v>
-      </c>
-      <c r="Y10" s="2">
-        <v>23760</v>
-      </c>
-      <c r="Z10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="2">
-        <v>28</v>
-      </c>
-      <c r="AD10" s="2">
-        <v>0.35</v>
-      </c>
-      <c r="AE10" s="2">
-        <v>2</v>
-      </c>
-      <c r="AF10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG10" s="2">
-        <v>540</v>
-      </c>
-      <c r="AH10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AI10" s="2">
-        <v>1700</v>
-      </c>
-      <c r="AJ10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK10" s="2">
-        <v>23</v>
-      </c>
-      <c r="AL10" s="2">
-        <v>3900</v>
-      </c>
-      <c r="AM10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AN10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AO10" s="2">
-        <v>87</v>
-      </c>
-      <c r="AP10" s="2">
-        <v>425</v>
-      </c>
-      <c r="AQ10" s="2"/>
-      <c r="AR10" s="2"/>
-      <c r="AS10" s="2"/>
-      <c r="AT10" s="2"/>
-      <c r="AU10" s="2"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:47" x14ac:dyDescent="0.25">
@@ -9384,26 +7567,26 @@
       <c r="D33" s="1"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="1"/>
       <c r="D34" s="1"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D35" s="1"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="1"/>
       <c r="D36" s="1"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="1"/>
       <c r="D38" s="1"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D39" s="1"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="1"/>
       <c r="D40" s="1"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
@@ -9416,48 +7599,42 @@
       <c r="D43" s="1"/>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="1"/>
       <c r="D44" s="1"/>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D45" s="1"/>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="1"/>
       <c r="D46" s="1"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D47" s="1"/>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="1"/>
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="1"/>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D55" s="1"/>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D56" s="1"/>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D57" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
rBOD & NIT working checkpoint
</commit_message>
<xml_diff>
--- a/exposan/werf/data/initial_conditions.xlsx
+++ b/exposan/werf/data/initial_conditions.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joy_c\Dropbox\PhD\Research\QSD\codes_developing\EXPOsan\exposan\werf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8DD14A-F1DA-4E71-A3EB-F4A3164FF222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB363F08-A252-414E-9397-D48A25273A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1635" yWindow="3480" windowWidth="22440" windowHeight="13680" firstSheet="3" activeTab="10" xr2:uid="{218DD762-44D5-4240-B5CB-C558EBE30BA7}"/>
+    <workbookView xWindow="-105" yWindow="10440" windowWidth="26010" windowHeight="10545" activeTab="7" xr2:uid="{218DD762-44D5-4240-B5CB-C558EBE30BA7}"/>
   </bookViews>
   <sheets>
     <sheet name="B1" sheetId="6" r:id="rId1"/>
     <sheet name="B2" sheetId="7" r:id="rId2"/>
     <sheet name="B3" sheetId="4" r:id="rId3"/>
-    <sheet name="C2" sheetId="8" r:id="rId4"/>
-    <sheet name="C3" sheetId="9" r:id="rId5"/>
+    <sheet name="C1" sheetId="23" r:id="rId4"/>
+    <sheet name="C2" sheetId="8" r:id="rId5"/>
     <sheet name="E2" sheetId="15" r:id="rId6"/>
     <sheet name="E2P" sheetId="11" r:id="rId7"/>
     <sheet name="G1" sheetId="12" r:id="rId8"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="75">
   <si>
     <t>S_O2</t>
   </si>
@@ -275,6 +275,9 @@
   <si>
     <t>H1</t>
   </si>
+  <si>
+    <t>F1</t>
+  </si>
 </sst>
 </file>
 
@@ -315,10 +318,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,7 +658,7 @@
   <dimension ref="A1:AE7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,7 +772,7 @@
         <v>12</v>
       </c>
       <c r="F2">
-        <v>0.5</v>
+        <v>7</v>
       </c>
       <c r="G2">
         <v>5</v>
@@ -817,14 +819,14 @@
       <c r="U2" s="1">
         <v>1E-8</v>
       </c>
-      <c r="V2">
-        <v>1.5</v>
+      <c r="V2" s="1">
+        <v>1E-8</v>
       </c>
       <c r="W2" s="1">
         <v>1E-8</v>
       </c>
-      <c r="X2">
-        <v>500</v>
+      <c r="X2" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y2" s="1">
         <v>1E-8</v>
@@ -865,7 +867,7 @@
         <v>14</v>
       </c>
       <c r="F3">
-        <v>0.3</v>
+        <v>6</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -912,14 +914,14 @@
       <c r="U3" s="1">
         <v>1E-8</v>
       </c>
-      <c r="V3">
-        <v>1.5</v>
+      <c r="V3" s="1">
+        <v>1E-8</v>
       </c>
       <c r="W3" s="1">
         <v>1E-8</v>
       </c>
-      <c r="X3">
-        <v>500</v>
+      <c r="X3" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y3" s="1">
         <v>1E-8</v>
@@ -960,7 +962,7 @@
         <v>16</v>
       </c>
       <c r="F4">
-        <v>0.25</v>
+        <v>5.5</v>
       </c>
       <c r="G4">
         <v>0.6</v>
@@ -1007,14 +1009,14 @@
       <c r="U4" s="1">
         <v>1E-8</v>
       </c>
-      <c r="V4">
-        <v>1.5</v>
+      <c r="V4" s="1">
+        <v>1E-8</v>
       </c>
       <c r="W4" s="1">
         <v>1E-8</v>
       </c>
-      <c r="X4">
-        <v>500</v>
+      <c r="X4" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y4" s="1">
         <v>1E-8</v>
@@ -1055,7 +1057,7 @@
         <v>18</v>
       </c>
       <c r="F5">
-        <v>0.21</v>
+        <v>5.5</v>
       </c>
       <c r="G5">
         <v>0.6</v>
@@ -1102,14 +1104,14 @@
       <c r="U5" s="1">
         <v>1E-8</v>
       </c>
-      <c r="V5">
-        <v>1.5</v>
+      <c r="V5" s="1">
+        <v>1E-8</v>
       </c>
       <c r="W5" s="1">
         <v>1E-8</v>
       </c>
-      <c r="X5">
-        <v>500</v>
+      <c r="X5" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y5" s="1">
         <v>1E-8</v>
@@ -1150,7 +1152,7 @@
         <v>20</v>
       </c>
       <c r="F6">
-        <v>0.19</v>
+        <v>5.5</v>
       </c>
       <c r="G6">
         <v>0.5</v>
@@ -1197,14 +1199,14 @@
       <c r="U6" s="1">
         <v>1E-8</v>
       </c>
-      <c r="V6">
-        <v>1.5</v>
+      <c r="V6" s="1">
+        <v>1E-8</v>
       </c>
       <c r="W6" s="1">
         <v>1E-8</v>
       </c>
-      <c r="X6">
-        <v>500</v>
+      <c r="X6" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y6" s="1">
         <v>1E-8</v>
@@ -1245,7 +1247,7 @@
         <v>22</v>
       </c>
       <c r="F7">
-        <v>0.18</v>
+        <v>5</v>
       </c>
       <c r="G7">
         <v>0.5</v>
@@ -1292,14 +1294,14 @@
       <c r="U7" s="1">
         <v>1E-8</v>
       </c>
-      <c r="V7">
-        <v>1.5</v>
+      <c r="V7" s="1">
+        <v>1E-8</v>
       </c>
       <c r="W7" s="1">
         <v>1E-8</v>
       </c>
-      <c r="X7">
-        <v>500</v>
+      <c r="X7" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y7" s="1">
         <v>1E-8</v>
@@ -2038,7 +2040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED027A3C-A3AE-4576-A4DA-71233CC9AAA8}">
   <dimension ref="A1:AF21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -2222,7 +2224,7 @@
       <c r="Z2" s="1">
         <v>0</v>
       </c>
-      <c r="AA2" s="2">
+      <c r="AA2">
         <v>195</v>
       </c>
       <c r="AB2" s="1">
@@ -2320,7 +2322,7 @@
       <c r="Z3" s="1">
         <v>0</v>
       </c>
-      <c r="AA3" s="2">
+      <c r="AA3">
         <v>195</v>
       </c>
       <c r="AB3" s="1">
@@ -2418,7 +2420,7 @@
       <c r="Z4" s="1">
         <v>0</v>
       </c>
-      <c r="AA4" s="2">
+      <c r="AA4">
         <v>195</v>
       </c>
       <c r="AB4" s="1">
@@ -2516,7 +2518,7 @@
       <c r="Z5" s="1">
         <v>0</v>
       </c>
-      <c r="AA5" s="2">
+      <c r="AA5">
         <v>195</v>
       </c>
       <c r="AB5" s="1">
@@ -2614,7 +2616,7 @@
       <c r="Z6" s="1">
         <v>0</v>
       </c>
-      <c r="AA6" s="2">
+      <c r="AA6">
         <v>195</v>
       </c>
       <c r="AB6" s="1">
@@ -2712,7 +2714,7 @@
       <c r="Z7" s="1">
         <v>0</v>
       </c>
-      <c r="AA7" s="2">
+      <c r="AA7">
         <v>195</v>
       </c>
       <c r="AB7" s="1">
@@ -6446,16 +6448,16 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{472A4E84-05F6-482F-94AF-2C8CE149BF8E}">
-  <dimension ref="A1:AU55"/>
+  <dimension ref="A1:AP56"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="24" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="10" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9.42578125" bestFit="1" customWidth="1"/>
@@ -6467,11 +6469,11 @@
     <col min="47" max="47" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>22</v>
       </c>
       <c r="D1" t="s">
@@ -6592,14 +6594,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
       <c r="B2">
         <v>12</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>5.3</v>
       </c>
       <c r="D2">
@@ -6720,14 +6722,14 @@
         <v>425</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>53</v>
       </c>
       <c r="B3">
         <v>12.71</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>5.6840000000000002</v>
       </c>
       <c r="D3">
@@ -6848,81 +6850,81 @@
         <v>425</v>
       </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
       <c r="B4">
-        <v>11.0383310595415</v>
-      </c>
-      <c r="C4" s="2">
-        <v>4.9395274502546904</v>
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
       </c>
       <c r="D4">
-        <v>92.600672629228598</v>
+        <v>101</v>
       </c>
       <c r="E4">
-        <v>9.8902367700285794</v>
+        <v>11</v>
       </c>
       <c r="F4">
-        <v>13.063916576479</v>
+        <v>14</v>
       </c>
       <c r="G4">
-        <v>15.279661618496201</v>
+        <v>17</v>
       </c>
       <c r="H4">
-        <v>76.440422875413205</v>
-      </c>
-      <c r="I4" s="1">
-        <v>2.22851976459277E-4</v>
+        <v>77</v>
+      </c>
+      <c r="I4">
+        <v>2.5580697591124903E-4</v>
       </c>
       <c r="J4">
-        <v>162.55311039355601</v>
+        <v>146</v>
       </c>
       <c r="K4">
-        <v>1010.2930974631701</v>
+        <v>983</v>
       </c>
       <c r="L4">
-        <v>2342.3906115907798</v>
+        <v>2066</v>
       </c>
       <c r="M4">
-        <v>488.00211806324501</v>
+        <v>435</v>
       </c>
       <c r="N4">
-        <v>17.9000000003083</v>
+        <v>18</v>
       </c>
       <c r="O4">
-        <v>43.133109867889303</v>
+        <v>1247</v>
       </c>
       <c r="P4">
-        <v>43.249105180293</v>
+        <v>1250</v>
       </c>
       <c r="Q4">
-        <v>55.201534626928499</v>
+        <v>1596</v>
       </c>
       <c r="R4">
-        <v>708.81639098357402</v>
+        <v>577</v>
       </c>
       <c r="S4">
-        <v>534.73394174362602</v>
+        <v>435</v>
       </c>
       <c r="T4">
-        <v>482.74753397462501</v>
+        <v>392</v>
       </c>
       <c r="U4">
-        <v>229.59957076101799</v>
+        <v>187</v>
       </c>
       <c r="V4">
-        <v>109.351380313028</v>
+        <v>89</v>
       </c>
       <c r="W4">
-        <v>702.08414576896905</v>
+        <v>570</v>
       </c>
       <c r="X4">
-        <v>337.90144596460198</v>
+        <v>274</v>
       </c>
       <c r="Y4">
-        <v>26012.215298871801</v>
+        <v>23786</v>
       </c>
       <c r="Z4">
         <v>0</v>
@@ -6934,25 +6936,25 @@
         <v>0</v>
       </c>
       <c r="AC4">
-        <v>28.000000000042</v>
+        <v>28</v>
       </c>
       <c r="AD4" s="1">
-        <v>9.6161849823588205E-2</v>
+        <v>0</v>
       </c>
       <c r="AE4">
-        <v>1.08883030146177</v>
+        <v>1</v>
       </c>
       <c r="AF4">
         <v>0</v>
       </c>
       <c r="AG4">
-        <v>546.51222804644499</v>
+        <v>546</v>
       </c>
       <c r="AH4" s="1">
-        <v>4.3387232579569502E-12</v>
+        <v>0</v>
       </c>
       <c r="AI4">
-        <v>7539.5268325717298</v>
+        <v>388</v>
       </c>
       <c r="AJ4">
         <v>0</v>
@@ -6967,120 +6969,120 @@
         <v>0</v>
       </c>
       <c r="AN4" s="1">
-        <v>6.5093450479321201E-6</v>
+        <v>0</v>
       </c>
       <c r="AO4">
-        <v>87.000000000168001</v>
+        <v>87</v>
       </c>
       <c r="AP4">
-        <v>424.99999999083798</v>
-      </c>
-    </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>110</v>
+      </c>
+      <c r="E5">
+        <v>11</v>
+      </c>
+      <c r="F5">
+        <v>15</v>
+      </c>
+      <c r="G5">
+        <v>18</v>
+      </c>
+      <c r="H5">
         <v>63</v>
       </c>
-      <c r="B5">
-        <v>14</v>
-      </c>
-      <c r="C5" s="2">
-        <v>6.2</v>
-      </c>
-      <c r="D5">
-        <v>126</v>
-      </c>
-      <c r="E5">
-        <v>12.9</v>
-      </c>
-      <c r="F5">
-        <v>16.8</v>
-      </c>
-      <c r="G5">
-        <v>20.400000000000002</v>
-      </c>
-      <c r="H5">
-        <v>58.8</v>
-      </c>
       <c r="I5">
-        <v>0.01</v>
+        <v>2.5580697591124903E-4</v>
       </c>
       <c r="J5">
-        <v>54.4</v>
+        <v>191</v>
       </c>
       <c r="K5">
-        <v>1068</v>
+        <v>881</v>
       </c>
       <c r="L5">
-        <v>928.19999999999993</v>
+        <v>1263</v>
       </c>
       <c r="M5">
-        <v>868</v>
+        <v>149</v>
       </c>
       <c r="N5">
-        <v>26.3</v>
+        <v>17</v>
       </c>
       <c r="O5">
-        <v>1302</v>
+        <v>1626</v>
       </c>
       <c r="P5">
-        <v>1361.3</v>
+        <v>1723</v>
       </c>
       <c r="Q5">
-        <v>1812.7</v>
+        <v>2325</v>
       </c>
       <c r="R5">
-        <v>514.59999999999991</v>
+        <v>708</v>
       </c>
       <c r="S5">
-        <v>401.7</v>
+        <v>561</v>
       </c>
       <c r="T5">
-        <v>374.90000000000003</v>
+        <v>535</v>
       </c>
       <c r="U5">
-        <v>159.6</v>
+        <v>238</v>
       </c>
       <c r="V5">
-        <v>89.6</v>
+        <v>111</v>
       </c>
       <c r="W5">
-        <v>500.6</v>
+        <v>742</v>
       </c>
       <c r="X5">
-        <v>258</v>
+        <v>356</v>
       </c>
       <c r="Y5">
-        <v>12923.199999999999</v>
+        <v>20123</v>
       </c>
       <c r="Z5">
-        <v>669.69999999999993</v>
+        <v>0</v>
       </c>
       <c r="AA5">
         <v>0</v>
       </c>
       <c r="AB5">
-        <v>915.4</v>
+        <v>0</v>
       </c>
       <c r="AC5">
-        <v>12.9</v>
-      </c>
-      <c r="AD5">
-        <v>0.1</v>
+        <v>27</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>0</v>
       </c>
       <c r="AE5">
-        <v>0.2</v>
+        <v>2</v>
       </c>
       <c r="AF5">
         <v>0</v>
       </c>
       <c r="AG5">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="AH5">
+        <v>542</v>
+      </c>
+      <c r="AH5" s="1">
         <v>0</v>
       </c>
       <c r="AI5">
-        <v>0.9</v>
+        <v>385</v>
       </c>
       <c r="AJ5">
         <v>0</v>
@@ -7094,269 +7096,264 @@
       <c r="AM5">
         <v>0</v>
       </c>
-      <c r="AN5">
+      <c r="AN5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO5">
+        <v>86</v>
+      </c>
+      <c r="AP5">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>6.2</v>
+      </c>
+      <c r="D6">
+        <v>126</v>
+      </c>
+      <c r="E6">
+        <v>12.9</v>
+      </c>
+      <c r="F6">
+        <v>16.8</v>
+      </c>
+      <c r="G6">
+        <v>20.400000000000002</v>
+      </c>
+      <c r="H6">
+        <v>58.8</v>
+      </c>
+      <c r="I6">
+        <v>0.01</v>
+      </c>
+      <c r="J6">
+        <v>54.4</v>
+      </c>
+      <c r="K6">
+        <v>1068</v>
+      </c>
+      <c r="L6">
+        <v>928.19999999999993</v>
+      </c>
+      <c r="M6">
+        <v>868</v>
+      </c>
+      <c r="N6">
+        <v>26.3</v>
+      </c>
+      <c r="O6">
+        <v>1302</v>
+      </c>
+      <c r="P6">
+        <v>1361.3</v>
+      </c>
+      <c r="Q6">
+        <v>1812.7</v>
+      </c>
+      <c r="R6">
+        <v>514.59999999999991</v>
+      </c>
+      <c r="S6">
+        <v>401.7</v>
+      </c>
+      <c r="T6">
+        <v>374.90000000000003</v>
+      </c>
+      <c r="U6">
+        <v>159.6</v>
+      </c>
+      <c r="V6">
+        <v>89.6</v>
+      </c>
+      <c r="W6">
+        <v>500.6</v>
+      </c>
+      <c r="X6">
+        <v>258</v>
+      </c>
+      <c r="Y6">
+        <v>12923.199999999999</v>
+      </c>
+      <c r="Z6">
+        <v>669.69999999999993</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>915.4</v>
+      </c>
+      <c r="AC6">
+        <v>12.9</v>
+      </c>
+      <c r="AD6">
+        <v>0.1</v>
+      </c>
+      <c r="AE6">
+        <v>0.2</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="AH6">
+        <v>0</v>
+      </c>
+      <c r="AI6">
+        <v>0.9</v>
+      </c>
+      <c r="AJ6">
+        <v>0</v>
+      </c>
+      <c r="AK6">
+        <v>0</v>
+      </c>
+      <c r="AL6">
+        <v>0</v>
+      </c>
+      <c r="AM6">
+        <v>0</v>
+      </c>
+      <c r="AN6">
         <v>1</v>
       </c>
-      <c r="AO5">
+      <c r="AO6">
         <v>61</v>
       </c>
-      <c r="AP5">
+      <c r="AP6">
         <v>12.6</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>73</v>
-      </c>
-      <c r="B6" s="2">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2">
-        <v>4.5</v>
-      </c>
-      <c r="D6" s="2">
-        <v>83</v>
-      </c>
-      <c r="E6" s="2">
-        <v>9</v>
-      </c>
-      <c r="F6" s="2">
-        <v>12</v>
-      </c>
-      <c r="G6" s="2">
-        <v>14</v>
-      </c>
-      <c r="H6" s="2">
-        <v>52</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0</v>
-      </c>
-      <c r="J6" s="2">
-        <v>180</v>
-      </c>
-      <c r="K6" s="2">
-        <v>915</v>
-      </c>
-      <c r="L6" s="2">
-        <v>1560</v>
-      </c>
-      <c r="M6" s="2">
-        <v>200</v>
-      </c>
-      <c r="N6" s="2">
-        <v>16</v>
-      </c>
-      <c r="O6" s="2">
-        <v>46</v>
-      </c>
-      <c r="P6" s="2">
-        <v>49</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>65</v>
-      </c>
-      <c r="R6" s="2">
-        <v>830</v>
-      </c>
-      <c r="S6" s="2">
-        <v>660</v>
-      </c>
-      <c r="T6" s="2">
-        <v>630</v>
-      </c>
-      <c r="U6" s="2">
-        <v>280</v>
-      </c>
-      <c r="V6" s="2">
-        <v>130</v>
-      </c>
-      <c r="W6" s="2">
-        <v>870</v>
-      </c>
-      <c r="X6" s="2">
-        <v>420</v>
-      </c>
-      <c r="Y6" s="2">
-        <v>23760</v>
-      </c>
-      <c r="Z6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="2">
-        <v>28</v>
-      </c>
-      <c r="AD6" s="2">
-        <v>0.35</v>
-      </c>
-      <c r="AE6" s="2">
-        <v>2</v>
-      </c>
-      <c r="AF6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG6" s="2">
-        <v>540</v>
-      </c>
-      <c r="AH6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AI6" s="2">
-        <v>1700</v>
-      </c>
-      <c r="AJ6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK6" s="2">
-        <v>23</v>
-      </c>
-      <c r="AL6" s="2">
-        <v>3900</v>
-      </c>
-      <c r="AM6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AN6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AO6" s="2">
-        <v>87</v>
-      </c>
-      <c r="AP6" s="2">
-        <v>425</v>
-      </c>
-      <c r="AQ6" s="2"/>
-      <c r="AR6" s="2"/>
-      <c r="AS6" s="2"/>
-      <c r="AT6" s="2"/>
-      <c r="AU6" s="2"/>
-    </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>71</v>
       </c>
       <c r="B7">
         <v>10</v>
       </c>
-      <c r="C7" s="2">
-        <v>4</v>
+      <c r="C7">
+        <v>4.5</v>
       </c>
       <c r="D7">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="E7">
         <v>9</v>
       </c>
       <c r="F7">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G7">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H7">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="I7">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="J7">
-        <v>100</v>
+        <v>180</v>
       </c>
       <c r="K7">
-        <v>900</v>
+        <v>915</v>
       </c>
       <c r="L7">
-        <v>1200</v>
+        <v>1560</v>
       </c>
       <c r="M7">
         <v>200</v>
       </c>
       <c r="N7">
-        <v>17.899999999999999</v>
+        <v>16</v>
       </c>
       <c r="O7">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="P7">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="Q7">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="R7">
-        <v>350</v>
+        <v>830</v>
       </c>
       <c r="S7">
-        <v>270</v>
+        <v>660</v>
       </c>
       <c r="T7">
-        <v>250</v>
+        <v>630</v>
       </c>
       <c r="U7">
-        <v>120</v>
+        <v>280</v>
       </c>
       <c r="V7">
-        <v>60</v>
+        <v>130</v>
       </c>
       <c r="W7">
-        <v>400</v>
+        <v>870</v>
       </c>
       <c r="X7">
-        <v>200</v>
+        <v>420</v>
       </c>
       <c r="Y7">
-        <v>32000</v>
-      </c>
-      <c r="Z7" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AA7" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AB7" s="1">
-        <v>1E-8</v>
+        <v>23760</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
       </c>
       <c r="AC7">
         <v>28</v>
       </c>
       <c r="AD7">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="AE7">
         <v>2</v>
       </c>
-      <c r="AF7" s="1">
-        <v>1.0000000000000001E-5</v>
+      <c r="AF7">
+        <v>0</v>
       </c>
       <c r="AG7">
-        <v>500</v>
+        <v>540</v>
       </c>
       <c r="AH7">
-        <v>3.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="AI7">
-        <v>9000</v>
-      </c>
-      <c r="AJ7" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AK7" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AL7" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AM7" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AN7" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>1700</v>
+      </c>
+      <c r="AJ7">
+        <v>0</v>
+      </c>
+      <c r="AK7">
+        <v>23</v>
+      </c>
+      <c r="AL7">
+        <v>3900</v>
+      </c>
+      <c r="AM7">
+        <v>0</v>
+      </c>
+      <c r="AN7">
+        <v>0</v>
       </c>
       <c r="AO7">
         <v>87</v>
@@ -7365,30 +7362,30 @@
         <v>425</v>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0.5</v>
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
       </c>
       <c r="D8">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H8">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="I8">
         <v>1E-4</v>
@@ -7397,82 +7394,82 @@
         <v>100</v>
       </c>
       <c r="K8">
-        <v>750</v>
+        <v>900</v>
       </c>
       <c r="L8">
-        <v>1500</v>
+        <v>1200</v>
       </c>
       <c r="M8">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="N8">
         <v>17.899999999999999</v>
       </c>
       <c r="O8">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="P8">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="Q8">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="R8">
-        <v>1000</v>
+        <v>350</v>
       </c>
       <c r="S8">
-        <v>1000</v>
+        <v>270</v>
       </c>
       <c r="T8">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="U8">
-        <v>650</v>
+        <v>120</v>
       </c>
       <c r="V8">
-        <v>350</v>
+        <v>60</v>
       </c>
       <c r="W8">
-        <v>850</v>
+        <v>400</v>
       </c>
       <c r="X8">
-        <v>600</v>
+        <v>200</v>
       </c>
       <c r="Y8">
         <v>32000</v>
       </c>
-      <c r="Z8">
-        <v>65</v>
-      </c>
-      <c r="AA8">
-        <v>0.01</v>
-      </c>
-      <c r="AB8">
-        <v>80</v>
+      <c r="Z8" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA8" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>1E-8</v>
       </c>
       <c r="AC8">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="AD8">
         <v>0.3</v>
       </c>
       <c r="AE8">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="AF8" s="1">
-        <v>0.1</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="AG8">
-        <v>950</v>
+        <v>500</v>
       </c>
       <c r="AH8">
-        <v>0.02</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="AI8">
-        <v>200</v>
+        <v>9000</v>
       </c>
       <c r="AJ8" s="1">
-        <v>0.01</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="AK8" s="1">
         <v>1.0000000000000001E-5</v>
@@ -7493,26 +7490,148 @@
         <v>425</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0.5</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>7</v>
+      </c>
+      <c r="I9">
+        <v>1E-4</v>
+      </c>
+      <c r="J9">
+        <v>100</v>
+      </c>
+      <c r="K9">
+        <v>750</v>
+      </c>
+      <c r="L9">
+        <v>1500</v>
+      </c>
+      <c r="M9">
+        <v>250</v>
+      </c>
+      <c r="N9">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="O9">
+        <v>10</v>
+      </c>
+      <c r="P9">
+        <v>10</v>
+      </c>
+      <c r="Q9">
+        <v>10</v>
+      </c>
+      <c r="R9">
+        <v>1000</v>
+      </c>
+      <c r="S9">
+        <v>1000</v>
+      </c>
+      <c r="T9">
+        <v>1000</v>
+      </c>
+      <c r="U9">
+        <v>650</v>
+      </c>
+      <c r="V9">
+        <v>350</v>
+      </c>
+      <c r="W9">
+        <v>850</v>
+      </c>
+      <c r="X9">
+        <v>600</v>
+      </c>
+      <c r="Y9">
+        <v>32000</v>
+      </c>
+      <c r="Z9">
+        <v>65</v>
+      </c>
+      <c r="AA9">
+        <v>0.01</v>
+      </c>
+      <c r="AB9">
+        <v>80</v>
+      </c>
+      <c r="AC9">
+        <v>60</v>
+      </c>
+      <c r="AD9">
+        <v>0.3</v>
+      </c>
+      <c r="AE9">
+        <v>50</v>
+      </c>
+      <c r="AF9" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="AG9">
+        <v>950</v>
+      </c>
+      <c r="AH9">
+        <v>0.02</v>
+      </c>
+      <c r="AI9">
+        <v>200</v>
+      </c>
+      <c r="AJ9" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="AK9" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AL9" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AM9" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AN9" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AO9">
+        <v>87</v>
+      </c>
+      <c r="AP9">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.25">
@@ -7567,10 +7686,10 @@
       <c r="D33" s="1"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="1"/>
       <c r="D34" s="1"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="1"/>
       <c r="D35" s="1"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
@@ -7580,10 +7699,10 @@
       <c r="D37" s="1"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="1"/>
       <c r="D38" s="1"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="1"/>
       <c r="D39" s="1"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
@@ -7599,10 +7718,10 @@
       <c r="D43" s="1"/>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="1"/>
       <c r="D44" s="1"/>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="1"/>
       <c r="D45" s="1"/>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
@@ -7612,29 +7731,32 @@
       <c r="D47" s="1"/>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="1"/>
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="1"/>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D55" s="1"/>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7646,7 +7768,7 @@
   <dimension ref="A1:AE7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7763,7 +7885,7 @@
         <v>8</v>
       </c>
       <c r="F2">
-        <v>0.45</v>
+        <v>5</v>
       </c>
       <c r="G2">
         <v>5</v>
@@ -7810,14 +7932,14 @@
       <c r="U2" s="1">
         <v>1E-8</v>
       </c>
-      <c r="V2">
-        <v>0.05</v>
-      </c>
-      <c r="W2">
-        <v>1</v>
-      </c>
-      <c r="X2">
-        <v>500</v>
+      <c r="V2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="W2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X2" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y2" s="1">
         <v>1E-8</v>
@@ -7858,7 +7980,7 @@
         <v>10</v>
       </c>
       <c r="F3">
-        <v>0.3</v>
+        <v>5</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -7905,14 +8027,14 @@
       <c r="U3" s="1">
         <v>1E-8</v>
       </c>
-      <c r="V3">
-        <v>0.05</v>
-      </c>
-      <c r="W3">
-        <v>1</v>
-      </c>
-      <c r="X3">
-        <v>500</v>
+      <c r="V3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="W3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X3" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y3" s="1">
         <v>1E-8</v>
@@ -7953,7 +8075,7 @@
         <v>11</v>
       </c>
       <c r="F4">
-        <v>0.25</v>
+        <v>5</v>
       </c>
       <c r="G4">
         <v>0.6</v>
@@ -8000,14 +8122,14 @@
       <c r="U4" s="1">
         <v>1E-8</v>
       </c>
-      <c r="V4">
-        <v>0.05</v>
-      </c>
-      <c r="W4">
-        <v>1</v>
-      </c>
-      <c r="X4">
-        <v>500</v>
+      <c r="V4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="W4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X4" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y4" s="1">
         <v>1E-8</v>
@@ -8048,7 +8170,7 @@
         <v>12</v>
       </c>
       <c r="F5">
-        <v>0.22</v>
+        <v>5</v>
       </c>
       <c r="G5">
         <v>0.5</v>
@@ -8095,14 +8217,14 @@
       <c r="U5" s="1">
         <v>1E-8</v>
       </c>
-      <c r="V5">
-        <v>0.05</v>
-      </c>
-      <c r="W5">
-        <v>1</v>
-      </c>
-      <c r="X5">
-        <v>500</v>
+      <c r="V5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="W5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X5" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y5" s="1">
         <v>1E-8</v>
@@ -8143,7 +8265,7 @@
         <v>14</v>
       </c>
       <c r="F6">
-        <v>0.2</v>
+        <v>5</v>
       </c>
       <c r="G6">
         <v>0.5</v>
@@ -8190,14 +8312,14 @@
       <c r="U6" s="1">
         <v>1E-8</v>
       </c>
-      <c r="V6">
-        <v>0.05</v>
-      </c>
-      <c r="W6">
-        <v>1</v>
-      </c>
-      <c r="X6">
-        <v>500</v>
+      <c r="V6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="W6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X6" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y6" s="1">
         <v>1E-8</v>
@@ -8238,7 +8360,7 @@
         <v>15</v>
       </c>
       <c r="F7">
-        <v>0.2</v>
+        <v>5</v>
       </c>
       <c r="G7">
         <v>0.5</v>
@@ -8285,14 +8407,14 @@
       <c r="U7" s="1">
         <v>1E-8</v>
       </c>
-      <c r="V7">
-        <v>0.05</v>
-      </c>
-      <c r="W7">
-        <v>1</v>
-      </c>
-      <c r="X7">
-        <v>500</v>
+      <c r="V7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="W7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X7" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y7" s="1">
         <v>1E-8</v>
@@ -8326,7 +8448,7 @@
   <dimension ref="A1:AE23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AE2" sqref="AE2"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8434,13 +8556,13 @@
         <v>17</v>
       </c>
       <c r="D2">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E2">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F2">
-        <v>0.4</v>
+        <v>6</v>
       </c>
       <c r="G2">
         <v>3</v>
@@ -8469,14 +8591,14 @@
       <c r="O2">
         <v>2100</v>
       </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
+      <c r="P2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="R2" s="1">
+        <v>1E-8</v>
       </c>
       <c r="S2">
         <v>140</v>
@@ -8488,13 +8610,13 @@
         <v>1E-8</v>
       </c>
       <c r="V2" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="W2" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="X2">
-        <v>700</v>
+        <v>1E-8</v>
+      </c>
+      <c r="X2" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y2" s="1">
         <v>1E-8</v>
@@ -8529,13 +8651,13 @@
         <v>16</v>
       </c>
       <c r="D3">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E3">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F3">
-        <v>0.3</v>
+        <v>5</v>
       </c>
       <c r="G3">
         <v>0.6</v>
@@ -8564,14 +8686,14 @@
       <c r="O3">
         <v>2100</v>
       </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
+      <c r="P3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="R3" s="1">
+        <v>1E-8</v>
       </c>
       <c r="S3">
         <v>140</v>
@@ -8583,13 +8705,13 @@
         <v>1E-8</v>
       </c>
       <c r="V3" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="W3" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="X3">
-        <v>700</v>
+        <v>1E-8</v>
+      </c>
+      <c r="X3" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y3" s="1">
         <v>1E-8</v>
@@ -8624,13 +8746,13 @@
         <v>16</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="E4">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F4">
-        <v>0.25</v>
+        <v>5</v>
       </c>
       <c r="G4">
         <v>0.5</v>
@@ -8659,14 +8781,14 @@
       <c r="O4">
         <v>2100</v>
       </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
+      <c r="P4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="R4" s="1">
+        <v>1E-8</v>
       </c>
       <c r="S4">
         <v>140</v>
@@ -8678,13 +8800,13 @@
         <v>1E-8</v>
       </c>
       <c r="V4" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="W4" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="X4">
-        <v>700</v>
+        <v>1E-8</v>
+      </c>
+      <c r="X4" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y4" s="1">
         <v>1E-8</v>
@@ -8719,13 +8841,13 @@
         <v>15</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E5">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F5">
-        <v>0.25</v>
+        <v>5</v>
       </c>
       <c r="G5">
         <v>0.4</v>
@@ -8754,14 +8876,14 @@
       <c r="O5">
         <v>2100</v>
       </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
+      <c r="P5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="R5" s="1">
+        <v>1E-8</v>
       </c>
       <c r="S5">
         <v>140</v>
@@ -8773,13 +8895,13 @@
         <v>1E-8</v>
       </c>
       <c r="V5" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="W5" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="X5">
-        <v>700</v>
+        <v>1E-8</v>
+      </c>
+      <c r="X5" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y5" s="1">
         <v>1E-8</v>
@@ -8814,13 +8936,13 @@
         <v>15</v>
       </c>
       <c r="D6">
-        <v>0.5</v>
+        <v>20</v>
       </c>
       <c r="E6">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F6">
-        <v>0.25</v>
+        <v>5</v>
       </c>
       <c r="G6">
         <v>0.4</v>
@@ -8849,14 +8971,14 @@
       <c r="O6">
         <v>2100</v>
       </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
+      <c r="P6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="R6" s="1">
+        <v>1E-8</v>
       </c>
       <c r="S6">
         <v>140</v>
@@ -8868,13 +8990,13 @@
         <v>1E-8</v>
       </c>
       <c r="V6" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="W6" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="X6">
-        <v>700</v>
+        <v>1E-8</v>
+      </c>
+      <c r="X6" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y6" s="1">
         <v>1E-8</v>
@@ -8909,13 +9031,13 @@
         <v>15</v>
       </c>
       <c r="D7">
-        <v>0.1</v>
+        <v>20</v>
       </c>
       <c r="E7">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F7">
-        <v>0.26</v>
+        <v>5</v>
       </c>
       <c r="G7">
         <v>0.5</v>
@@ -8944,14 +9066,14 @@
       <c r="O7">
         <v>2100</v>
       </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
+      <c r="P7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="R7" s="1">
+        <v>1E-8</v>
       </c>
       <c r="S7">
         <v>140</v>
@@ -8963,13 +9085,13 @@
         <v>1E-8</v>
       </c>
       <c r="V7" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="W7" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="X7">
-        <v>700</v>
+        <v>1E-8</v>
+      </c>
+      <c r="X7" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y7" s="1">
         <v>1E-8</v>
@@ -9103,11 +9225,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BAD5EA-F348-48A3-B633-7255CE54E243}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E960D6A2-41BB-4299-A7F8-14217D39C67E}">
   <dimension ref="A1:AE7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AB2" sqref="AB2"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9212,91 +9334,91 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>15.971701436463601</v>
+        <v>16</v>
       </c>
       <c r="D2">
-        <v>12.478397391190899</v>
+        <v>16</v>
       </c>
       <c r="E2">
-        <v>11.939059143897</v>
+        <v>15</v>
       </c>
       <c r="F2">
-        <v>0.40568974343973402</v>
+        <v>7</v>
       </c>
       <c r="G2">
-        <v>2.28532503405529</v>
+        <v>5</v>
       </c>
       <c r="H2">
-        <v>0.51071461273790897</v>
+        <v>1</v>
       </c>
       <c r="I2">
-        <v>17.9120553184164</v>
+        <v>18</v>
       </c>
       <c r="J2">
-        <v>33.508060419989697</v>
+        <v>45</v>
       </c>
       <c r="K2">
-        <v>28.004173154075499</v>
+        <v>28.000000008171401</v>
       </c>
       <c r="L2">
-        <v>49.8650536327319</v>
+        <v>50</v>
       </c>
       <c r="M2">
-        <v>1084.4341884594701</v>
+        <v>1100</v>
       </c>
       <c r="N2">
-        <v>154.44610099616699</v>
+        <v>160</v>
       </c>
       <c r="O2">
-        <v>1568.1939576355701</v>
+        <v>1400</v>
       </c>
       <c r="P2" s="1">
-        <v>3.3822830241745699E-9</v>
+        <v>1E-8</v>
       </c>
       <c r="Q2" s="1">
-        <v>6.9605187292693698E-10</v>
+        <v>1E-8</v>
       </c>
       <c r="R2" s="1">
-        <v>5.3783110684136303E-12</v>
+        <v>1E-8</v>
       </c>
       <c r="S2">
-        <v>50.387849658292097</v>
+        <v>70</v>
       </c>
       <c r="T2">
-        <v>129.16429734229101</v>
+        <v>140</v>
       </c>
       <c r="U2" s="1">
-        <v>1.46570857376267E-5</v>
-      </c>
-      <c r="V2">
-        <v>1.46748294386595E-2</v>
-      </c>
-      <c r="W2">
-        <v>1.3055713970776199</v>
-      </c>
-      <c r="X2">
-        <v>378.131909413328</v>
+        <v>1E-8</v>
+      </c>
+      <c r="V2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="W2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X2" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y2" s="1">
-        <v>1.4657055899174099E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="Z2" s="1">
-        <v>1.46570495617937E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="AA2" s="1">
-        <v>1.4657065807208301E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="AB2" s="1">
-        <v>1.4657048878436601E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="AC2" s="1">
-        <v>1.4657065807208001E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="AD2">
-        <v>86.9990036927028</v>
+        <v>87</v>
       </c>
       <c r="AE2">
-        <v>425.00000000003899</v>
+        <v>425</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
@@ -9307,91 +9429,91 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>15.4039586857216</v>
+        <v>16</v>
       </c>
       <c r="D3">
-        <v>9.8719380225966908</v>
+        <v>12</v>
       </c>
       <c r="E3">
-        <v>13.940476118451301</v>
+        <v>16</v>
       </c>
       <c r="F3">
-        <v>0.26686860650720401</v>
+        <v>6</v>
       </c>
       <c r="G3">
-        <v>0.80664257051971999</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>8.7025270524595993E-2</v>
+        <v>0.2</v>
       </c>
       <c r="I3">
-        <v>17.912057578407499</v>
+        <v>18</v>
       </c>
       <c r="J3">
-        <v>21.116951377903501</v>
+        <v>30</v>
       </c>
       <c r="K3">
-        <v>28.0041739364096</v>
+        <v>28.0000000081758</v>
       </c>
       <c r="L3">
-        <v>49.865054669333901</v>
+        <v>50</v>
       </c>
       <c r="M3">
-        <v>1085.3883560822401</v>
+        <v>1100</v>
       </c>
       <c r="N3">
-        <v>130.65523763580401</v>
+        <v>140</v>
       </c>
       <c r="O3">
-        <v>1580.18059136495</v>
+        <v>1400</v>
       </c>
       <c r="P3" s="1">
-        <v>3.38573581806908E-9</v>
+        <v>1E-8</v>
       </c>
       <c r="Q3" s="1">
-        <v>6.9740921158043999E-10</v>
+        <v>1E-8</v>
       </c>
       <c r="R3" s="1">
-        <v>2.5635474952528901E-12</v>
+        <v>1E-8</v>
       </c>
       <c r="S3">
-        <v>50.842455168429296</v>
+        <v>70</v>
       </c>
       <c r="T3">
-        <v>129.152963918468</v>
+        <v>140</v>
       </c>
       <c r="U3" s="1">
-        <v>1.4659593239335001E-5</v>
-      </c>
-      <c r="V3">
-        <v>1.46773399759208E-2</v>
-      </c>
-      <c r="W3">
-        <v>1.3055493316879101</v>
-      </c>
-      <c r="X3">
-        <v>378.15657629876301</v>
+        <v>1E-8</v>
+      </c>
+      <c r="V3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="W3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X3" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y3" s="1">
-        <v>1.46595633957777E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="Z3" s="1">
-        <v>1.4659557058427799E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="AA3" s="1">
-        <v>1.46595733037642E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="AB3" s="1">
-        <v>1.4659556375073999E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="AC3" s="1">
-        <v>1.46595733037639E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="AD3">
-        <v>86.999003505926694</v>
+        <v>87</v>
       </c>
       <c r="AE3">
-        <v>425.00000000004002</v>
+        <v>425</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
@@ -9402,91 +9524,91 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>15.0533473635461</v>
+        <v>16</v>
       </c>
       <c r="D4">
-        <v>7.4679935864291904</v>
+        <v>10</v>
       </c>
       <c r="E4">
-        <v>15.8940254372271</v>
+        <v>20</v>
       </c>
       <c r="F4">
-        <v>0.17408651517353499</v>
+        <v>5.5</v>
       </c>
       <c r="G4">
-        <v>0.65602046298124495</v>
+        <v>0.6</v>
       </c>
       <c r="H4">
-        <v>3.2502623021770101E-2</v>
+        <v>0.06</v>
       </c>
       <c r="I4">
-        <v>17.912059838738099</v>
+        <v>18</v>
       </c>
       <c r="J4">
-        <v>13.788142801348201</v>
+        <v>25</v>
       </c>
       <c r="K4">
-        <v>28.004174718861702</v>
+        <v>28.000000008180098</v>
       </c>
       <c r="L4">
-        <v>49.8650557061641</v>
+        <v>50</v>
       </c>
       <c r="M4">
-        <v>1086.3481873656499</v>
+        <v>1100</v>
       </c>
       <c r="N4">
-        <v>109.881243905839</v>
+        <v>120</v>
       </c>
       <c r="O4">
-        <v>1589.19704579733</v>
+        <v>1400</v>
       </c>
       <c r="P4" s="1">
-        <v>3.38728319834106E-9</v>
+        <v>1E-8</v>
       </c>
       <c r="Q4" s="1">
-        <v>6.9788586979376202E-10</v>
+        <v>1E-8</v>
       </c>
       <c r="R4" s="1">
-        <v>1.1238537195714401E-12</v>
+        <v>1E-8</v>
       </c>
       <c r="S4">
-        <v>51.2743918303822</v>
+        <v>70</v>
       </c>
       <c r="T4">
-        <v>129.153077970742</v>
+        <v>140</v>
       </c>
       <c r="U4" s="1">
-        <v>1.46621011627338E-5</v>
-      </c>
-      <c r="V4">
-        <v>1.4679850935383E-2</v>
-      </c>
-      <c r="W4">
-        <v>1.3055272618740601</v>
-      </c>
-      <c r="X4">
-        <v>378.15171049972997</v>
+        <v>1E-8</v>
+      </c>
+      <c r="V4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="W4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X4" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y4" s="1">
-        <v>1.46620713140709E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="Z4" s="1">
-        <v>1.4662064976751599E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="AA4" s="1">
-        <v>1.46620812220094E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="AB4" s="1">
-        <v>1.4662064293401199E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="AC4" s="1">
-        <v>1.46620812220091E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="AD4">
-        <v>86.999003319122494</v>
+        <v>87</v>
       </c>
       <c r="AE4">
-        <v>425.00000000004098</v>
+        <v>425</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
@@ -9497,91 +9619,91 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>14.835633042732701</v>
+        <v>16</v>
       </c>
       <c r="D5">
-        <v>5.2909932453474804</v>
+        <v>6</v>
       </c>
       <c r="E5">
-        <v>17.718892219548401</v>
+        <v>23</v>
       </c>
       <c r="F5">
-        <v>0.107409569913944</v>
+        <v>5.5</v>
       </c>
       <c r="G5">
-        <v>0.58988861156732797</v>
+        <v>0.6</v>
       </c>
       <c r="H5">
-        <v>2.03994477068483E-2</v>
+        <v>0.03</v>
       </c>
       <c r="I5">
-        <v>17.9120620994943</v>
+        <v>18</v>
       </c>
       <c r="J5">
-        <v>9.44747896308915</v>
+        <v>15</v>
       </c>
       <c r="K5">
-        <v>28.004175501461201</v>
+        <v>28.0000000081845</v>
       </c>
       <c r="L5">
-        <v>49.865056743261903</v>
+        <v>50</v>
       </c>
       <c r="M5">
-        <v>1087.3124457506999</v>
+        <v>1100</v>
       </c>
       <c r="N5">
-        <v>92.113646341271405</v>
+        <v>100</v>
       </c>
       <c r="O5">
-        <v>1596.2366387976101</v>
+        <v>1400</v>
       </c>
       <c r="P5" s="1">
-        <v>3.3880641365267801E-9</v>
+        <v>1E-8</v>
       </c>
       <c r="Q5" s="1">
-        <v>6.9793765254478605E-10</v>
+        <v>1E-8</v>
       </c>
       <c r="R5" s="1">
-        <v>5.7677245380565098E-13</v>
+        <v>1E-8</v>
       </c>
       <c r="S5">
-        <v>51.667779826438</v>
+        <v>70</v>
       </c>
       <c r="T5">
-        <v>129.153192044349</v>
+        <v>140</v>
       </c>
       <c r="U5" s="1">
-        <v>1.4664609515189199E-5</v>
-      </c>
-      <c r="V5">
-        <v>1.46823623244214E-2</v>
-      </c>
-      <c r="W5">
-        <v>1.3055051875713</v>
-      </c>
-      <c r="X5">
-        <v>378.14684387601199</v>
+        <v>1E-8</v>
+      </c>
+      <c r="V5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="W5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X5" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y5" s="1">
-        <v>1.46645796614199E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="Z5" s="1">
-        <v>1.4664573324131601E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="AA5" s="1">
-        <v>1.46645895693101E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="AB5" s="1">
-        <v>1.4664572640784401E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="AC5" s="1">
-        <v>1.4664589569309801E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="AD5">
-        <v>86.999003132283207</v>
+        <v>87</v>
       </c>
       <c r="AE5">
-        <v>425.00000000004201</v>
+        <v>425</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
@@ -9592,91 +9714,91 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>14.6951634648394</v>
+        <v>16</v>
       </c>
       <c r="D6">
-        <v>3.43217997624122</v>
+        <v>3</v>
       </c>
       <c r="E6">
-        <v>19.318273213829102</v>
+        <v>25</v>
       </c>
       <c r="F6">
-        <v>6.5330867112335794E-2</v>
+        <v>5.5</v>
       </c>
       <c r="G6">
-        <v>0.54831640754200694</v>
+        <v>0.5</v>
       </c>
       <c r="H6">
-        <v>1.6627456877792001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="I6">
-        <v>17.9120643606743</v>
+        <v>18</v>
       </c>
       <c r="J6">
-        <v>6.8312987213797598</v>
+        <v>11</v>
       </c>
       <c r="K6">
-        <v>28.004176284207499</v>
+        <v>28.000000008188799</v>
       </c>
       <c r="L6">
-        <v>49.865057780626401</v>
+        <v>50</v>
       </c>
       <c r="M6">
-        <v>1088.2799835488299</v>
+        <v>1100</v>
       </c>
       <c r="N6">
-        <v>77.229539508241203</v>
+        <v>80</v>
       </c>
       <c r="O6">
-        <v>1601.43983832806</v>
+        <v>1400</v>
       </c>
       <c r="P6" s="1">
-        <v>3.3885596139397498E-9</v>
+        <v>1E-8</v>
       </c>
       <c r="Q6" s="1">
-        <v>6.9784037437320498E-10</v>
+        <v>1E-8</v>
       </c>
       <c r="R6" s="1">
-        <v>3.8458523616187098E-13</v>
+        <v>1E-8</v>
       </c>
       <c r="S6">
-        <v>51.999904470552998</v>
+        <v>70</v>
       </c>
       <c r="T6">
-        <v>129.15330613919201</v>
+        <v>140</v>
       </c>
       <c r="U6" s="1">
-        <v>1.4667118296617301E-5</v>
-      </c>
-      <c r="V6">
-        <v>1.46848741429517E-2</v>
-      </c>
-      <c r="W6">
-        <v>1.3054831087798899</v>
-      </c>
-      <c r="X6">
-        <v>378.14197642779402</v>
+        <v>1E-8</v>
+      </c>
+      <c r="V6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="W6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X6" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y6" s="1">
-        <v>1.4667088437740701E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="Z6" s="1">
-        <v>1.46670821004835E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="AA6" s="1">
-        <v>1.46670983455823E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="AB6" s="1">
-        <v>1.46670814171397E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="AC6" s="1">
-        <v>1.4667098345582001E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="AD6">
-        <v>86.999002945408805</v>
+        <v>87</v>
       </c>
       <c r="AE6">
-        <v>425.00000000004201</v>
+        <v>425</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
@@ -9687,91 +9809,91 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>14.600204981909901</v>
+        <v>16</v>
       </c>
       <c r="D7">
-        <v>1.97093856394816</v>
+        <v>3</v>
       </c>
       <c r="E7">
-        <v>20.606962014706301</v>
+        <v>28</v>
       </c>
       <c r="F7">
-        <v>4.6218770758075803E-2</v>
+        <v>5</v>
       </c>
       <c r="G7">
-        <v>0.51332916230752301</v>
+        <v>0.5</v>
       </c>
       <c r="H7">
-        <v>1.49954010246778E-2</v>
+        <v>0.02</v>
       </c>
       <c r="I7">
-        <v>17.9120666222781</v>
+        <v>18</v>
       </c>
       <c r="J7">
-        <v>5.2172166789254497</v>
+        <v>9</v>
       </c>
       <c r="K7">
-        <v>28.004177067100599</v>
+        <v>28.000000008193201</v>
       </c>
       <c r="L7">
-        <v>49.865058818257602</v>
+        <v>50</v>
       </c>
       <c r="M7">
-        <v>1089.2497504718999</v>
+        <v>1100</v>
       </c>
       <c r="N7">
-        <v>65.007299728345401</v>
+        <v>70</v>
       </c>
       <c r="O7">
-        <v>1604.9646879509801</v>
+        <v>1400</v>
       </c>
       <c r="P7" s="1">
-        <v>3.3889458905085399E-9</v>
+        <v>1E-8</v>
       </c>
       <c r="Q7" s="1">
-        <v>6.9769985334181395E-10</v>
+        <v>1E-8</v>
       </c>
       <c r="R7" s="1">
-        <v>3.1843463307294298E-13</v>
+        <v>1E-8</v>
       </c>
       <c r="S7">
-        <v>52.250967662514299</v>
+        <v>70</v>
       </c>
       <c r="T7">
-        <v>129.15342025527599</v>
+        <v>140</v>
       </c>
       <c r="U7" s="1">
-        <v>1.4669627507092799E-5</v>
-      </c>
-      <c r="V7">
-        <v>1.4687386391048799E-2</v>
-      </c>
-      <c r="W7">
-        <v>1.30546102549868</v>
-      </c>
-      <c r="X7">
-        <v>378.13710815493403</v>
+        <v>1E-8</v>
+      </c>
+      <c r="V7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="W7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X7" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y7" s="1">
-        <v>1.4669597643108099E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="Z7" s="1">
-        <v>1.46695913058821E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="AA7" s="1">
-        <v>1.46696075509006E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="AB7" s="1">
-        <v>1.46695906225417E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="AC7" s="1">
-        <v>1.46696075509004E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="AD7">
-        <v>86.999002758499401</v>
+        <v>87</v>
       </c>
       <c r="AE7">
-        <v>425.00000000004297</v>
+        <v>425</v>
       </c>
     </row>
   </sheetData>
@@ -9780,11 +9902,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{123566AA-3B42-445A-8039-2B5CB75FF954}">
-  <dimension ref="A1:AE23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BAD5EA-F348-48A3-B633-7255CE54E243}">
+  <dimension ref="A1:AE7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="P2" sqref="P2:R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9889,28 +10011,28 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>15.964168264823</v>
+        <v>16</v>
       </c>
       <c r="D2">
-        <v>11.955471759513101</v>
+        <v>16</v>
       </c>
       <c r="E2">
-        <v>9.5606557228841602</v>
+        <v>15</v>
       </c>
       <c r="F2">
-        <v>0.389188365112768</v>
+        <v>7</v>
       </c>
       <c r="G2">
-        <v>2.17499290792734</v>
+        <v>5</v>
       </c>
       <c r="H2">
-        <v>0.48854195924149801</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <v>17.900000000000201</v>
       </c>
       <c r="J2">
-        <v>33.508424248904497</v>
+        <v>35</v>
       </c>
       <c r="K2">
         <v>27.999999999999702</v>
@@ -9919,55 +10041,55 @@
         <v>49.999999999999403</v>
       </c>
       <c r="M2">
-        <v>1133.6174667732</v>
+        <v>1100</v>
       </c>
       <c r="N2">
-        <v>154.10430344009899</v>
+        <v>155</v>
       </c>
       <c r="O2">
-        <v>1644.2773206821801</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
+        <v>1500</v>
+      </c>
+      <c r="P2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="R2" s="1">
+        <v>1E-8</v>
       </c>
       <c r="S2">
-        <v>55.0026849181762</v>
+        <v>60</v>
       </c>
       <c r="T2">
-        <v>132.99113953556699</v>
+        <v>140</v>
       </c>
       <c r="U2" s="1">
-        <v>2.2199861704192199E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="V2" s="1">
-        <v>2.2176095190051401E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="W2" s="1">
-        <v>2.2369842791142799E-16</v>
-      </c>
-      <c r="X2">
-        <v>251.690191789316</v>
+        <v>1E-8</v>
+      </c>
+      <c r="X2" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y2" s="1">
-        <v>2.2369842791142799E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="Z2" s="1">
-        <v>2.2369842791142799E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="AA2" s="1">
-        <v>2.2369842791142799E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="AB2" s="1">
-        <v>2.2369842791142799E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="AC2" s="1">
-        <v>2.2369842791142799E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="AD2">
         <v>86.999999999998806</v>
@@ -9984,28 +10106,28 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>15.4010957280505</v>
+        <v>16</v>
       </c>
       <c r="D3">
-        <v>9.1664325729033305</v>
+        <v>12</v>
       </c>
       <c r="E3">
-        <v>11.7511644522135</v>
+        <v>16</v>
       </c>
       <c r="F3">
-        <v>0.25512871183025598</v>
+        <v>6</v>
       </c>
       <c r="G3">
-        <v>0.77736928316923404</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>8.2527746041897804E-2</v>
+        <v>0.2</v>
       </c>
       <c r="I3">
         <v>17.900000000000301</v>
       </c>
       <c r="J3">
-        <v>21.1409928148957</v>
+        <v>25</v>
       </c>
       <c r="K3">
         <v>27.999999999999599</v>
@@ -10014,55 +10136,55 @@
         <v>49.999999999999297</v>
       </c>
       <c r="M3">
-        <v>1134.6181907672301</v>
+        <v>1100</v>
       </c>
       <c r="N3">
-        <v>130.110958000295</v>
+        <v>130</v>
       </c>
       <c r="O3">
-        <v>1656.1349312129801</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
+        <v>1500</v>
+      </c>
+      <c r="P3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="R3" s="1">
+        <v>1E-8</v>
       </c>
       <c r="S3">
-        <v>55.493911727025399</v>
+        <v>60</v>
       </c>
       <c r="T3">
-        <v>132.984333703663</v>
+        <v>140</v>
       </c>
       <c r="U3" s="1">
-        <v>2.26467727424356E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="V3" s="1">
-        <v>2.2459340064511698E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="W3" s="1">
-        <v>2.2663135879130801E-16</v>
-      </c>
-      <c r="X3">
-        <v>251.70774914433801</v>
+        <v>1E-8</v>
+      </c>
+      <c r="X3" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y3" s="1">
-        <v>2.2663135879130801E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="Z3" s="1">
-        <v>2.2663135879130801E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="AA3" s="1">
-        <v>2.2663135879130801E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="AB3" s="1">
-        <v>2.2663135879130801E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="AC3" s="1">
-        <v>2.2663135879130801E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="AD3">
         <v>86.999999999998707</v>
@@ -10079,28 +10201,28 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>15.0533472392958</v>
+        <v>16</v>
       </c>
       <c r="D4">
-        <v>6.6117757178559202</v>
+        <v>10</v>
       </c>
       <c r="E4">
-        <v>13.8631919379094</v>
+        <v>20</v>
       </c>
       <c r="F4">
-        <v>0.16529604909947901</v>
+        <v>5.5</v>
       </c>
       <c r="G4">
-        <v>0.63561469745252397</v>
+        <v>0.6</v>
       </c>
       <c r="H4">
-        <v>3.1536109742727997E-2</v>
+        <v>0.06</v>
       </c>
       <c r="I4">
         <v>17.900000000000301</v>
       </c>
       <c r="J4">
-        <v>13.8259193889279</v>
+        <v>15</v>
       </c>
       <c r="K4">
         <v>27.999999999999599</v>
@@ -10109,55 +10231,55 @@
         <v>49.999999999999297</v>
       </c>
       <c r="M4">
-        <v>1135.6245853652399</v>
+        <v>1100</v>
       </c>
       <c r="N4">
-        <v>109.28441893184301</v>
+        <v>110</v>
       </c>
       <c r="O4">
-        <v>1664.98266235388</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
+        <v>1500</v>
+      </c>
+      <c r="P4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="R4" s="1">
+        <v>1E-8</v>
       </c>
       <c r="S4">
-        <v>55.955090681462501</v>
+        <v>60</v>
       </c>
       <c r="T4">
-        <v>132.98433370365001</v>
+        <v>140</v>
       </c>
       <c r="U4" s="1">
-        <v>2.2293828391950002E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="V4" s="1">
-        <v>2.2242799101473699E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="W4" s="1">
-        <v>2.2704949760496199E-16</v>
-      </c>
-      <c r="X4">
-        <v>251.707749151249</v>
+        <v>1E-8</v>
+      </c>
+      <c r="X4" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y4" s="1">
-        <v>2.2704949760496199E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="Z4" s="1">
-        <v>2.2704949760496199E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="AA4" s="1">
-        <v>2.2704949760496199E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="AB4" s="1">
-        <v>2.2704949760496199E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="AC4" s="1">
-        <v>2.2704949760496199E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="AD4">
         <v>86.999999999998593</v>
@@ -10174,28 +10296,28 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>14.8369717697799</v>
+        <v>16</v>
       </c>
       <c r="D5">
-        <v>4.3433769441294601</v>
+        <v>6</v>
       </c>
       <c r="E5">
-        <v>15.791038639826199</v>
+        <v>23</v>
       </c>
       <c r="F5">
-        <v>0.10267137491153901</v>
+        <v>5.5</v>
       </c>
       <c r="G5">
-        <v>0.57152937934399295</v>
+        <v>0.6</v>
       </c>
       <c r="H5">
-        <v>2.0359511269457401E-2</v>
+        <v>0.03</v>
       </c>
       <c r="I5">
         <v>17.900000000000301</v>
       </c>
       <c r="J5">
-        <v>9.4914415236919094</v>
+        <v>10</v>
       </c>
       <c r="K5">
         <v>27.999999999999599</v>
@@ -10204,55 +10326,55 @@
         <v>49.999999999999197</v>
       </c>
       <c r="M5">
-        <v>1136.6353294017699</v>
+        <v>1100</v>
       </c>
       <c r="N5">
-        <v>91.579657074113499</v>
+        <v>100</v>
       </c>
       <c r="O5">
-        <v>1671.7876931640101</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
+        <v>1500</v>
+      </c>
+      <c r="P5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="R5" s="1">
+        <v>1E-8</v>
       </c>
       <c r="S5">
-        <v>56.364210345591701</v>
+        <v>60</v>
       </c>
       <c r="T5">
-        <v>132.984333703651</v>
+        <v>140</v>
       </c>
       <c r="U5" s="1">
-        <v>2.23115472375581E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="V5" s="1">
-        <v>2.2568157184515598E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="W5" s="1">
-        <v>2.25663866432334E-16</v>
-      </c>
-      <c r="X5">
-        <v>251.707749151738</v>
+        <v>1E-8</v>
+      </c>
+      <c r="X5" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y5" s="1">
-        <v>2.25663866432334E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="Z5" s="1">
-        <v>2.25663866432334E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="AA5" s="1">
-        <v>2.25663866432334E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="AB5" s="1">
-        <v>2.25663866432334E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="AC5" s="1">
-        <v>2.25663866432334E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="AD5">
         <v>86.999999999998494</v>
@@ -10269,28 +10391,28 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>14.6969935739787</v>
+        <v>16</v>
       </c>
       <c r="D6">
-        <v>2.4912622088890002</v>
+        <v>3</v>
       </c>
       <c r="E6">
-        <v>17.399262288382801</v>
+        <v>25</v>
       </c>
       <c r="F6">
-        <v>6.5717484233544093E-2</v>
+        <v>5.5</v>
       </c>
       <c r="G6">
-        <v>0.53117462088732303</v>
+        <v>0.5</v>
       </c>
       <c r="H6">
-        <v>1.6801983986823001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="I6">
         <v>17.900000000000301</v>
       </c>
       <c r="J6">
-        <v>6.8800570700563899</v>
+        <v>7</v>
       </c>
       <c r="K6">
         <v>27.999999999999599</v>
@@ -10299,55 +10421,55 @@
         <v>49.999999999999197</v>
       </c>
       <c r="M6">
-        <v>1137.64921606396</v>
+        <v>1100</v>
       </c>
       <c r="N6">
-        <v>76.836036315346206</v>
+        <v>80</v>
       </c>
       <c r="O6">
-        <v>1676.7093531605401</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
+        <v>1500</v>
+      </c>
+      <c r="P6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="R6" s="1">
+        <v>1E-8</v>
       </c>
       <c r="S6">
-        <v>56.689355797798498</v>
+        <v>60</v>
       </c>
       <c r="T6">
-        <v>132.98433370365001</v>
+        <v>140</v>
       </c>
       <c r="U6" s="1">
-        <v>2.2636056658874998E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="V6" s="1">
-        <v>2.2328061073998998E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="W6" s="1">
-        <v>2.2756738177842602E-16</v>
-      </c>
-      <c r="X6">
-        <v>251.70774915165401</v>
+        <v>1E-8</v>
+      </c>
+      <c r="X6" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y6" s="1">
-        <v>2.2756738177842602E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="Z6" s="1">
-        <v>2.2756738177842602E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="AA6" s="1">
-        <v>2.2756738177842602E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="AB6" s="1">
-        <v>2.2756738177842602E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="AC6" s="1">
-        <v>2.2756738177842602E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="AD6">
         <v>86.999999999998394</v>
@@ -10364,28 +10486,28 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>14.6021934286321</v>
+        <v>16</v>
       </c>
       <c r="D7">
-        <v>1.1843205924461</v>
+        <v>3</v>
       </c>
       <c r="E7">
-        <v>18.553075184225101</v>
+        <v>28</v>
       </c>
       <c r="F7">
-        <v>5.2735791199725199E-2</v>
+        <v>5</v>
       </c>
       <c r="G7">
-        <v>0.49096727308696603</v>
+        <v>0.5</v>
       </c>
       <c r="H7">
-        <v>1.50744031299521E-2</v>
+        <v>0.02</v>
       </c>
       <c r="I7">
         <v>17.9000000000004</v>
       </c>
       <c r="J7">
-        <v>5.2743682992074703</v>
+        <v>6</v>
       </c>
       <c r="K7">
         <v>27.999999999999499</v>
@@ -10394,55 +10516,55 @@
         <v>49.999999999999098</v>
       </c>
       <c r="M7">
-        <v>1138.6651536781501</v>
+        <v>1100</v>
       </c>
       <c r="N7">
-        <v>64.796429484577402</v>
+        <v>70</v>
       </c>
       <c r="O7">
-        <v>1679.93123660022</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
+        <v>1500</v>
+      </c>
+      <c r="P7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="R7" s="1">
+        <v>1E-8</v>
       </c>
       <c r="S7">
-        <v>56.898968138018297</v>
+        <v>60</v>
       </c>
       <c r="T7">
-        <v>132.98433370365001</v>
+        <v>140</v>
       </c>
       <c r="U7" s="1">
-        <v>2.2367208035685199E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="V7" s="1">
-        <v>2.2537623622731301E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="W7" s="1">
-        <v>2.2659118654067102E-16</v>
-      </c>
-      <c r="X7">
-        <v>251.70774915122701</v>
+        <v>1E-8</v>
+      </c>
+      <c r="X7" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y7" s="1">
-        <v>2.2659118654067102E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="Z7" s="1">
-        <v>2.2659118654067102E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="AA7" s="1">
-        <v>2.2659118654067102E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="AB7" s="1">
-        <v>2.2659118654067102E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="AC7" s="1">
-        <v>2.2659118654067102E-16</v>
+        <v>1E-8</v>
       </c>
       <c r="AD7">
         <v>86.999999999998295</v>
@@ -10450,66 +10572,6 @@
       <c r="AE7">
         <v>424.99999999999301</v>
       </c>
-    </row>
-    <row r="18" spans="21:29" x14ac:dyDescent="0.25">
-      <c r="U18" s="1"/>
-      <c r="V18" s="1"/>
-      <c r="W18" s="1"/>
-      <c r="Y18" s="1"/>
-      <c r="Z18" s="1"/>
-      <c r="AA18" s="1"/>
-      <c r="AB18" s="1"/>
-      <c r="AC18" s="1"/>
-    </row>
-    <row r="19" spans="21:29" x14ac:dyDescent="0.25">
-      <c r="U19" s="1"/>
-      <c r="V19" s="1"/>
-      <c r="W19" s="1"/>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="1"/>
-      <c r="AA19" s="1"/>
-      <c r="AB19" s="1"/>
-      <c r="AC19" s="1"/>
-    </row>
-    <row r="20" spans="21:29" x14ac:dyDescent="0.25">
-      <c r="U20" s="1"/>
-      <c r="V20" s="1"/>
-      <c r="W20" s="1"/>
-      <c r="Y20" s="1"/>
-      <c r="Z20" s="1"/>
-      <c r="AA20" s="1"/>
-      <c r="AB20" s="1"/>
-      <c r="AC20" s="1"/>
-    </row>
-    <row r="21" spans="21:29" x14ac:dyDescent="0.25">
-      <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
-      <c r="W21" s="1"/>
-      <c r="Y21" s="1"/>
-      <c r="Z21" s="1"/>
-      <c r="AA21" s="1"/>
-      <c r="AB21" s="1"/>
-      <c r="AC21" s="1"/>
-    </row>
-    <row r="22" spans="21:29" x14ac:dyDescent="0.25">
-      <c r="U22" s="1"/>
-      <c r="V22" s="1"/>
-      <c r="W22" s="1"/>
-      <c r="Y22" s="1"/>
-      <c r="Z22" s="1"/>
-      <c r="AA22" s="1"/>
-      <c r="AB22" s="1"/>
-      <c r="AC22" s="1"/>
-    </row>
-    <row r="23" spans="21:29" x14ac:dyDescent="0.25">
-      <c r="U23" s="1"/>
-      <c r="V23" s="1"/>
-      <c r="W23" s="1"/>
-      <c r="Y23" s="1"/>
-      <c r="Z23" s="1"/>
-      <c r="AA23" s="1"/>
-      <c r="AB23" s="1"/>
-      <c r="AC23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10521,7 +10583,7 @@
   <dimension ref="A1:AE7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AA3" sqref="AA3"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10635,7 +10697,7 @@
         <v>20</v>
       </c>
       <c r="F2">
-        <v>0.5</v>
+        <v>6</v>
       </c>
       <c r="G2">
         <v>2</v>
@@ -10682,14 +10744,14 @@
       <c r="U2" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="V2">
-        <v>0.01</v>
-      </c>
-      <c r="W2">
-        <v>2</v>
-      </c>
-      <c r="X2">
-        <v>350</v>
+      <c r="V2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="W2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X2" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y2" s="1">
         <v>1E-8</v>
@@ -10730,7 +10792,7 @@
         <v>20</v>
       </c>
       <c r="F3">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -10777,14 +10839,14 @@
       <c r="U3" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="V3">
-        <v>0.01</v>
-      </c>
-      <c r="W3">
-        <v>2</v>
-      </c>
-      <c r="X3">
-        <v>350</v>
+      <c r="V3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="W3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X3" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y3" s="1">
         <v>1E-8</v>
@@ -10825,7 +10887,7 @@
         <v>20</v>
       </c>
       <c r="F4">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="G4">
         <v>0.5</v>
@@ -10872,14 +10934,14 @@
       <c r="U4" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="V4">
-        <v>0.01</v>
-      </c>
-      <c r="W4">
-        <v>2</v>
-      </c>
-      <c r="X4">
-        <v>350</v>
+      <c r="V4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="W4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X4" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y4" s="1">
         <v>1E-8</v>
@@ -10920,7 +10982,7 @@
         <v>20</v>
       </c>
       <c r="F5">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="G5">
         <v>0.5</v>
@@ -10967,14 +11029,14 @@
       <c r="U5" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="V5">
-        <v>0.01</v>
-      </c>
-      <c r="W5">
-        <v>2</v>
-      </c>
-      <c r="X5">
-        <v>350</v>
+      <c r="V5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="W5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X5" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y5" s="1">
         <v>1E-8</v>
@@ -11015,7 +11077,7 @@
         <v>20</v>
       </c>
       <c r="F6">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="G6">
         <v>0.5</v>
@@ -11062,14 +11124,14 @@
       <c r="U6" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="V6">
-        <v>0.01</v>
-      </c>
-      <c r="W6">
-        <v>2</v>
-      </c>
-      <c r="X6">
-        <v>350</v>
+      <c r="V6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="W6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X6" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y6" s="1">
         <v>1E-8</v>
@@ -11110,7 +11172,7 @@
         <v>20</v>
       </c>
       <c r="F7">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="G7">
         <v>0.5</v>
@@ -11157,14 +11219,14 @@
       <c r="U7" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="V7">
-        <v>0.01</v>
-      </c>
-      <c r="W7">
-        <v>2</v>
-      </c>
-      <c r="X7">
-        <v>350</v>
+      <c r="V7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="W7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X7" s="1">
+        <v>1E-8</v>
       </c>
       <c r="Y7" s="1">
         <v>1E-8</v>
@@ -11195,10 +11257,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5589379-171B-4A97-AC18-14A5DD584161}">
-  <dimension ref="A1:AE7"/>
+  <dimension ref="A1:AE15"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="AA3" sqref="AA3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11312,7 +11374,7 @@
         <v>20</v>
       </c>
       <c r="F2">
-        <v>0.5</v>
+        <v>6</v>
       </c>
       <c r="G2">
         <v>2</v>
@@ -11333,7 +11395,7 @@
         <v>50</v>
       </c>
       <c r="M2">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="N2">
         <v>60</v>
@@ -11362,11 +11424,11 @@
       <c r="V2" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="W2">
-        <v>0.1</v>
-      </c>
-      <c r="X2">
-        <v>500</v>
+      <c r="W2" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="X2" s="1">
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="Y2" s="1">
         <v>1E-8</v>
@@ -11407,7 +11469,7 @@
         <v>20</v>
       </c>
       <c r="F3">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -11428,7 +11490,7 @@
         <v>50</v>
       </c>
       <c r="M3">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="N3">
         <v>50</v>
@@ -11457,11 +11519,11 @@
       <c r="V3" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="W3">
-        <v>0.1</v>
-      </c>
-      <c r="X3">
-        <v>500</v>
+      <c r="W3" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="X3" s="1">
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="Y3" s="1">
         <v>1E-8</v>
@@ -11502,7 +11564,7 @@
         <v>20</v>
       </c>
       <c r="F4">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="G4">
         <v>0.5</v>
@@ -11523,7 +11585,7 @@
         <v>50</v>
       </c>
       <c r="M4">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="N4">
         <v>40</v>
@@ -11552,11 +11614,11 @@
       <c r="V4" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="W4">
-        <v>0.1</v>
-      </c>
-      <c r="X4">
-        <v>500</v>
+      <c r="W4" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="X4" s="1">
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="Y4" s="1">
         <v>1E-8</v>
@@ -11597,7 +11659,7 @@
         <v>20</v>
       </c>
       <c r="F5">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="G5">
         <v>0.5</v>
@@ -11618,7 +11680,7 @@
         <v>50</v>
       </c>
       <c r="M5">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="N5">
         <v>30</v>
@@ -11647,11 +11709,11 @@
       <c r="V5" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="W5">
-        <v>0.1</v>
-      </c>
-      <c r="X5">
-        <v>500</v>
+      <c r="W5" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="X5" s="1">
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="Y5" s="1">
         <v>1E-8</v>
@@ -11692,7 +11754,7 @@
         <v>20</v>
       </c>
       <c r="F6">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="G6">
         <v>0.5</v>
@@ -11713,7 +11775,7 @@
         <v>50</v>
       </c>
       <c r="M6">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="N6">
         <v>25</v>
@@ -11742,11 +11804,11 @@
       <c r="V6" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="W6">
-        <v>0.1</v>
-      </c>
-      <c r="X6">
-        <v>500</v>
+      <c r="W6" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="X6" s="1">
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="Y6" s="1">
         <v>1E-8</v>
@@ -11787,7 +11849,7 @@
         <v>20</v>
       </c>
       <c r="F7">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="G7">
         <v>0.5</v>
@@ -11808,7 +11870,7 @@
         <v>50</v>
       </c>
       <c r="M7">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="N7">
         <v>25</v>
@@ -11837,11 +11899,11 @@
       <c r="V7" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="W7">
-        <v>0.1</v>
-      </c>
-      <c r="X7">
-        <v>500</v>
+      <c r="W7" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="X7" s="1">
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="Y7" s="1">
         <v>1E-8</v>
@@ -11864,6 +11926,72 @@
       <c r="AE7">
         <v>425.00000000005502</v>
       </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="1"/>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11874,8 +12002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC5318B9-9FE8-4735-97AC-C84ECA362166}">
   <dimension ref="A1:AE7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Y4" sqref="Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12033,32 +12161,32 @@
       <c r="T2">
         <v>110</v>
       </c>
-      <c r="U2">
-        <v>4800</v>
-      </c>
-      <c r="V2">
-        <v>9</v>
-      </c>
-      <c r="W2">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="X2">
-        <v>2400</v>
-      </c>
-      <c r="Y2">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="Z2">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AA2">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AB2">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AC2">
-        <v>1.0000000000000001E-5</v>
+      <c r="U2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="V2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="W2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>1E-8</v>
       </c>
       <c r="AD2">
         <v>86</v>
@@ -12128,32 +12256,32 @@
       <c r="T3">
         <v>110</v>
       </c>
-      <c r="U3">
-        <v>1600</v>
-      </c>
-      <c r="V3">
-        <v>3</v>
-      </c>
-      <c r="W3">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="X3">
-        <v>800</v>
-      </c>
-      <c r="Y3">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="Z3">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AA3">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AB3">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AC3">
-        <v>1.0000000000000001E-5</v>
+      <c r="U3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="V3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="W3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>1E-8</v>
       </c>
       <c r="AD3">
         <v>86</v>
@@ -12223,32 +12351,32 @@
       <c r="T4">
         <v>110</v>
       </c>
-      <c r="U4">
-        <v>1400</v>
-      </c>
-      <c r="V4">
-        <v>2.5</v>
-      </c>
-      <c r="W4">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="X4">
-        <v>700</v>
-      </c>
-      <c r="Y4">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="Z4">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AA4">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AB4">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AC4">
-        <v>1.0000000000000001E-5</v>
+      <c r="U4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="V4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="W4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>1E-8</v>
       </c>
       <c r="AD4">
         <v>86</v>
@@ -12318,32 +12446,32 @@
       <c r="T5">
         <v>110</v>
       </c>
-      <c r="U5">
-        <v>1400</v>
-      </c>
-      <c r="V5">
-        <v>2.5</v>
-      </c>
-      <c r="W5">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="X5">
-        <v>700</v>
-      </c>
-      <c r="Y5">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="Z5">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AA5">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AB5">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AC5">
-        <v>1.0000000000000001E-5</v>
+      <c r="U5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="V5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="W5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>1E-8</v>
       </c>
       <c r="AD5">
         <v>86</v>
@@ -12413,32 +12541,32 @@
       <c r="T6">
         <v>110</v>
       </c>
-      <c r="U6">
-        <v>1400</v>
-      </c>
-      <c r="V6">
-        <v>2.5</v>
-      </c>
-      <c r="W6">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="X6">
-        <v>700</v>
-      </c>
-      <c r="Y6">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="Z6">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AA6">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AB6">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AC6">
-        <v>1.0000000000000001E-5</v>
+      <c r="U6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="V6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="W6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>1E-8</v>
       </c>
       <c r="AD6">
         <v>86</v>
@@ -12508,32 +12636,32 @@
       <c r="T7">
         <v>110</v>
       </c>
-      <c r="U7">
-        <v>1400</v>
-      </c>
-      <c r="V7">
-        <v>2.5</v>
-      </c>
-      <c r="W7">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="X7">
-        <v>700</v>
-      </c>
-      <c r="Y7">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="Z7">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AA7">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AB7">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AC7">
-        <v>1.0000000000000001E-5</v>
+      <c r="U7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="V7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="W7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="X7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>1E-8</v>
       </c>
       <c r="AD7">
         <v>86</v>

</xml_diff>

<commit_message>
converged but failed EBPR
</commit_message>
<xml_diff>
--- a/exposan/werf/data/initial_conditions.xlsx
+++ b/exposan/werf/data/initial_conditions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joy_c\Dropbox\PhD\Research\QSD\codes_developing\EXPOsan\exposan\werf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAD7F26-A9A0-40A8-9920-78B7AB062D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC9C976-AFAB-4A0D-9C4C-D00119AACE3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" firstSheet="5" activeTab="14" xr2:uid="{218DD762-44D5-4240-B5CB-C558EBE30BA7}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" firstSheet="5" activeTab="15" xr2:uid="{218DD762-44D5-4240-B5CB-C558EBE30BA7}"/>
   </bookViews>
   <sheets>
     <sheet name="B1" sheetId="6" r:id="rId1"/>
@@ -5154,8 +5154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42016BA4-57DB-462D-9767-837B2F986A82}">
   <dimension ref="A1:AE16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5891,8 +5891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12367F69-A662-4BD3-AE36-01641D10E752}">
   <dimension ref="A1:AE16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6569,6 +6569,9 @@
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
@@ -6578,6 +6581,9 @@
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="R12" s="1"/>
       <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
@@ -6587,6 +6593,9 @@
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="R13" s="1"/>
       <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
@@ -6596,6 +6605,9 @@
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="R14" s="1"/>
       <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
@@ -6605,6 +6617,9 @@
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="R15" s="1"/>
       <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
@@ -6630,7 +6645,7 @@
   <dimension ref="A1:AF7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+      <selection activeCell="AB6" sqref="AB6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7291,13 +7306,13 @@
         <v>0.01</v>
       </c>
       <c r="X7">
-        <v>10</v>
+        <v>0.01</v>
       </c>
       <c r="Y7">
-        <v>300</v>
+        <v>0.01</v>
       </c>
       <c r="Z7">
-        <v>10000</v>
+        <v>0.01</v>
       </c>
       <c r="AA7">
         <v>0.01</v>

</xml_diff>

<commit_message>
minor control optimization on G1
</commit_message>
<xml_diff>
--- a/exposan/werf/data/initial_conditions.xlsx
+++ b/exposan/werf/data/initial_conditions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joy_c\Dropbox\PhD\Research\QSD\codes_developing\EXPOsan\exposan\werf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0E244D-6A77-46F3-8ACC-82C128D5C3CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FA3BAD-0A55-4DAC-90C9-49674D3246D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23133" yWindow="-93" windowWidth="23226" windowHeight="13866" firstSheet="5" activeTab="16" xr2:uid="{218DD762-44D5-4240-B5CB-C558EBE30BA7}"/>
+    <workbookView xWindow="-23133" yWindow="-93" windowWidth="23226" windowHeight="13866" firstSheet="5" activeTab="17" xr2:uid="{218DD762-44D5-4240-B5CB-C558EBE30BA7}"/>
   </bookViews>
   <sheets>
     <sheet name="B1" sheetId="6" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="77">
   <si>
     <t>S_O2</t>
   </si>
@@ -285,9 +285,6 @@
   <si>
     <t>N2</t>
   </si>
-  <si>
-    <t>G</t>
-  </si>
 </sst>
 </file>
 
@@ -328,10 +325,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6636,10 +6632,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CB7F0C9-B54B-4F93-93CE-9E10B0EA4FF3}">
-  <dimension ref="A1:AF36"/>
+  <dimension ref="A1:AF35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7139,94 +7135,94 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <v>0.2</v>
       </c>
       <c r="E6">
-        <v>50</v>
+        <v>240</v>
       </c>
       <c r="F6">
-        <v>200</v>
+        <v>3000</v>
       </c>
       <c r="G6">
         <v>0.4</v>
       </c>
       <c r="H6">
+        <v>1E-3</v>
+      </c>
+      <c r="I6">
+        <v>18</v>
+      </c>
+      <c r="J6">
+        <v>110</v>
+      </c>
+      <c r="K6">
+        <v>1200</v>
+      </c>
+      <c r="L6">
+        <v>750</v>
+      </c>
+      <c r="M6">
+        <v>8000</v>
+      </c>
+      <c r="N6">
+        <v>120</v>
+      </c>
+      <c r="O6">
+        <v>4500</v>
+      </c>
+      <c r="P6">
+        <v>1500</v>
+      </c>
+      <c r="Q6">
+        <v>400</v>
+      </c>
+      <c r="R6">
         <v>0.1</v>
-      </c>
-      <c r="I6">
-        <v>20</v>
-      </c>
-      <c r="J6">
-        <v>84</v>
-      </c>
-      <c r="K6">
-        <v>28</v>
-      </c>
-      <c r="L6">
-        <v>10</v>
-      </c>
-      <c r="M6">
-        <v>7000</v>
-      </c>
-      <c r="N6">
-        <v>100</v>
-      </c>
-      <c r="O6">
-        <v>4000</v>
-      </c>
-      <c r="P6">
-        <v>500</v>
-      </c>
-      <c r="Q6">
-        <v>100</v>
-      </c>
-      <c r="R6">
-        <v>1</v>
       </c>
       <c r="S6">
         <v>200</v>
       </c>
       <c r="T6">
-        <v>10</v>
-      </c>
-      <c r="U6">
-        <v>0.01</v>
-      </c>
-      <c r="V6">
-        <v>0.01</v>
-      </c>
-      <c r="W6">
-        <v>0.01</v>
-      </c>
-      <c r="X6">
-        <v>0.01</v>
-      </c>
-      <c r="Y6">
-        <v>0.01</v>
-      </c>
-      <c r="Z6">
-        <v>0.01</v>
-      </c>
-      <c r="AA6">
-        <v>0.01</v>
-      </c>
-      <c r="AB6">
-        <v>0.01</v>
-      </c>
-      <c r="AC6">
-        <v>0.01</v>
+        <v>140</v>
+      </c>
+      <c r="U6" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="V6" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="W6" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="X6" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="AD6">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AE6">
         <v>425</v>
@@ -7431,118 +7427,23 @@
         <v>997000</v>
       </c>
     </row>
-    <row r="9" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1</v>
-      </c>
-      <c r="C9" s="2">
-        <v>30</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="E9" s="2">
-        <v>240</v>
-      </c>
-      <c r="F9" s="2">
-        <v>3000</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H9" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="I9" s="2">
-        <v>18</v>
-      </c>
-      <c r="J9" s="2">
-        <v>110</v>
-      </c>
-      <c r="K9" s="2">
-        <v>1200</v>
-      </c>
-      <c r="L9" s="2">
-        <v>750</v>
-      </c>
-      <c r="M9" s="2">
-        <v>8000</v>
-      </c>
-      <c r="N9" s="2">
-        <v>120</v>
-      </c>
-      <c r="O9" s="2">
-        <v>4500</v>
-      </c>
-      <c r="P9" s="2">
-        <v>1500</v>
-      </c>
-      <c r="Q9" s="2">
-        <v>400</v>
-      </c>
-      <c r="R9" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="S9" s="2">
-        <v>200</v>
-      </c>
-      <c r="T9" s="2">
-        <v>140</v>
-      </c>
-      <c r="U9" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="V9" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="W9" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="X9" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="Y9" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="Z9" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AA9" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AB9" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AC9" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AD9">
-        <v>87</v>
-      </c>
-      <c r="AE9">
-        <v>425</v>
-      </c>
-      <c r="AF9">
-        <v>997000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="D10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="D9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
@@ -7567,9 +7468,6 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7580,8 +7478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{472A4E84-05F6-482F-94AF-2C8CE149BF8E}">
   <dimension ref="A1:AP59"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8310,7 +8208,7 @@
         <v>365</v>
       </c>
       <c r="Y6">
-        <v>20200</v>
+        <v>20000</v>
       </c>
       <c r="Z6">
         <v>800</v>
@@ -8322,7 +8220,7 @@
         <v>1200</v>
       </c>
       <c r="AC6">
-        <v>27</v>
+        <v>700</v>
       </c>
       <c r="AD6">
         <v>0.1</v>
@@ -8875,6 +8773,18 @@
       <c r="AP10" s="1">
         <v>425</v>
       </c>
+    </row>
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="J12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AE12" s="1"/>
+      <c r="AG12" s="1"/>
+      <c r="AI12" s="1"/>
+      <c r="AK12" s="1"/>
+      <c r="AL12" s="1"/>
+      <c r="AM12" s="1"/>
+      <c r="AN12" s="1"/>
+      <c r="AO12" s="1"/>
     </row>
     <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="D13" s="1"/>
@@ -13314,8 +13224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC5318B9-9FE8-4735-97AC-C84ECA362166}">
   <dimension ref="A1:AE15"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:R7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13417,7 +13327,7 @@
         <v>59</v>
       </c>
       <c r="B2">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="C2">
         <v>25</v>
@@ -13426,16 +13336,16 @@
         <v>0.01</v>
       </c>
       <c r="E2">
-        <v>6</v>
+        <v>0.5</v>
       </c>
       <c r="F2">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="G2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="I2">
         <v>18</v>
@@ -13453,7 +13363,7 @@
         <v>3000</v>
       </c>
       <c r="N2">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="O2">
         <v>2500</v>
@@ -13462,10 +13372,10 @@
         <v>2000</v>
       </c>
       <c r="Q2">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="R2">
-        <v>65</v>
+        <v>120</v>
       </c>
       <c r="S2">
         <v>270</v>
@@ -13512,7 +13422,7 @@
         <v>60</v>
       </c>
       <c r="B3">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>25</v>
@@ -13521,16 +13431,16 @@
         <v>25</v>
       </c>
       <c r="E3">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="F3">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I3">
         <v>18</v>
@@ -13557,10 +13467,10 @@
         <v>700</v>
       </c>
       <c r="Q3">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="R3">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="S3">
         <v>100</v>
@@ -13607,7 +13517,7 @@
         <v>61</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="C4">
         <v>25</v>
@@ -13616,7 +13526,7 @@
         <v>6</v>
       </c>
       <c r="E4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4">
         <v>7</v>
@@ -13625,7 +13535,7 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="I4">
         <v>18</v>
@@ -13652,7 +13562,7 @@
         <v>600</v>
       </c>
       <c r="Q4">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="R4">
         <v>20</v>
@@ -13711,7 +13621,7 @@
         <v>5</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5">
         <v>5</v>
@@ -13720,7 +13630,7 @@
         <v>0.5</v>
       </c>
       <c r="H5">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="I5">
         <v>18</v>
@@ -13747,10 +13657,10 @@
         <v>600</v>
       </c>
       <c r="Q5">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="R5">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="S5">
         <v>80</v>
@@ -13806,7 +13716,7 @@
         <v>2</v>
       </c>
       <c r="E6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6">
         <v>2</v>
@@ -13815,7 +13725,7 @@
         <v>0.4</v>
       </c>
       <c r="H6">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="I6">
         <v>18</v>
@@ -13842,7 +13752,7 @@
         <v>600</v>
       </c>
       <c r="Q6">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="R6">
         <v>5</v>
@@ -13901,16 +13811,16 @@
         <v>0.5</v>
       </c>
       <c r="E7">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <v>0.4</v>
       </c>
       <c r="H7">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="I7">
         <v>18</v>
@@ -13937,7 +13847,7 @@
         <v>600</v>
       </c>
       <c r="Q7">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="R7">
         <v>1</v>

</xml_diff>

<commit_message>
H1 converged to steady state
</commit_message>
<xml_diff>
--- a/exposan/werf/data/initial_conditions.xlsx
+++ b/exposan/werf/data/initial_conditions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joy_c\Dropbox\PhD\Research\QSD\codes_developing\EXPOsan\exposan\werf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FA3BAD-0A55-4DAC-90C9-49674D3246D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262FCC02-A93D-49A1-B115-C373286718E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23133" yWindow="-93" windowWidth="23226" windowHeight="13866" firstSheet="5" activeTab="17" xr2:uid="{218DD762-44D5-4240-B5CB-C558EBE30BA7}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" firstSheet="5" activeTab="10" xr2:uid="{218DD762-44D5-4240-B5CB-C558EBE30BA7}"/>
   </bookViews>
   <sheets>
     <sheet name="B1" sheetId="6" r:id="rId1"/>
@@ -23,14 +23,13 @@
     <sheet name="G1" sheetId="12" r:id="rId8"/>
     <sheet name="G2" sheetId="13" r:id="rId9"/>
     <sheet name="G3" sheetId="14" r:id="rId10"/>
-    <sheet name="H1" sheetId="22" r:id="rId11"/>
-    <sheet name="H" sheetId="24" r:id="rId12"/>
-    <sheet name="I1" sheetId="17" r:id="rId13"/>
-    <sheet name="I2" sheetId="16" r:id="rId14"/>
-    <sheet name="I3" sheetId="18" r:id="rId15"/>
-    <sheet name="N1" sheetId="19" r:id="rId16"/>
-    <sheet name="AED" sheetId="10" r:id="rId17"/>
-    <sheet name="adm" sheetId="2" r:id="rId18"/>
+    <sheet name="H1" sheetId="24" r:id="rId11"/>
+    <sheet name="I1" sheetId="17" r:id="rId12"/>
+    <sheet name="I2" sheetId="16" r:id="rId13"/>
+    <sheet name="I3" sheetId="18" r:id="rId14"/>
+    <sheet name="N1" sheetId="19" r:id="rId15"/>
+    <sheet name="AED" sheetId="10" r:id="rId16"/>
+    <sheet name="adm" sheetId="2" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="76">
   <si>
     <t>S_O2</t>
   </si>
@@ -280,9 +279,6 @@
     <t>F1</t>
   </si>
   <si>
-    <t>H</t>
-  </si>
-  <si>
     <t>N2</t>
   </si>
 </sst>
@@ -325,9 +321,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2047,11 +2044,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED027A3C-A3AE-4576-A4DA-71233CC9AAA8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC57E7B5-9D7C-460D-9380-266229D6CBEE}">
   <dimension ref="A1:AF21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2160,31 +2157,31 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>16</v>
       </c>
       <c r="D2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>4</v>
+        <v>0.1</v>
       </c>
       <c r="F2">
-        <v>0.28000000000000003</v>
+        <v>5</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="H2">
-        <v>1.7</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <v>15</v>
       </c>
       <c r="J2">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K2">
         <v>28</v>
@@ -2193,49 +2190,49 @@
         <v>50</v>
       </c>
       <c r="M2">
-        <v>1400</v>
+        <v>1000</v>
       </c>
       <c r="N2">
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="O2">
-        <v>1450</v>
-      </c>
-      <c r="P2" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="R2" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>500</v>
+      </c>
+      <c r="P2">
+        <v>100</v>
+      </c>
+      <c r="Q2">
+        <v>100</v>
+      </c>
+      <c r="R2">
+        <v>10</v>
       </c>
       <c r="S2">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="T2">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="U2" s="1">
         <v>1E-8</v>
       </c>
-      <c r="V2">
-        <v>2.2799999999999998</v>
+      <c r="V2" s="1">
+        <v>3</v>
       </c>
       <c r="W2" s="1">
         <v>1E-8</v>
       </c>
-      <c r="X2">
-        <v>154</v>
+      <c r="X2" s="1">
+        <v>2.6</v>
       </c>
       <c r="Y2" s="1">
         <v>1E-8</v>
       </c>
       <c r="Z2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA2">
-        <v>195</v>
+        <v>1E-8</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>100</v>
       </c>
       <c r="AB2" s="1">
         <v>1E-8</v>
@@ -2258,31 +2255,31 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2.9999999999999997E-4</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>16</v>
       </c>
       <c r="D3">
-        <v>6.5</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>3</v>
+        <v>0.1</v>
       </c>
       <c r="F3">
-        <v>0.28000000000000003</v>
+        <v>5</v>
       </c>
       <c r="G3">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="H3">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="I3">
         <v>15</v>
       </c>
       <c r="J3">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K3">
         <v>28</v>
@@ -2291,49 +2288,49 @@
         <v>50</v>
       </c>
       <c r="M3">
-        <v>1400</v>
+        <v>1000</v>
       </c>
       <c r="N3">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="O3">
-        <v>1450</v>
-      </c>
-      <c r="P3" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="R3" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>500</v>
+      </c>
+      <c r="P3">
+        <v>100</v>
+      </c>
+      <c r="Q3">
+        <v>100</v>
+      </c>
+      <c r="R3">
+        <v>10</v>
       </c>
       <c r="S3">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="T3">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="U3" s="1">
         <v>1E-8</v>
       </c>
-      <c r="V3">
-        <v>2.2799999999999998</v>
+      <c r="V3" s="1">
+        <v>3</v>
       </c>
       <c r="W3" s="1">
         <v>1E-8</v>
       </c>
-      <c r="X3">
-        <v>154</v>
+      <c r="X3" s="1">
+        <v>2.6</v>
       </c>
       <c r="Y3" s="1">
         <v>1E-8</v>
       </c>
       <c r="Z3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA3">
-        <v>195</v>
+        <v>1E-8</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>100</v>
       </c>
       <c r="AB3" s="1">
         <v>1E-8</v>
@@ -2362,25 +2359,25 @@
         <v>16</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>8</v>
+        <v>0.1</v>
       </c>
       <c r="F4">
-        <v>0.28000000000000003</v>
+        <v>5</v>
       </c>
       <c r="G4">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="H4">
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="I4">
         <v>15</v>
       </c>
       <c r="J4">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="K4">
         <v>28</v>
@@ -2389,49 +2386,49 @@
         <v>50</v>
       </c>
       <c r="M4">
-        <v>1400</v>
+        <v>1000</v>
       </c>
       <c r="N4">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="O4">
-        <v>1450</v>
-      </c>
-      <c r="P4" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="R4" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>500</v>
+      </c>
+      <c r="P4">
+        <v>100</v>
+      </c>
+      <c r="Q4">
+        <v>100</v>
+      </c>
+      <c r="R4">
+        <v>10</v>
       </c>
       <c r="S4">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="T4">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="U4" s="1">
         <v>1E-8</v>
       </c>
-      <c r="V4">
-        <v>2.2799999999999998</v>
+      <c r="V4" s="1">
+        <v>3</v>
       </c>
       <c r="W4" s="1">
         <v>1E-8</v>
       </c>
-      <c r="X4">
-        <v>154</v>
+      <c r="X4" s="1">
+        <v>2.6</v>
       </c>
       <c r="Y4" s="1">
         <v>1E-8</v>
       </c>
       <c r="Z4" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA4">
-        <v>195</v>
+        <v>1E-8</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>100</v>
       </c>
       <c r="AB4" s="1">
         <v>1E-8</v>
@@ -2460,25 +2457,25 @@
         <v>16</v>
       </c>
       <c r="D5">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>9</v>
+        <v>0.1</v>
       </c>
       <c r="F5">
-        <v>0.28000000000000003</v>
+        <v>5</v>
       </c>
       <c r="G5">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="H5">
-        <v>0.02</v>
+        <v>1</v>
       </c>
       <c r="I5">
         <v>15</v>
       </c>
       <c r="J5">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="K5">
         <v>28</v>
@@ -2487,49 +2484,49 @@
         <v>50</v>
       </c>
       <c r="M5">
-        <v>1400</v>
+        <v>1000</v>
       </c>
       <c r="N5">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="O5">
-        <v>1450</v>
-      </c>
-      <c r="P5" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="R5" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>500</v>
+      </c>
+      <c r="P5">
+        <v>100</v>
+      </c>
+      <c r="Q5">
+        <v>100</v>
+      </c>
+      <c r="R5">
+        <v>10</v>
       </c>
       <c r="S5">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="T5">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="U5" s="1">
         <v>1E-8</v>
       </c>
-      <c r="V5">
-        <v>2.2799999999999998</v>
+      <c r="V5" s="1">
+        <v>3</v>
       </c>
       <c r="W5" s="1">
         <v>1E-8</v>
       </c>
-      <c r="X5">
-        <v>154</v>
+      <c r="X5" s="1">
+        <v>2.6</v>
       </c>
       <c r="Y5" s="1">
         <v>1E-8</v>
       </c>
       <c r="Z5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA5">
-        <v>195</v>
+        <v>1E-8</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>100</v>
       </c>
       <c r="AB5" s="1">
         <v>1E-8</v>
@@ -2552,31 +2549,31 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>16</v>
       </c>
       <c r="D6">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>8</v>
+        <v>0.1</v>
       </c>
       <c r="F6">
-        <v>0.28000000000000003</v>
+        <v>5</v>
       </c>
       <c r="G6">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="H6">
-        <v>0.04</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <v>15</v>
       </c>
       <c r="J6">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="K6">
         <v>28</v>
@@ -2585,49 +2582,49 @@
         <v>50</v>
       </c>
       <c r="M6">
-        <v>1400</v>
+        <v>1000</v>
       </c>
       <c r="N6">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="O6">
-        <v>1450</v>
-      </c>
-      <c r="P6" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="R6" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>500</v>
+      </c>
+      <c r="P6">
+        <v>100</v>
+      </c>
+      <c r="Q6">
+        <v>100</v>
+      </c>
+      <c r="R6">
+        <v>10</v>
       </c>
       <c r="S6">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="T6">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="U6" s="1">
         <v>1E-8</v>
       </c>
-      <c r="V6">
-        <v>2.2799999999999998</v>
+      <c r="V6" s="1">
+        <v>3</v>
       </c>
       <c r="W6" s="1">
         <v>1E-8</v>
       </c>
-      <c r="X6">
-        <v>154</v>
+      <c r="X6" s="1">
+        <v>2.6</v>
       </c>
       <c r="Y6" s="1">
         <v>1E-8</v>
       </c>
       <c r="Z6" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA6">
-        <v>195</v>
+        <v>1E-8</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>100</v>
       </c>
       <c r="AB6" s="1">
         <v>1E-8</v>
@@ -2656,25 +2653,25 @@
         <v>16</v>
       </c>
       <c r="D7">
-        <v>0.15</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>8.5</v>
+        <v>0.1</v>
       </c>
       <c r="F7">
-        <v>0.28000000000000003</v>
+        <v>5</v>
       </c>
       <c r="G7">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="H7">
-        <v>0.02</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <v>15</v>
       </c>
       <c r="J7">
-        <v>6.5</v>
+        <v>30</v>
       </c>
       <c r="K7">
         <v>28</v>
@@ -2683,49 +2680,49 @@
         <v>50</v>
       </c>
       <c r="M7">
-        <v>1400</v>
+        <v>1000</v>
       </c>
       <c r="N7">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="O7">
-        <v>1450</v>
-      </c>
-      <c r="P7" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="R7" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>500</v>
+      </c>
+      <c r="P7">
+        <v>100</v>
+      </c>
+      <c r="Q7">
+        <v>100</v>
+      </c>
+      <c r="R7">
+        <v>10</v>
       </c>
       <c r="S7">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="T7">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="U7" s="1">
         <v>1E-8</v>
       </c>
-      <c r="V7">
-        <v>2.2799999999999998</v>
+      <c r="V7" s="1">
+        <v>3</v>
       </c>
       <c r="W7" s="1">
         <v>1E-8</v>
       </c>
-      <c r="X7">
-        <v>154</v>
+      <c r="X7" s="1">
+        <v>2.6</v>
       </c>
       <c r="Y7" s="1">
         <v>1E-8</v>
       </c>
       <c r="Z7" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA7">
-        <v>195</v>
+        <v>1E-8</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>100</v>
       </c>
       <c r="AB7" s="1">
         <v>1E-8</v>
@@ -2744,6 +2741,7 @@
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="P10" s="1"/>
       <c r="U10" s="1"/>
       <c r="W10" s="1"/>
       <c r="Y10" s="1"/>
@@ -2753,6 +2751,7 @@
       <c r="AC10" s="1"/>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="P11" s="1"/>
       <c r="U11" s="1"/>
       <c r="W11" s="1"/>
       <c r="Y11" s="1"/>
@@ -2762,6 +2761,7 @@
       <c r="AC11" s="1"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="P12" s="1"/>
       <c r="R12" s="1"/>
       <c r="U12" s="1"/>
       <c r="W12" s="1"/>
@@ -2772,6 +2772,7 @@
       <c r="AC12" s="1"/>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="P13" s="1"/>
       <c r="R13" s="1"/>
       <c r="U13" s="1"/>
       <c r="W13" s="1"/>
@@ -2782,6 +2783,7 @@
       <c r="AC13" s="1"/>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="P14" s="1"/>
       <c r="R14" s="1"/>
       <c r="U14" s="1"/>
       <c r="W14" s="1"/>
@@ -2792,6 +2794,7 @@
       <c r="AC14" s="1"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="P15" s="1"/>
       <c r="R15" s="1"/>
       <c r="U15" s="1"/>
       <c r="W15" s="1"/>
@@ -2802,6 +2805,7 @@
       <c r="AC15" s="1"/>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="P16" s="1"/>
       <c r="U16" s="1"/>
       <c r="W16" s="1"/>
       <c r="Y16" s="1"/>
@@ -2852,811 +2856,6 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC57E7B5-9D7C-460D-9380-266229D6CBEE}">
-  <dimension ref="A1:AF21"/>
-  <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="16" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" t="s">
-        <v>47</v>
-      </c>
-      <c r="V1" t="s">
-        <v>43</v>
-      </c>
-      <c r="W1" t="s">
-        <v>49</v>
-      </c>
-      <c r="X1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>16</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>0.1</v>
-      </c>
-      <c r="F2">
-        <v>5</v>
-      </c>
-      <c r="G2">
-        <v>0.1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>15</v>
-      </c>
-      <c r="J2">
-        <v>30</v>
-      </c>
-      <c r="K2">
-        <v>28</v>
-      </c>
-      <c r="L2">
-        <v>50</v>
-      </c>
-      <c r="M2">
-        <v>1000</v>
-      </c>
-      <c r="N2">
-        <v>100</v>
-      </c>
-      <c r="O2">
-        <v>500</v>
-      </c>
-      <c r="P2">
-        <v>100</v>
-      </c>
-      <c r="Q2">
-        <v>100</v>
-      </c>
-      <c r="R2">
-        <v>10</v>
-      </c>
-      <c r="S2">
-        <v>100</v>
-      </c>
-      <c r="T2">
-        <v>140</v>
-      </c>
-      <c r="U2" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="V2" s="1">
-        <v>3</v>
-      </c>
-      <c r="W2" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="X2" s="1">
-        <v>2.6</v>
-      </c>
-      <c r="Y2" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="Z2" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AA2" s="1">
-        <v>100</v>
-      </c>
-      <c r="AB2" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AC2" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AD2">
-        <v>87</v>
-      </c>
-      <c r="AE2">
-        <v>425</v>
-      </c>
-      <c r="AF2">
-        <v>996640</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>16</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>0.1</v>
-      </c>
-      <c r="F3">
-        <v>5</v>
-      </c>
-      <c r="G3">
-        <v>0.1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>15</v>
-      </c>
-      <c r="J3">
-        <v>30</v>
-      </c>
-      <c r="K3">
-        <v>28</v>
-      </c>
-      <c r="L3">
-        <v>50</v>
-      </c>
-      <c r="M3">
-        <v>1000</v>
-      </c>
-      <c r="N3">
-        <v>100</v>
-      </c>
-      <c r="O3">
-        <v>500</v>
-      </c>
-      <c r="P3">
-        <v>100</v>
-      </c>
-      <c r="Q3">
-        <v>100</v>
-      </c>
-      <c r="R3">
-        <v>10</v>
-      </c>
-      <c r="S3">
-        <v>100</v>
-      </c>
-      <c r="T3">
-        <v>140</v>
-      </c>
-      <c r="U3" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="V3" s="1">
-        <v>3</v>
-      </c>
-      <c r="W3" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="X3" s="1">
-        <v>2.6</v>
-      </c>
-      <c r="Y3" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="Z3" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AA3" s="1">
-        <v>100</v>
-      </c>
-      <c r="AB3" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AC3" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AD3">
-        <v>87</v>
-      </c>
-      <c r="AE3">
-        <v>425</v>
-      </c>
-      <c r="AF3">
-        <v>996640</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>16</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>0.1</v>
-      </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
-      <c r="G4">
-        <v>0.1</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>15</v>
-      </c>
-      <c r="J4">
-        <v>30</v>
-      </c>
-      <c r="K4">
-        <v>28</v>
-      </c>
-      <c r="L4">
-        <v>50</v>
-      </c>
-      <c r="M4">
-        <v>1000</v>
-      </c>
-      <c r="N4">
-        <v>100</v>
-      </c>
-      <c r="O4">
-        <v>500</v>
-      </c>
-      <c r="P4">
-        <v>100</v>
-      </c>
-      <c r="Q4">
-        <v>100</v>
-      </c>
-      <c r="R4">
-        <v>10</v>
-      </c>
-      <c r="S4">
-        <v>100</v>
-      </c>
-      <c r="T4">
-        <v>140</v>
-      </c>
-      <c r="U4" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="V4" s="1">
-        <v>3</v>
-      </c>
-      <c r="W4" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="X4" s="1">
-        <v>2.6</v>
-      </c>
-      <c r="Y4" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="Z4" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AA4" s="1">
-        <v>100</v>
-      </c>
-      <c r="AB4" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AC4" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AD4">
-        <v>87</v>
-      </c>
-      <c r="AE4">
-        <v>425</v>
-      </c>
-      <c r="AF4">
-        <v>996640</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>16</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>0.1</v>
-      </c>
-      <c r="F5">
-        <v>5</v>
-      </c>
-      <c r="G5">
-        <v>0.1</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>15</v>
-      </c>
-      <c r="J5">
-        <v>30</v>
-      </c>
-      <c r="K5">
-        <v>28</v>
-      </c>
-      <c r="L5">
-        <v>50</v>
-      </c>
-      <c r="M5">
-        <v>1000</v>
-      </c>
-      <c r="N5">
-        <v>100</v>
-      </c>
-      <c r="O5">
-        <v>500</v>
-      </c>
-      <c r="P5">
-        <v>100</v>
-      </c>
-      <c r="Q5">
-        <v>100</v>
-      </c>
-      <c r="R5">
-        <v>10</v>
-      </c>
-      <c r="S5">
-        <v>100</v>
-      </c>
-      <c r="T5">
-        <v>140</v>
-      </c>
-      <c r="U5" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="V5" s="1">
-        <v>3</v>
-      </c>
-      <c r="W5" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="X5" s="1">
-        <v>2.6</v>
-      </c>
-      <c r="Y5" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="Z5" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AA5" s="1">
-        <v>100</v>
-      </c>
-      <c r="AB5" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AC5" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AD5">
-        <v>87</v>
-      </c>
-      <c r="AE5">
-        <v>425</v>
-      </c>
-      <c r="AF5">
-        <v>996640</v>
-      </c>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>16</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>0.1</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="G6">
-        <v>0.1</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>15</v>
-      </c>
-      <c r="J6">
-        <v>30</v>
-      </c>
-      <c r="K6">
-        <v>28</v>
-      </c>
-      <c r="L6">
-        <v>50</v>
-      </c>
-      <c r="M6">
-        <v>1000</v>
-      </c>
-      <c r="N6">
-        <v>100</v>
-      </c>
-      <c r="O6">
-        <v>500</v>
-      </c>
-      <c r="P6">
-        <v>100</v>
-      </c>
-      <c r="Q6">
-        <v>100</v>
-      </c>
-      <c r="R6">
-        <v>10</v>
-      </c>
-      <c r="S6">
-        <v>100</v>
-      </c>
-      <c r="T6">
-        <v>140</v>
-      </c>
-      <c r="U6" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="V6" s="1">
-        <v>3</v>
-      </c>
-      <c r="W6" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="X6" s="1">
-        <v>2.6</v>
-      </c>
-      <c r="Y6" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="Z6" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AA6" s="1">
-        <v>100</v>
-      </c>
-      <c r="AB6" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AC6" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AD6">
-        <v>87</v>
-      </c>
-      <c r="AE6">
-        <v>425</v>
-      </c>
-      <c r="AF6">
-        <v>996640</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>16</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>0.1</v>
-      </c>
-      <c r="F7">
-        <v>5</v>
-      </c>
-      <c r="G7">
-        <v>0.1</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>15</v>
-      </c>
-      <c r="J7">
-        <v>30</v>
-      </c>
-      <c r="K7">
-        <v>28</v>
-      </c>
-      <c r="L7">
-        <v>50</v>
-      </c>
-      <c r="M7">
-        <v>1000</v>
-      </c>
-      <c r="N7">
-        <v>100</v>
-      </c>
-      <c r="O7">
-        <v>500</v>
-      </c>
-      <c r="P7">
-        <v>100</v>
-      </c>
-      <c r="Q7">
-        <v>100</v>
-      </c>
-      <c r="R7">
-        <v>10</v>
-      </c>
-      <c r="S7">
-        <v>100</v>
-      </c>
-      <c r="T7">
-        <v>140</v>
-      </c>
-      <c r="U7" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="V7" s="1">
-        <v>3</v>
-      </c>
-      <c r="W7" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="X7" s="1">
-        <v>2.6</v>
-      </c>
-      <c r="Y7" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="Z7" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AA7" s="1">
-        <v>100</v>
-      </c>
-      <c r="AB7" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AC7" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AD7">
-        <v>87</v>
-      </c>
-      <c r="AE7">
-        <v>425</v>
-      </c>
-      <c r="AF7">
-        <v>996640</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="U10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
-      <c r="AC10" s="1"/>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="U11" s="1"/>
-      <c r="W11" s="1"/>
-      <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
-      <c r="AA11" s="1"/>
-      <c r="AB11" s="1"/>
-      <c r="AC11" s="1"/>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="R12" s="1"/>
-      <c r="U12" s="1"/>
-      <c r="W12" s="1"/>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
-      <c r="AA12" s="1"/>
-      <c r="AB12" s="1"/>
-      <c r="AC12" s="1"/>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="R13" s="1"/>
-      <c r="U13" s="1"/>
-      <c r="W13" s="1"/>
-      <c r="Y13" s="1"/>
-      <c r="Z13" s="1"/>
-      <c r="AA13" s="1"/>
-      <c r="AB13" s="1"/>
-      <c r="AC13" s="1"/>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="R14" s="1"/>
-      <c r="U14" s="1"/>
-      <c r="W14" s="1"/>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
-      <c r="AA14" s="1"/>
-      <c r="AB14" s="1"/>
-      <c r="AC14" s="1"/>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="R15" s="1"/>
-      <c r="U15" s="1"/>
-      <c r="W15" s="1"/>
-      <c r="Y15" s="1"/>
-      <c r="Z15" s="1"/>
-      <c r="AA15" s="1"/>
-      <c r="AB15" s="1"/>
-      <c r="AC15" s="1"/>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="U16" s="1"/>
-      <c r="W16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
-      <c r="AA16" s="1"/>
-      <c r="AB16" s="1"/>
-      <c r="AC16" s="1"/>
-    </row>
-    <row r="17" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="1"/>
-      <c r="AA17" s="1"/>
-      <c r="AB17" s="1"/>
-      <c r="AC17" s="1"/>
-    </row>
-    <row r="18" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="Y18" s="1"/>
-      <c r="Z18" s="1"/>
-      <c r="AA18" s="1"/>
-      <c r="AB18" s="1"/>
-      <c r="AC18" s="1"/>
-    </row>
-    <row r="19" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R19" s="1"/>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="1"/>
-      <c r="AA19" s="1"/>
-      <c r="AB19" s="1"/>
-      <c r="AC19" s="1"/>
-    </row>
-    <row r="20" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="Y20" s="1"/>
-      <c r="Z20" s="1"/>
-      <c r="AA20" s="1"/>
-      <c r="AB20" s="1"/>
-      <c r="AC20" s="1"/>
-    </row>
-    <row r="21" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="Y21" s="1"/>
-      <c r="Z21" s="1"/>
-      <c r="AA21" s="1"/>
-      <c r="AB21" s="1"/>
-      <c r="AC21" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D7FEF2-86A6-4650-A253-23D719FC805E}">
   <dimension ref="A1:AE21"/>
   <sheetViews>
@@ -4428,7 +3627,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E4487D-883D-4E85-B2E5-7356A39B3F61}">
   <dimension ref="A1:AE21"/>
   <sheetViews>
@@ -5152,7 +4351,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42016BA4-57DB-462D-9767-837B2F986A82}">
   <dimension ref="A1:AE16"/>
   <sheetViews>
@@ -5889,7 +5088,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12367F69-A662-4BD3-AE36-01641D10E752}">
   <dimension ref="A1:AE16"/>
   <sheetViews>
@@ -6630,7 +5829,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CB7F0C9-B54B-4F93-93CE-9E10B0EA4FF3}">
   <dimension ref="A1:AF35"/>
   <sheetViews>
@@ -7331,7 +6530,7 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -7474,12 +6673,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{472A4E84-05F6-482F-94AF-2C8CE149BF8E}">
-  <dimension ref="A1:AP59"/>
+  <dimension ref="A1:AQ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7497,7 +6696,7 @@
     <col min="47" max="47" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>21</v>
       </c>
@@ -7621,8 +6820,11 @@
       <c r="AP1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AQ1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -7749,8 +6951,11 @@
       <c r="AP2">
         <v>425</v>
       </c>
-    </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AQ2" s="2">
+        <v>997000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -7877,8 +7082,11 @@
       <c r="AP3">
         <v>425</v>
       </c>
-    </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AQ3" s="2">
+        <v>997000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -8005,8 +7213,11 @@
       <c r="AP4">
         <v>425</v>
       </c>
-    </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AQ4" s="2">
+        <v>997000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>74</v>
       </c>
@@ -8133,8 +7344,11 @@
       <c r="AP5">
         <v>424</v>
       </c>
-    </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AQ5" s="2">
+        <v>997000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>63</v>
       </c>
@@ -8261,8 +7475,11 @@
       <c r="AP6">
         <v>425</v>
       </c>
-    </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AQ6" s="2">
+        <v>997000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>73</v>
       </c>
@@ -8285,112 +7502,115 @@
         <v>14</v>
       </c>
       <c r="H7">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I7">
-        <v>1E-4</v>
+        <v>2.03E-4</v>
       </c>
       <c r="J7">
-        <v>180</v>
-      </c>
-      <c r="K7">
-        <v>915</v>
+        <v>170</v>
+      </c>
+      <c r="K7" s="2">
+        <v>900</v>
       </c>
       <c r="L7">
-        <v>1560</v>
+        <v>1460</v>
       </c>
       <c r="M7">
-        <v>200</v>
+        <v>230</v>
       </c>
       <c r="N7">
         <v>16</v>
       </c>
       <c r="O7">
-        <v>46</v>
+        <v>1300</v>
       </c>
       <c r="P7">
-        <v>49</v>
+        <v>1400</v>
       </c>
       <c r="Q7">
-        <v>65</v>
+        <v>2000</v>
       </c>
       <c r="R7">
-        <v>830</v>
+        <v>700</v>
       </c>
       <c r="S7">
-        <v>660</v>
+        <v>600</v>
       </c>
       <c r="T7">
-        <v>630</v>
+        <v>560</v>
       </c>
       <c r="U7">
-        <v>280</v>
+        <v>250</v>
       </c>
       <c r="V7">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="W7">
-        <v>870</v>
+        <v>750</v>
       </c>
       <c r="X7">
-        <v>420</v>
+        <v>350</v>
       </c>
       <c r="Y7">
-        <v>23760</v>
-      </c>
-      <c r="Z7" s="1">
-        <v>1E-8</v>
+        <v>23700</v>
+      </c>
+      <c r="Z7">
+        <v>0.5</v>
       </c>
       <c r="AA7" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AB7" s="1">
-        <v>1E-8</v>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AB7">
+        <v>0.5</v>
       </c>
       <c r="AC7">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="AD7">
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="AE7">
         <v>2</v>
       </c>
       <c r="AF7" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="AG7">
-        <v>540</v>
+        <v>700</v>
       </c>
       <c r="AH7" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="AI7">
-        <v>1700</v>
+        <v>560</v>
       </c>
       <c r="AJ7" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AK7" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="AK7">
+        <v>40</v>
       </c>
       <c r="AL7" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>3200</v>
       </c>
       <c r="AM7" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="AN7" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AO7">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="AO7" s="2">
         <v>87</v>
       </c>
-      <c r="AP7">
+      <c r="AP7" s="2">
         <v>425</v>
       </c>
-    </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AQ7" s="2">
+        <v>997000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>71</v>
       </c>
@@ -8517,8 +7737,11 @@
       <c r="AP8">
         <v>425</v>
       </c>
-    </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AQ8" s="2">
+        <v>997000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>72</v>
       </c>
@@ -8645,159 +7868,51 @@
       <c r="AP9">
         <v>425</v>
       </c>
-    </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>75</v>
-      </c>
-      <c r="B10">
-        <v>10</v>
-      </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10">
-        <v>83</v>
-      </c>
-      <c r="E10">
-        <v>9</v>
-      </c>
-      <c r="F10">
-        <v>12</v>
-      </c>
-      <c r="G10">
-        <v>14</v>
-      </c>
-      <c r="H10">
-        <v>50</v>
-      </c>
-      <c r="I10">
-        <v>2.03E-4</v>
-      </c>
-      <c r="J10">
-        <v>170</v>
-      </c>
-      <c r="K10" s="1">
-        <v>900</v>
-      </c>
-      <c r="L10">
-        <v>1460</v>
-      </c>
-      <c r="M10">
-        <v>230</v>
-      </c>
-      <c r="N10">
-        <v>16</v>
-      </c>
-      <c r="O10">
-        <v>1300</v>
-      </c>
-      <c r="P10">
-        <v>1400</v>
-      </c>
-      <c r="Q10">
-        <v>2000</v>
-      </c>
-      <c r="R10">
-        <v>700</v>
-      </c>
-      <c r="S10">
-        <v>600</v>
-      </c>
-      <c r="T10">
-        <v>560</v>
-      </c>
-      <c r="U10">
-        <v>250</v>
-      </c>
-      <c r="V10">
-        <v>120</v>
-      </c>
-      <c r="W10">
-        <v>750</v>
-      </c>
-      <c r="X10">
-        <v>350</v>
-      </c>
-      <c r="Y10">
-        <v>23700</v>
-      </c>
-      <c r="Z10">
-        <v>0.5</v>
-      </c>
-      <c r="AA10" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="AB10">
-        <v>0.5</v>
-      </c>
-      <c r="AC10">
-        <v>50</v>
-      </c>
-      <c r="AD10">
-        <v>0.4</v>
-      </c>
-      <c r="AE10">
-        <v>2</v>
-      </c>
-      <c r="AF10" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="AG10">
-        <v>700</v>
-      </c>
-      <c r="AH10" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="AI10">
-        <v>560</v>
-      </c>
-      <c r="AJ10" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="AK10">
-        <v>40</v>
-      </c>
-      <c r="AL10" s="1">
-        <v>3200</v>
-      </c>
-      <c r="AM10" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="AN10" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="AO10" s="1">
-        <v>87</v>
-      </c>
-      <c r="AP10" s="1">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="J12" s="1"/>
-      <c r="Z12" s="1"/>
-      <c r="AE12" s="1"/>
-      <c r="AG12" s="1"/>
-      <c r="AI12" s="1"/>
-      <c r="AK12" s="1"/>
-      <c r="AL12" s="1"/>
-      <c r="AM12" s="1"/>
-      <c r="AN12" s="1"/>
-      <c r="AO12" s="1"/>
-    </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AQ9" s="2">
+        <v>997000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="K10" s="2"/>
+      <c r="AA10" s="1"/>
+      <c r="AF10" s="1"/>
+      <c r="AH10" s="1"/>
+      <c r="AJ10" s="1"/>
+      <c r="AL10" s="1"/>
+      <c r="AM10" s="1"/>
+      <c r="AN10" s="1"/>
+      <c r="AO10" s="2"/>
+      <c r="AP10" s="2"/>
+      <c r="AQ10" s="2"/>
+    </row>
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="J11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AE11" s="1"/>
+      <c r="AG11" s="1"/>
+      <c r="AI11" s="1"/>
+      <c r="AK11" s="1"/>
+      <c r="AL11" s="1"/>
+      <c r="AM11" s="1"/>
+      <c r="AN11" s="1"/>
+      <c r="AO11" s="1"/>
+    </row>
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="D16" s="1"/>
     </row>
@@ -8814,11 +7929,11 @@
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="D21" s="1"/>
     </row>
@@ -8879,11 +7994,11 @@
       <c r="D35" s="1"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="D36" s="1"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="D37" s="1"/>
     </row>
@@ -8900,33 +8015,34 @@
       <c r="D40" s="1"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="D41" s="1"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="D42" s="1"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="D43" s="1"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="D44" s="1"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="D45" s="1"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="D46" s="1"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="D47" s="1"/>
     </row>
@@ -8951,7 +8067,6 @@
       <c r="D51" s="1"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="D52" s="1"/>
     </row>
@@ -8969,16 +8084,12 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
-      <c r="D56" s="1"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B59" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
consistent PAO kinetics across BNR configs
</commit_message>
<xml_diff>
--- a/exposan/werf/data/initial_conditions.xlsx
+++ b/exposan/werf/data/initial_conditions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joy_c\Dropbox\PhD\Research\QSD\codes_developing\EXPOsan\exposan\werf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262FCC02-A93D-49A1-B115-C373286718E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F494E081-167F-4577-B8F8-079F5BFC52B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" firstSheet="5" activeTab="10" xr2:uid="{218DD762-44D5-4240-B5CB-C558EBE30BA7}"/>
+    <workbookView xWindow="3795" yWindow="5625" windowWidth="19455" windowHeight="13680" firstSheet="5" activeTab="10" xr2:uid="{218DD762-44D5-4240-B5CB-C558EBE30BA7}"/>
   </bookViews>
   <sheets>
     <sheet name="B1" sheetId="6" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="76">
   <si>
     <t>S_O2</t>
   </si>
@@ -321,10 +321,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1339,37 +1338,12 @@
   <dimension ref="A1:AE11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="29" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="31" width="9.5703125" customWidth="1"/>
     <col min="32" max="33" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1479,10 +1453,10 @@
         <v>0.01</v>
       </c>
       <c r="E2">
-        <v>1.5</v>
+        <v>5</v>
       </c>
       <c r="F2">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="G2">
         <v>2</v>
@@ -1503,16 +1477,16 @@
         <v>50</v>
       </c>
       <c r="M2">
-        <v>3600</v>
+        <v>3000</v>
       </c>
       <c r="N2">
         <v>70</v>
       </c>
       <c r="O2">
-        <v>2400</v>
+        <v>2000</v>
       </c>
       <c r="P2">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="Q2">
         <v>300</v>
@@ -1574,10 +1548,10 @@
         <v>20</v>
       </c>
       <c r="E3">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="F3">
-        <v>0.5</v>
+        <v>20</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -1598,7 +1572,7 @@
         <v>50</v>
       </c>
       <c r="M3">
-        <v>1200</v>
+        <v>1000</v>
       </c>
       <c r="N3">
         <v>60</v>
@@ -1607,7 +1581,7 @@
         <v>1000</v>
       </c>
       <c r="P3">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="Q3">
         <v>80</v>
@@ -1669,10 +1643,10 @@
         <v>5</v>
       </c>
       <c r="E4">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="F4">
-        <v>0.2</v>
+        <v>3</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -1702,7 +1676,7 @@
         <v>800</v>
       </c>
       <c r="P4">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="Q4">
         <v>90</v>
@@ -1764,10 +1738,10 @@
         <v>5</v>
       </c>
       <c r="E5">
-        <v>0.1</v>
+        <v>5</v>
       </c>
       <c r="F5">
-        <v>0.2</v>
+        <v>2</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -1797,7 +1771,7 @@
         <v>800</v>
       </c>
       <c r="P5">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="Q5">
         <v>90</v>
@@ -1859,10 +1833,10 @@
         <v>2</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F6">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <v>0.5</v>
@@ -1892,7 +1866,7 @@
         <v>800</v>
       </c>
       <c r="P6">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="Q6">
         <v>90</v>
@@ -1951,13 +1925,13 @@
         <v>25</v>
       </c>
       <c r="D7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F7">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="G7">
         <v>0.5</v>
@@ -1987,7 +1961,7 @@
         <v>800</v>
       </c>
       <c r="P7">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="Q7">
         <v>90</v>
@@ -2047,8 +2021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC57E7B5-9D7C-460D-9380-266229D6CBEE}">
   <dimension ref="A1:AF21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2166,13 +2140,13 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>0.1</v>
+        <v>8</v>
       </c>
       <c r="F2">
         <v>5</v>
       </c>
       <c r="G2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -2264,13 +2238,13 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>0.1</v>
+        <v>8</v>
       </c>
       <c r="F3">
         <v>5</v>
       </c>
       <c r="G3">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -2362,13 +2336,13 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>0.1</v>
+        <v>8</v>
       </c>
       <c r="F4">
         <v>5</v>
       </c>
       <c r="G4">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -2460,13 +2434,13 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>0.1</v>
+        <v>8</v>
       </c>
       <c r="F5">
         <v>5</v>
       </c>
       <c r="G5">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -2558,13 +2532,13 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>0.1</v>
+        <v>8</v>
       </c>
       <c r="F6">
         <v>5</v>
       </c>
       <c r="G6">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2656,13 +2630,13 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <v>0.1</v>
+        <v>8</v>
       </c>
       <c r="F7">
         <v>5</v>
       </c>
       <c r="G7">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -2857,10 +2831,809 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D7FEF2-86A6-4650-A253-23D719FC805E}">
+  <dimension ref="A1:AF21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="16" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V1" t="s">
+        <v>43</v>
+      </c>
+      <c r="W1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2">
+        <v>1E-3</v>
+      </c>
+      <c r="C2">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>18</v>
+      </c>
+      <c r="E2">
+        <v>0.1</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <v>18</v>
+      </c>
+      <c r="J2">
+        <v>50</v>
+      </c>
+      <c r="K2">
+        <v>28</v>
+      </c>
+      <c r="L2">
+        <v>50</v>
+      </c>
+      <c r="M2">
+        <v>2500</v>
+      </c>
+      <c r="N2">
+        <v>120</v>
+      </c>
+      <c r="O2">
+        <v>1000</v>
+      </c>
+      <c r="P2">
+        <v>300</v>
+      </c>
+      <c r="Q2">
+        <v>50</v>
+      </c>
+      <c r="R2">
+        <v>25</v>
+      </c>
+      <c r="S2">
+        <v>70</v>
+      </c>
+      <c r="T2">
+        <v>130</v>
+      </c>
+      <c r="U2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="V2">
+        <v>10</v>
+      </c>
+      <c r="W2" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AD2">
+        <v>87</v>
+      </c>
+      <c r="AE2">
+        <v>425</v>
+      </c>
+      <c r="AF2">
+        <v>996615.44462133199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3">
+        <v>0.01</v>
+      </c>
+      <c r="C3">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>18</v>
+      </c>
+      <c r="J3">
+        <v>25</v>
+      </c>
+      <c r="K3">
+        <v>28</v>
+      </c>
+      <c r="L3">
+        <v>50</v>
+      </c>
+      <c r="M3">
+        <v>2500</v>
+      </c>
+      <c r="N3">
+        <v>50</v>
+      </c>
+      <c r="O3">
+        <v>1000</v>
+      </c>
+      <c r="P3">
+        <v>300</v>
+      </c>
+      <c r="Q3">
+        <v>50</v>
+      </c>
+      <c r="R3">
+        <v>10</v>
+      </c>
+      <c r="S3">
+        <v>70</v>
+      </c>
+      <c r="T3">
+        <v>130</v>
+      </c>
+      <c r="U3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="V3">
+        <v>10</v>
+      </c>
+      <c r="W3" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AD3">
+        <v>87</v>
+      </c>
+      <c r="AE3">
+        <v>425</v>
+      </c>
+      <c r="AF3">
+        <v>996615.44461688295</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>0.5</v>
+      </c>
+      <c r="H4">
+        <v>0.1</v>
+      </c>
+      <c r="I4">
+        <v>18</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="K4">
+        <v>28</v>
+      </c>
+      <c r="L4">
+        <v>50</v>
+      </c>
+      <c r="M4">
+        <v>2500</v>
+      </c>
+      <c r="N4">
+        <v>35</v>
+      </c>
+      <c r="O4">
+        <v>1000</v>
+      </c>
+      <c r="P4">
+        <v>300</v>
+      </c>
+      <c r="Q4">
+        <v>50</v>
+      </c>
+      <c r="R4">
+        <v>5</v>
+      </c>
+      <c r="S4">
+        <v>70</v>
+      </c>
+      <c r="T4">
+        <v>130</v>
+      </c>
+      <c r="U4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="V4">
+        <v>10</v>
+      </c>
+      <c r="W4" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="X4">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AD4">
+        <v>87</v>
+      </c>
+      <c r="AE4">
+        <v>425</v>
+      </c>
+      <c r="AF4">
+        <v>996615.44461571099</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>0.5</v>
+      </c>
+      <c r="H5">
+        <v>0.1</v>
+      </c>
+      <c r="I5">
+        <v>18</v>
+      </c>
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>28</v>
+      </c>
+      <c r="L5">
+        <v>50</v>
+      </c>
+      <c r="M5">
+        <v>2500</v>
+      </c>
+      <c r="N5">
+        <v>25</v>
+      </c>
+      <c r="O5">
+        <v>1000</v>
+      </c>
+      <c r="P5">
+        <v>300</v>
+      </c>
+      <c r="Q5">
+        <v>50</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>70</v>
+      </c>
+      <c r="T5">
+        <v>130</v>
+      </c>
+      <c r="U5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="V5">
+        <v>10</v>
+      </c>
+      <c r="W5" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AD5">
+        <v>87</v>
+      </c>
+      <c r="AE5">
+        <v>425</v>
+      </c>
+      <c r="AF5">
+        <v>996615.44461530598</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6">
+        <v>0.01</v>
+      </c>
+      <c r="C6">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>0.5</v>
+      </c>
+      <c r="H6">
+        <v>0.1</v>
+      </c>
+      <c r="I6">
+        <v>18</v>
+      </c>
+      <c r="J6">
+        <v>6</v>
+      </c>
+      <c r="K6">
+        <v>28</v>
+      </c>
+      <c r="L6">
+        <v>50</v>
+      </c>
+      <c r="M6">
+        <v>2500</v>
+      </c>
+      <c r="N6">
+        <v>20</v>
+      </c>
+      <c r="O6">
+        <v>1000</v>
+      </c>
+      <c r="P6">
+        <v>300</v>
+      </c>
+      <c r="Q6">
+        <v>50</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>70</v>
+      </c>
+      <c r="T6">
+        <v>130</v>
+      </c>
+      <c r="U6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="V6">
+        <v>10</v>
+      </c>
+      <c r="W6" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AD6">
+        <v>87</v>
+      </c>
+      <c r="AE6">
+        <v>425</v>
+      </c>
+      <c r="AF6">
+        <v>996615.44461224903</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>0.5</v>
+      </c>
+      <c r="H7">
+        <v>0.1</v>
+      </c>
+      <c r="I7">
+        <v>18</v>
+      </c>
+      <c r="J7">
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <v>28</v>
+      </c>
+      <c r="L7">
+        <v>50</v>
+      </c>
+      <c r="M7">
+        <v>2500</v>
+      </c>
+      <c r="N7">
+        <v>20</v>
+      </c>
+      <c r="O7">
+        <v>1000</v>
+      </c>
+      <c r="P7">
+        <v>300</v>
+      </c>
+      <c r="Q7">
+        <v>50</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>70</v>
+      </c>
+      <c r="T7">
+        <v>130</v>
+      </c>
+      <c r="U7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="V7">
+        <v>10</v>
+      </c>
+      <c r="W7" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="X7">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="AD7">
+        <v>87</v>
+      </c>
+      <c r="AE7">
+        <v>425</v>
+      </c>
+      <c r="AF7">
+        <v>996615.44461174996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="U10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="U11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="U12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="U13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="1"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="U14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="U15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="1"/>
+    </row>
+    <row r="17" spans="18:29" x14ac:dyDescent="0.25">
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="1"/>
+    </row>
+    <row r="18" spans="18:29" x14ac:dyDescent="0.25">
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="1"/>
+    </row>
+    <row r="19" spans="18:29" x14ac:dyDescent="0.25">
+      <c r="R19" s="1"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1"/>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="1"/>
+      <c r="AC19" s="1"/>
+    </row>
+    <row r="20" spans="18:29" x14ac:dyDescent="0.25">
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="1"/>
+    </row>
+    <row r="21" spans="18:29" x14ac:dyDescent="0.25">
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="1"/>
+      <c r="AC21" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E4487D-883D-4E85-B2E5-7356A39B3F61}">
   <dimension ref="A1:AE21"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2978,13 +3751,13 @@
         <v>0.1</v>
       </c>
       <c r="F2">
-        <v>0.4</v>
+        <v>17</v>
       </c>
       <c r="G2">
         <v>5</v>
       </c>
       <c r="H2">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="I2">
         <v>18</v>
@@ -2999,40 +3772,40 @@
         <v>50</v>
       </c>
       <c r="M2">
-        <v>2500</v>
+        <v>1400</v>
       </c>
       <c r="N2">
         <v>120</v>
       </c>
       <c r="O2">
-        <v>1300</v>
+        <v>1000</v>
       </c>
       <c r="P2">
-        <v>10</v>
+        <v>150</v>
       </c>
       <c r="Q2">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="R2">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="S2">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="T2">
         <v>130</v>
       </c>
-      <c r="U2">
-        <v>0.1</v>
-      </c>
-      <c r="V2">
-        <v>3</v>
+      <c r="U2" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="V2" s="1">
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="W2">
+        <v>8</v>
+      </c>
+      <c r="X2">
         <v>1</v>
-      </c>
-      <c r="X2">
-        <v>650</v>
       </c>
       <c r="Y2" s="1">
         <v>1E-8</v>
@@ -3067,19 +3840,19 @@
         <v>18</v>
       </c>
       <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
         <v>8</v>
       </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>0.01</v>
-      </c>
       <c r="G3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I3">
         <v>18</v>
@@ -3094,40 +3867,40 @@
         <v>50</v>
       </c>
       <c r="M3">
-        <v>2500</v>
+        <v>1400</v>
       </c>
       <c r="N3">
         <v>50</v>
       </c>
       <c r="O3">
-        <v>1300</v>
+        <v>1000</v>
       </c>
       <c r="P3">
+        <v>150</v>
+      </c>
+      <c r="Q3">
+        <v>50</v>
+      </c>
+      <c r="R3">
         <v>10</v>
       </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
-      <c r="R3">
-        <v>1</v>
-      </c>
       <c r="S3">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="T3">
         <v>130</v>
       </c>
-      <c r="U3">
-        <v>0.1</v>
-      </c>
-      <c r="V3">
-        <v>3</v>
+      <c r="U3" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="V3" s="1">
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="W3">
+        <v>8</v>
+      </c>
+      <c r="X3">
         <v>1</v>
-      </c>
-      <c r="X3">
-        <v>650</v>
       </c>
       <c r="Y3" s="1">
         <v>1E-8</v>
@@ -3162,19 +3935,19 @@
         <v>18</v>
       </c>
       <c r="D4">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F4">
-        <v>0.01</v>
+        <v>5</v>
       </c>
       <c r="G4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="I4">
         <v>18</v>
@@ -3189,40 +3962,40 @@
         <v>50</v>
       </c>
       <c r="M4">
-        <v>2500</v>
+        <v>1400</v>
       </c>
       <c r="N4">
         <v>35</v>
       </c>
       <c r="O4">
-        <v>1300</v>
+        <v>1000</v>
       </c>
       <c r="P4">
-        <v>10</v>
+        <v>150</v>
       </c>
       <c r="Q4">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="R4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="S4">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="T4">
         <v>130</v>
       </c>
-      <c r="U4">
-        <v>0.1</v>
-      </c>
-      <c r="V4">
-        <v>3</v>
+      <c r="U4" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="V4" s="1">
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="W4">
+        <v>8</v>
+      </c>
+      <c r="X4">
         <v>1</v>
-      </c>
-      <c r="X4">
-        <v>650</v>
       </c>
       <c r="Y4" s="1">
         <v>1E-8</v>
@@ -3257,13 +4030,13 @@
         <v>18</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>7</v>
       </c>
       <c r="F5">
-        <v>0.01</v>
+        <v>4</v>
       </c>
       <c r="G5">
         <v>0.5</v>
@@ -3284,40 +4057,40 @@
         <v>50</v>
       </c>
       <c r="M5">
-        <v>2500</v>
+        <v>1400</v>
       </c>
       <c r="N5">
         <v>25</v>
       </c>
       <c r="O5">
-        <v>1300</v>
+        <v>1000</v>
       </c>
       <c r="P5">
-        <v>10</v>
+        <v>150</v>
       </c>
       <c r="Q5">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="R5">
         <v>1</v>
       </c>
       <c r="S5">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="T5">
         <v>130</v>
       </c>
-      <c r="U5">
-        <v>0.1</v>
-      </c>
-      <c r="V5">
-        <v>3</v>
+      <c r="U5" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="V5" s="1">
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="W5">
+        <v>8</v>
+      </c>
+      <c r="X5">
         <v>1</v>
-      </c>
-      <c r="X5">
-        <v>650</v>
       </c>
       <c r="Y5" s="1">
         <v>1E-8</v>
@@ -3352,13 +4125,13 @@
         <v>18</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6">
         <v>3</v>
       </c>
       <c r="F6">
-        <v>0.3</v>
+        <v>4</v>
       </c>
       <c r="G6">
         <v>0.5</v>
@@ -3379,40 +4152,40 @@
         <v>50</v>
       </c>
       <c r="M6">
-        <v>2500</v>
+        <v>1400</v>
       </c>
       <c r="N6">
         <v>20</v>
       </c>
       <c r="O6">
-        <v>1300</v>
+        <v>1000</v>
       </c>
       <c r="P6">
-        <v>10</v>
+        <v>150</v>
       </c>
       <c r="Q6">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="R6">
         <v>1</v>
       </c>
       <c r="S6">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="T6">
         <v>130</v>
       </c>
-      <c r="U6">
-        <v>0.1</v>
-      </c>
-      <c r="V6">
-        <v>3</v>
+      <c r="U6" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="V6" s="1">
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="W6">
+        <v>8</v>
+      </c>
+      <c r="X6">
         <v>1</v>
-      </c>
-      <c r="X6">
-        <v>650</v>
       </c>
       <c r="Y6" s="1">
         <v>1E-8</v>
@@ -3447,13 +4220,13 @@
         <v>18</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <v>4</v>
       </c>
       <c r="F7">
-        <v>0.3</v>
+        <v>4</v>
       </c>
       <c r="G7">
         <v>0.5</v>
@@ -3474,40 +4247,40 @@
         <v>50</v>
       </c>
       <c r="M7">
-        <v>2500</v>
+        <v>1400</v>
       </c>
       <c r="N7">
         <v>20</v>
       </c>
       <c r="O7">
-        <v>1300</v>
+        <v>1000</v>
       </c>
       <c r="P7">
-        <v>10</v>
+        <v>150</v>
       </c>
       <c r="Q7">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="R7">
         <v>1</v>
       </c>
       <c r="S7">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="T7">
         <v>130</v>
       </c>
-      <c r="U7">
-        <v>0.1</v>
-      </c>
-      <c r="V7">
-        <v>3</v>
+      <c r="U7" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="V7" s="1">
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="W7">
+        <v>8</v>
+      </c>
+      <c r="X7">
         <v>1</v>
-      </c>
-      <c r="X7">
-        <v>650</v>
       </c>
       <c r="Y7" s="1">
         <v>1E-8</v>
@@ -3532,7 +4305,8 @@
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="W10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
@@ -3540,7 +4314,8 @@
       <c r="AC10" s="1"/>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="W11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
@@ -3548,7 +4323,8 @@
       <c r="AC11" s="1"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="W12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
@@ -3556,7 +4332,8 @@
       <c r="AC12" s="1"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="W13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
@@ -3564,7 +4341,8 @@
       <c r="AC13" s="1"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="W14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
@@ -3572,736 +4350,13 @@
       <c r="AC14" s="1"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="W15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
       <c r="AC15" s="1"/>
-    </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
-      <c r="AA16" s="1"/>
-      <c r="AB16" s="1"/>
-      <c r="AC16" s="1"/>
-    </row>
-    <row r="17" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="1"/>
-      <c r="AA17" s="1"/>
-      <c r="AB17" s="1"/>
-      <c r="AC17" s="1"/>
-    </row>
-    <row r="18" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="Y18" s="1"/>
-      <c r="Z18" s="1"/>
-      <c r="AA18" s="1"/>
-      <c r="AB18" s="1"/>
-      <c r="AC18" s="1"/>
-    </row>
-    <row r="19" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="R19" s="1"/>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="1"/>
-      <c r="AA19" s="1"/>
-      <c r="AB19" s="1"/>
-      <c r="AC19" s="1"/>
-    </row>
-    <row r="20" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="Y20" s="1"/>
-      <c r="Z20" s="1"/>
-      <c r="AA20" s="1"/>
-      <c r="AB20" s="1"/>
-      <c r="AC20" s="1"/>
-    </row>
-    <row r="21" spans="18:29" x14ac:dyDescent="0.25">
-      <c r="Y21" s="1"/>
-      <c r="Z21" s="1"/>
-      <c r="AA21" s="1"/>
-      <c r="AB21" s="1"/>
-      <c r="AC21" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E4487D-883D-4E85-B2E5-7356A39B3F61}">
-  <dimension ref="A1:AE21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="16" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" t="s">
-        <v>47</v>
-      </c>
-      <c r="V1" t="s">
-        <v>43</v>
-      </c>
-      <c r="W1" t="s">
-        <v>49</v>
-      </c>
-      <c r="X1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2">
-        <v>1E-3</v>
-      </c>
-      <c r="C2">
-        <v>18</v>
-      </c>
-      <c r="D2">
-        <v>18</v>
-      </c>
-      <c r="E2">
-        <v>0.1</v>
-      </c>
-      <c r="F2">
-        <v>0.4</v>
-      </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
-      <c r="H2">
-        <v>50</v>
-      </c>
-      <c r="I2">
-        <v>18</v>
-      </c>
-      <c r="J2">
-        <v>50</v>
-      </c>
-      <c r="K2">
-        <v>28</v>
-      </c>
-      <c r="L2">
-        <v>50</v>
-      </c>
-      <c r="M2">
-        <v>2500</v>
-      </c>
-      <c r="N2">
-        <v>120</v>
-      </c>
-      <c r="O2">
-        <v>1300</v>
-      </c>
-      <c r="P2">
-        <v>100</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="R2">
-        <v>1</v>
-      </c>
-      <c r="S2">
-        <v>70</v>
-      </c>
-      <c r="T2">
-        <v>130</v>
-      </c>
-      <c r="U2">
-        <v>10</v>
-      </c>
-      <c r="V2">
-        <v>0.1</v>
-      </c>
-      <c r="W2">
-        <v>1</v>
-      </c>
-      <c r="X2">
-        <v>800</v>
-      </c>
-      <c r="Y2" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="Z2" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AA2" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AB2" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AC2" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AD2">
-        <v>87</v>
-      </c>
-      <c r="AE2">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3">
-        <v>0.01</v>
-      </c>
-      <c r="C3">
-        <v>18</v>
-      </c>
-      <c r="D3">
-        <v>6</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>0.01</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>10</v>
-      </c>
-      <c r="I3">
-        <v>18</v>
-      </c>
-      <c r="J3">
-        <v>25</v>
-      </c>
-      <c r="K3">
-        <v>28</v>
-      </c>
-      <c r="L3">
-        <v>50</v>
-      </c>
-      <c r="M3">
-        <v>2500</v>
-      </c>
-      <c r="N3">
-        <v>50</v>
-      </c>
-      <c r="O3">
-        <v>1300</v>
-      </c>
-      <c r="P3">
-        <v>100</v>
-      </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
-      <c r="R3">
-        <v>1</v>
-      </c>
-      <c r="S3">
-        <v>70</v>
-      </c>
-      <c r="T3">
-        <v>130</v>
-      </c>
-      <c r="U3">
-        <v>10</v>
-      </c>
-      <c r="V3">
-        <v>0.1</v>
-      </c>
-      <c r="W3">
-        <v>1</v>
-      </c>
-      <c r="X3">
-        <v>800</v>
-      </c>
-      <c r="Y3" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="Z3" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AA3" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AB3" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AC3" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AD3">
-        <v>87</v>
-      </c>
-      <c r="AE3">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>18</v>
-      </c>
-      <c r="D4">
-        <v>5</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="F4">
-        <v>0.01</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>18</v>
-      </c>
-      <c r="J4">
-        <v>10</v>
-      </c>
-      <c r="K4">
-        <v>28</v>
-      </c>
-      <c r="L4">
-        <v>50</v>
-      </c>
-      <c r="M4">
-        <v>2500</v>
-      </c>
-      <c r="N4">
-        <v>35</v>
-      </c>
-      <c r="O4">
-        <v>1300</v>
-      </c>
-      <c r="P4">
-        <v>100</v>
-      </c>
-      <c r="Q4">
-        <v>1</v>
-      </c>
-      <c r="R4">
-        <v>1</v>
-      </c>
-      <c r="S4">
-        <v>70</v>
-      </c>
-      <c r="T4">
-        <v>130</v>
-      </c>
-      <c r="U4">
-        <v>10</v>
-      </c>
-      <c r="V4">
-        <v>0.1</v>
-      </c>
-      <c r="W4">
-        <v>1</v>
-      </c>
-      <c r="X4">
-        <v>800</v>
-      </c>
-      <c r="Y4" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="Z4" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AA4" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AB4" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AC4" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AD4">
-        <v>87</v>
-      </c>
-      <c r="AE4">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>18</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>7</v>
-      </c>
-      <c r="F5">
-        <v>0.01</v>
-      </c>
-      <c r="G5">
-        <v>0.5</v>
-      </c>
-      <c r="H5">
-        <v>0.1</v>
-      </c>
-      <c r="I5">
-        <v>18</v>
-      </c>
-      <c r="J5">
-        <v>5</v>
-      </c>
-      <c r="K5">
-        <v>28</v>
-      </c>
-      <c r="L5">
-        <v>50</v>
-      </c>
-      <c r="M5">
-        <v>2500</v>
-      </c>
-      <c r="N5">
-        <v>25</v>
-      </c>
-      <c r="O5">
-        <v>1300</v>
-      </c>
-      <c r="P5">
-        <v>100</v>
-      </c>
-      <c r="Q5">
-        <v>1</v>
-      </c>
-      <c r="R5">
-        <v>1</v>
-      </c>
-      <c r="S5">
-        <v>70</v>
-      </c>
-      <c r="T5">
-        <v>130</v>
-      </c>
-      <c r="U5">
-        <v>10</v>
-      </c>
-      <c r="V5">
-        <v>0.1</v>
-      </c>
-      <c r="W5">
-        <v>1</v>
-      </c>
-      <c r="X5">
-        <v>800</v>
-      </c>
-      <c r="Y5" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="Z5" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AA5" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AB5" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AC5" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AD5">
-        <v>87</v>
-      </c>
-      <c r="AE5">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6">
-        <v>0.01</v>
-      </c>
-      <c r="C6">
-        <v>18</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>0.3</v>
-      </c>
-      <c r="G6">
-        <v>0.5</v>
-      </c>
-      <c r="H6">
-        <v>0.1</v>
-      </c>
-      <c r="I6">
-        <v>18</v>
-      </c>
-      <c r="J6">
-        <v>6</v>
-      </c>
-      <c r="K6">
-        <v>28</v>
-      </c>
-      <c r="L6">
-        <v>50</v>
-      </c>
-      <c r="M6">
-        <v>2500</v>
-      </c>
-      <c r="N6">
-        <v>20</v>
-      </c>
-      <c r="O6">
-        <v>1300</v>
-      </c>
-      <c r="P6">
-        <v>100</v>
-      </c>
-      <c r="Q6">
-        <v>1</v>
-      </c>
-      <c r="R6">
-        <v>1</v>
-      </c>
-      <c r="S6">
-        <v>70</v>
-      </c>
-      <c r="T6">
-        <v>130</v>
-      </c>
-      <c r="U6">
-        <v>10</v>
-      </c>
-      <c r="V6">
-        <v>0.1</v>
-      </c>
-      <c r="W6">
-        <v>1</v>
-      </c>
-      <c r="X6">
-        <v>800</v>
-      </c>
-      <c r="Y6" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="Z6" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AA6" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AB6" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AC6" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AD6">
-        <v>87</v>
-      </c>
-      <c r="AE6">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>18</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7">
-        <v>0.3</v>
-      </c>
-      <c r="G7">
-        <v>0.5</v>
-      </c>
-      <c r="H7">
-        <v>0.1</v>
-      </c>
-      <c r="I7">
-        <v>18</v>
-      </c>
-      <c r="J7">
-        <v>5</v>
-      </c>
-      <c r="K7">
-        <v>28</v>
-      </c>
-      <c r="L7">
-        <v>50</v>
-      </c>
-      <c r="M7">
-        <v>2500</v>
-      </c>
-      <c r="N7">
-        <v>20</v>
-      </c>
-      <c r="O7">
-        <v>1300</v>
-      </c>
-      <c r="P7">
-        <v>100</v>
-      </c>
-      <c r="Q7">
-        <v>1</v>
-      </c>
-      <c r="R7">
-        <v>1</v>
-      </c>
-      <c r="S7">
-        <v>70</v>
-      </c>
-      <c r="T7">
-        <v>130</v>
-      </c>
-      <c r="U7">
-        <v>10</v>
-      </c>
-      <c r="V7">
-        <v>0.1</v>
-      </c>
-      <c r="W7">
-        <v>1</v>
-      </c>
-      <c r="X7">
-        <v>800</v>
-      </c>
-      <c r="Y7" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="Z7" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AA7" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AB7" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AC7" s="1">
-        <v>1E-8</v>
-      </c>
-      <c r="AD7">
-        <v>87</v>
-      </c>
-      <c r="AE7">
-        <v>425</v>
-      </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="Y16" s="1"/>
@@ -4356,7 +4411,7 @@
   <dimension ref="A1:AE16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4470,13 +4525,13 @@
         <v>0.02</v>
       </c>
       <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="G2">
         <v>5</v>
       </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
       <c r="H2">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="I2">
         <v>18</v>
@@ -4491,7 +4546,7 @@
         <v>50</v>
       </c>
       <c r="M2">
-        <v>2800</v>
+        <v>2000</v>
       </c>
       <c r="N2">
         <v>110</v>
@@ -4509,7 +4564,7 @@
         <v>25</v>
       </c>
       <c r="S2">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="T2">
         <v>140</v>
@@ -4568,10 +4623,10 @@
         <v>5</v>
       </c>
       <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
         <v>2</v>
-      </c>
-      <c r="H3">
-        <v>15</v>
       </c>
       <c r="I3">
         <v>18</v>
@@ -4586,7 +4641,7 @@
         <v>50</v>
       </c>
       <c r="M3">
-        <v>2800</v>
+        <v>2000</v>
       </c>
       <c r="N3">
         <v>50</v>
@@ -4604,7 +4659,7 @@
         <v>10</v>
       </c>
       <c r="S3">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="T3">
         <v>140</v>
@@ -4660,13 +4715,13 @@
         <v>2</v>
       </c>
       <c r="F4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I4">
         <v>18</v>
@@ -4681,7 +4736,7 @@
         <v>50</v>
       </c>
       <c r="M4">
-        <v>2800</v>
+        <v>2000</v>
       </c>
       <c r="N4">
         <v>35</v>
@@ -4699,7 +4754,7 @@
         <v>5</v>
       </c>
       <c r="S4">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="T4">
         <v>140</v>
@@ -4755,10 +4810,10 @@
         <v>6</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5">
         <v>0.5</v>
@@ -4776,7 +4831,7 @@
         <v>50</v>
       </c>
       <c r="M5">
-        <v>2800</v>
+        <v>2000</v>
       </c>
       <c r="N5">
         <v>25</v>
@@ -4794,7 +4849,7 @@
         <v>1</v>
       </c>
       <c r="S5">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="T5">
         <v>140</v>
@@ -4850,7 +4905,7 @@
         <v>2</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <v>0.5</v>
@@ -4871,7 +4926,7 @@
         <v>50</v>
       </c>
       <c r="M6">
-        <v>2800</v>
+        <v>2000</v>
       </c>
       <c r="N6">
         <v>20</v>
@@ -4889,7 +4944,7 @@
         <v>1</v>
       </c>
       <c r="S6">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="T6">
         <v>140</v>
@@ -4945,10 +5000,10 @@
         <v>3</v>
       </c>
       <c r="F7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <v>0.1</v>
@@ -4966,7 +5021,7 @@
         <v>50</v>
       </c>
       <c r="M7">
-        <v>2800</v>
+        <v>2000</v>
       </c>
       <c r="N7">
         <v>20</v>
@@ -4984,7 +5039,7 @@
         <v>1</v>
       </c>
       <c r="S7">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="T7">
         <v>140</v>
@@ -5022,6 +5077,10 @@
       <c r="AE7">
         <v>425</v>
       </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="Z10" s="1"/>
+      <c r="AB10" s="1"/>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="U11" s="1"/>
@@ -5831,10 +5890,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CB7F0C9-B54B-4F93-93CE-9E10B0EA4FF3}">
-  <dimension ref="A1:AF35"/>
+  <dimension ref="A1:AF37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6438,88 +6497,88 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D7">
         <v>0.2</v>
       </c>
       <c r="E7">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="F7">
-        <v>400</v>
+        <v>1000</v>
       </c>
       <c r="G7">
         <v>0.4</v>
       </c>
       <c r="H7">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
       <c r="I7">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J7">
         <v>84</v>
       </c>
       <c r="K7">
-        <v>28</v>
+        <v>500</v>
       </c>
       <c r="L7">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="M7">
-        <v>8000</v>
+        <v>10000</v>
       </c>
       <c r="N7">
         <v>100</v>
       </c>
       <c r="O7">
-        <v>2800</v>
+        <v>3500</v>
       </c>
       <c r="P7">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="Q7">
-        <v>10</v>
+        <v>150</v>
       </c>
       <c r="R7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="S7">
         <v>200</v>
       </c>
       <c r="T7">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="U7">
         <v>0.01</v>
       </c>
-      <c r="V7">
-        <v>0.01</v>
-      </c>
-      <c r="W7">
-        <v>0.01</v>
-      </c>
-      <c r="X7">
-        <v>0.01</v>
-      </c>
-      <c r="Y7">
-        <v>0.01</v>
-      </c>
-      <c r="Z7">
-        <v>0.01</v>
-      </c>
-      <c r="AA7">
-        <v>0.01</v>
-      </c>
-      <c r="AB7">
-        <v>0.01</v>
-      </c>
-      <c r="AC7">
-        <v>0.01</v>
+      <c r="V7" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="W7" s="1">
+        <v>2400</v>
+      </c>
+      <c r="X7" s="1">
+        <v>300</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="AD7">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AE7">
         <v>425</v>
@@ -6638,6 +6697,20 @@
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
     </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="F10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+    </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
@@ -6667,6 +6740,12 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6678,7 +6757,7 @@
   <dimension ref="A1:AQ58"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6951,7 +7030,7 @@
       <c r="AP2">
         <v>425</v>
       </c>
-      <c r="AQ2" s="2">
+      <c r="AQ2">
         <v>997000</v>
       </c>
     </row>
@@ -7082,7 +7161,7 @@
       <c r="AP3">
         <v>425</v>
       </c>
-      <c r="AQ3" s="2">
+      <c r="AQ3">
         <v>997000</v>
       </c>
     </row>
@@ -7213,7 +7292,7 @@
       <c r="AP4">
         <v>425</v>
       </c>
-      <c r="AQ4" s="2">
+      <c r="AQ4">
         <v>997000</v>
       </c>
     </row>
@@ -7344,7 +7423,7 @@
       <c r="AP5">
         <v>424</v>
       </c>
-      <c r="AQ5" s="2">
+      <c r="AQ5">
         <v>997000</v>
       </c>
     </row>
@@ -7475,7 +7554,7 @@
       <c r="AP6">
         <v>425</v>
       </c>
-      <c r="AQ6" s="2">
+      <c r="AQ6">
         <v>997000</v>
       </c>
     </row>
@@ -7510,7 +7589,7 @@
       <c r="J7">
         <v>170</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7">
         <v>900</v>
       </c>
       <c r="L7">
@@ -7600,13 +7679,13 @@
       <c r="AN7" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="AO7" s="2">
+      <c r="AO7">
         <v>87</v>
       </c>
-      <c r="AP7" s="2">
+      <c r="AP7">
         <v>425</v>
       </c>
-      <c r="AQ7" s="2">
+      <c r="AQ7">
         <v>997000</v>
       </c>
     </row>
@@ -7737,7 +7816,7 @@
       <c r="AP8">
         <v>425</v>
       </c>
-      <c r="AQ8" s="2">
+      <c r="AQ8">
         <v>997000</v>
       </c>
     </row>
@@ -7868,12 +7947,11 @@
       <c r="AP9">
         <v>425</v>
       </c>
-      <c r="AQ9" s="2">
+      <c r="AQ9">
         <v>997000</v>
       </c>
     </row>
     <row r="10" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="K10" s="2"/>
       <c r="AA10" s="1"/>
       <c r="AF10" s="1"/>
       <c r="AH10" s="1"/>
@@ -7881,9 +7959,6 @@
       <c r="AL10" s="1"/>
       <c r="AM10" s="1"/>
       <c r="AN10" s="1"/>
-      <c r="AO10" s="2"/>
-      <c r="AP10" s="2"/>
-      <c r="AQ10" s="2"/>
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="J11" s="1"/>

</xml_diff>